<commit_message>
added notes for 10_ES5_Dtl-Ch01L02: JS Overview
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8141F3F3-80E2-4D65-9116-FD350517B635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F5BAEB-D5B1-4348-8C4A-05E85890F70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="17" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="5115" yWindow="1710" windowWidth="20565" windowHeight="13140" firstSheet="4" activeTab="9" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -28,9 +28,10 @@
     <sheet name="13Git" sheetId="12" r:id="rId13"/>
     <sheet name="14ThirdLib" sheetId="13" r:id="rId14"/>
     <sheet name="15Build" sheetId="14" r:id="rId15"/>
-    <sheet name="16Vue_intro" sheetId="15" r:id="rId16"/>
-    <sheet name="17Vue_comp" sheetId="16" r:id="rId17"/>
-    <sheet name="18Miniapp" sheetId="17" r:id="rId18"/>
+    <sheet name="16Vue_scratch" sheetId="19" r:id="rId16"/>
+    <sheet name="17Vue_intro" sheetId="15" r:id="rId17"/>
+    <sheet name="18Vue_comp" sheetId="16" r:id="rId18"/>
+    <sheet name="19Miniapp" sheetId="17" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="600">
   <si>
     <t>1. 环境准备</t>
   </si>
@@ -770,9 +771,6 @@
   </si>
   <si>
     <t>24. json，异步加载，时间线（2节） (2小节)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 已学2%</t>
   </si>
   <si>
     <t>25. 正则表达式（2节） (2小节)</t>
@@ -1838,12 +1836,69 @@
     <t>20-2.安装Node和Mongo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>01.Vue基础知识1 (6小节)</t>
+  </si>
+  <si>
+    <t>02.Vue基础知识2 (5小节)</t>
+  </si>
+  <si>
+    <t>03.Vue常用组件使用 (5小节)</t>
+  </si>
+  <si>
+    <t>1.从vue到前端</t>
+  </si>
+  <si>
+    <t>2.vue初体验</t>
+  </si>
+  <si>
+    <t>3.vue必会概念</t>
+  </si>
+  <si>
+    <t>4.学习须知</t>
+  </si>
+  <si>
+    <t>5.模板语法和计算属性</t>
+  </si>
+  <si>
+    <t>6.组件必会概念</t>
+  </si>
+  <si>
+    <t>1. 使用脚手架搭建工程</t>
+  </si>
+  <si>
+    <t>2. 开发通用组件</t>
+  </si>
+  <si>
+    <t>3. 自定义事件</t>
+  </si>
+  <si>
+    <t>4. 开发频道菜单</t>
+  </si>
+  <si>
+    <t>5.获取频道数据</t>
+  </si>
+  <si>
+    <t>1.完成频道列表组件</t>
+  </si>
+  <si>
+    <t>2.继续完善频道列表</t>
+  </si>
+  <si>
+    <t>3.搜索框组件</t>
+  </si>
+  <si>
+    <t>4.侧边栏和页面组件</t>
+  </si>
+  <si>
+    <t>5.尾声：学无止境</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1929,6 +1984,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
@@ -2051,7 +2114,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2169,8 +2232,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="20"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2506,6 +2590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1401E8D-40FC-4FEC-80E2-AB1337891220}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -2980,11 +3065,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427F4DB1-3E3A-4CF5-BB6A-F387BAED2E70}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3005,12 +3089,12 @@
         <v>53</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3026,7 +3110,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B4">
         <v>81</v>
@@ -3037,7 +3121,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -3048,12 +3132,12 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -3064,7 +3148,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B8">
         <v>65</v>
@@ -3075,7 +3159,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B9">
         <v>52</v>
@@ -3086,7 +3170,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B10">
         <v>85</v>
@@ -3097,7 +3181,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B11">
         <v>69</v>
@@ -3108,12 +3192,12 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="34" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B13">
         <v>37</v>
@@ -3124,7 +3208,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B14">
         <v>58</v>
@@ -3135,7 +3219,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -3146,7 +3230,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B16">
         <v>45</v>
@@ -3157,7 +3241,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B17">
         <v>45</v>
@@ -3168,7 +3252,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B18">
         <v>54</v>
@@ -3179,7 +3263,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -3190,7 +3274,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B20">
         <v>7</v>
@@ -3201,7 +3285,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B21">
         <v>31</v>
@@ -3212,7 +3296,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B22">
         <v>73</v>
@@ -3223,7 +3307,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B23">
         <v>52</v>
@@ -3234,7 +3318,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B24">
         <v>18</v>
@@ -3245,12 +3329,12 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="34" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B26">
         <v>19</v>
@@ -3261,7 +3345,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B27">
         <v>42</v>
@@ -3272,7 +3356,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B28">
         <v>36</v>
@@ -3283,7 +3367,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B29">
         <v>7</v>
@@ -3294,7 +3378,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B30">
         <v>50</v>
@@ -3305,7 +3389,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B31">
         <v>43</v>
@@ -3316,7 +3400,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B32">
         <v>40</v>
@@ -3327,7 +3411,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B33">
         <v>96</v>
@@ -3338,7 +3422,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B34">
         <v>23</v>
@@ -3349,7 +3433,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B35">
         <v>69</v>
@@ -3360,12 +3444,12 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="34" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B37">
         <v>74</v>
@@ -3376,7 +3460,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B38">
         <v>60</v>
@@ -3387,7 +3471,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B39">
         <v>41</v>
@@ -3398,7 +3482,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B40">
         <v>61</v>
@@ -3409,7 +3493,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B41">
         <v>38</v>
@@ -3420,7 +3504,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B42">
         <v>57</v>
@@ -3431,7 +3515,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B43">
         <v>37</v>
@@ -3442,7 +3526,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B44">
         <v>63</v>
@@ -3453,12 +3537,12 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="34" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B46">
         <v>68</v>
@@ -3469,7 +3553,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B47">
         <v>60</v>
@@ -3480,7 +3564,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3491,7 +3575,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B49">
         <v>77</v>
@@ -3502,7 +3586,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B50">
         <v>39</v>
@@ -3513,7 +3597,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B51">
         <v>12</v>
@@ -3524,7 +3608,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B52">
         <v>59</v>
@@ -3535,7 +3619,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B53">
         <v>37</v>
@@ -3546,7 +3630,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B54">
         <v>60</v>
@@ -3557,7 +3641,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B55">
         <v>66</v>
@@ -3568,7 +3652,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B56">
         <v>60</v>
@@ -3579,7 +3663,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B57">
         <v>59</v>
@@ -3590,12 +3674,12 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="34" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B59">
         <v>39</v>
@@ -3606,7 +3690,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B60">
         <v>67</v>
@@ -3617,7 +3701,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B61">
         <v>16</v>
@@ -3628,7 +3712,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B62">
         <v>54</v>
@@ -3639,7 +3723,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B63">
         <v>49</v>
@@ -3650,7 +3734,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B64">
         <v>55</v>
@@ -3661,7 +3745,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B65">
         <v>45</v>
@@ -3672,7 +3756,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B66">
         <v>20</v>
@@ -3683,7 +3767,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B67">
         <v>58</v>
@@ -3694,7 +3778,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B68">
         <v>33</v>
@@ -3705,12 +3789,12 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="34" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B70">
         <v>22</v>
@@ -3721,7 +3805,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B71">
         <v>36</v>
@@ -3732,7 +3816,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B72">
         <v>53</v>
@@ -3743,7 +3827,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B73">
         <v>35</v>
@@ -3754,7 +3838,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B74">
         <v>61</v>
@@ -3765,7 +3849,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B75">
         <v>79</v>
@@ -3776,7 +3860,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B76">
         <v>20</v>
@@ -3787,7 +3871,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B77">
         <v>21</v>
@@ -3798,7 +3882,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B78">
         <v>35</v>
@@ -3809,7 +3893,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B79">
         <v>51</v>
@@ -3820,7 +3904,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B80">
         <v>45</v>
@@ -3831,7 +3915,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B81">
         <v>14</v>
@@ -3842,7 +3926,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B82">
         <v>60</v>
@@ -3853,7 +3937,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B83">
         <v>49</v>
@@ -3864,12 +3948,12 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="34" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B85">
         <v>36</v>
@@ -3880,7 +3964,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B86">
         <v>21</v>
@@ -3891,7 +3975,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B87">
         <v>105</v>
@@ -3902,7 +3986,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B88">
         <v>41</v>
@@ -3913,7 +3997,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B89">
         <v>62</v>
@@ -3924,12 +4008,12 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="34" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B91">
         <v>69</v>
@@ -3940,7 +4024,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B92">
         <v>69</v>
@@ -3951,7 +4035,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B93">
         <v>62</v>
@@ -3962,7 +4046,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B94">
         <v>76</v>
@@ -3973,7 +4057,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B95">
         <v>64</v>
@@ -3984,7 +4068,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B96">
         <v>42</v>
@@ -3995,7 +4079,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B97">
         <v>44</v>
@@ -4006,7 +4090,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B98">
         <v>39</v>
@@ -4017,7 +4101,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B99">
         <v>31</v>
@@ -4028,7 +4112,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B100">
         <v>21</v>
@@ -4039,12 +4123,12 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="34" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B102">
         <v>67</v>
@@ -4055,7 +4139,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B103">
         <v>51</v>
@@ -4066,7 +4150,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B104">
         <v>29</v>
@@ -4077,7 +4161,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B105">
         <v>30</v>
@@ -4088,7 +4172,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B106">
         <v>44</v>
@@ -4099,7 +4183,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B107">
         <v>60</v>
@@ -4110,7 +4194,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B108">
         <v>55</v>
@@ -4121,7 +4205,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B109">
         <v>63</v>
@@ -4132,7 +4216,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B110">
         <v>60</v>
@@ -4143,7 +4227,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B111">
         <v>87</v>
@@ -4154,12 +4238,12 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="34" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B113">
         <v>11</v>
@@ -4182,6 +4266,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39AD0F8-0D2C-49A2-997C-DACB9B26CA76}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4265,6 +4350,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC9628E-F669-40A2-855C-BA931809CE20}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A2:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4278,67 +4364,67 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -4349,6 +4435,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176B4581-7942-4FCC-A12F-3EC4A3FA8D07}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4362,37 +4449,37 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -4403,6 +4490,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B832BBF-CF90-430B-B2E0-B6425812829B}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4416,37 +4504,37 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4457,6 +4545,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00865C93-FCC5-4D30-A25D-4C01DD061FF8}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A2:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4470,42 +4559,42 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -4515,11 +4604,246 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D093D58B-B7D0-4ABE-B71F-06475D33804E}">
+  <sheetPr codeName="Sheet16"/>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.375" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>584</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>586</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>587</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>588</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>589</v>
+      </c>
+      <c r="B8">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>590</v>
+      </c>
+      <c r="B10">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>591</v>
+      </c>
+      <c r="B11">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>592</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>593</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>594</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>595</v>
+      </c>
+      <c r="B16">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>596</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>597</v>
+      </c>
+      <c r="B18">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>598</v>
+      </c>
+      <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>599</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：8:07:22</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AF8CD0-73B6-411F-82CC-0DBAA39229A0}">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4541,12 +4865,12 @@
         <v>53</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B2">
         <v>23</v>
@@ -4557,7 +4881,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B3">
         <v>22</v>
@@ -4568,7 +4892,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B4">
         <v>48</v>
@@ -4579,7 +4903,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -4590,7 +4914,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -4601,7 +4925,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B7">
         <v>47</v>
@@ -4612,7 +4936,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B8">
         <v>38</v>
@@ -4623,7 +4947,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B9">
         <v>84</v>
@@ -4634,7 +4958,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B10">
         <v>17</v>
@@ -4645,7 +4969,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B11">
         <v>112</v>
@@ -4656,7 +4980,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B12">
         <v>33</v>
@@ -4667,7 +4991,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B13">
         <v>54</v>
@@ -4678,7 +5002,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B14">
         <v>71</v>
@@ -4689,7 +5013,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B15">
         <v>57</v>
@@ -4700,7 +5024,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B16">
         <v>34</v>
@@ -4711,7 +5035,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B17">
         <v>44</v>
@@ -4722,7 +5046,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B18">
         <v>41</v>
@@ -4733,7 +5057,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B19">
         <v>34</v>
@@ -4744,7 +5068,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B20">
         <v>41</v>
@@ -4755,7 +5079,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -4766,7 +5090,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B22">
         <v>27</v>
@@ -4777,7 +5101,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B23">
         <v>26</v>
@@ -4788,7 +5112,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B24">
         <v>94</v>
@@ -4799,7 +5123,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -4810,7 +5134,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B26">
         <v>39</v>
@@ -4821,7 +5145,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B27">
         <v>43</v>
@@ -4832,7 +5156,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B28">
         <v>48</v>
@@ -4843,7 +5167,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -4854,7 +5178,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B30">
         <v>40</v>
@@ -4865,7 +5189,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B31">
         <v>37</v>
@@ -4876,7 +5200,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B32">
         <v>10</v>
@@ -4887,7 +5211,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B33">
         <v>39</v>
@@ -4898,7 +5222,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B34">
         <v>46</v>
@@ -4909,7 +5233,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B35">
         <v>98</v>
@@ -4920,7 +5244,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B36">
         <v>23</v>
@@ -4931,7 +5255,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B37">
         <v>14</v>
@@ -4942,7 +5266,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B38">
         <v>12</v>
@@ -4953,7 +5277,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B39">
         <v>17</v>
@@ -4964,7 +5288,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B40">
         <v>14</v>
@@ -4975,7 +5299,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B41">
         <v>55</v>
@@ -4986,7 +5310,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B42">
         <v>23</v>
@@ -4997,7 +5321,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B43">
         <v>6</v>
@@ -5008,7 +5332,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -5019,7 +5343,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B45">
         <v>32</v>
@@ -5040,8 +5364,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE55571-67F4-430B-911B-F444D39A2E21}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5067,12 +5392,12 @@
         <v>53</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B2">
         <v>19</v>
@@ -5083,7 +5408,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -5094,7 +5419,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -5105,7 +5430,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -5116,12 +5441,12 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B7">
         <v>15</v>
@@ -5132,7 +5457,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B8">
         <v>58</v>
@@ -5143,7 +5468,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="38" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B9">
         <v>17</v>
@@ -5154,7 +5479,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B10">
         <v>62</v>
@@ -5165,7 +5490,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B11">
         <v>46</v>
@@ -5176,7 +5501,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B12">
         <v>58</v>
@@ -5187,7 +5512,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B13">
         <v>40</v>
@@ -5198,7 +5523,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B14">
         <v>57</v>
@@ -5209,7 +5534,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B15">
         <v>78</v>
@@ -5220,7 +5545,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B16">
         <v>43</v>
@@ -5231,7 +5556,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B17">
         <v>79</v>
@@ -5242,7 +5567,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B18">
         <v>15</v>
@@ -5253,7 +5578,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B19">
         <v>75</v>
@@ -5264,7 +5589,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B20">
         <v>14</v>
@@ -5275,7 +5600,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B21">
         <v>35</v>
@@ -5286,12 +5611,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5302,7 +5627,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B24">
         <v>17</v>
@@ -5313,7 +5638,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -5324,7 +5649,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B26">
         <v>13</v>
@@ -5335,7 +5660,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B27">
         <v>23</v>
@@ -5346,7 +5671,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -5357,7 +5682,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B29">
         <v>18</v>
@@ -5368,7 +5693,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -5379,7 +5704,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -5390,7 +5715,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B32">
         <v>22</v>
@@ -5400,8 +5725,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="39" t="s">
-        <v>564</v>
+      <c r="A33" t="s">
+        <v>563</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -5412,12 +5737,12 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B35">
         <v>23</v>
@@ -5428,7 +5753,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B36">
         <v>26</v>
@@ -5449,11 +5774,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E16794E-744F-4D5E-88D3-DF76CD9771EA}">
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
@@ -5478,12 +5804,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -5494,7 +5820,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B4">
         <v>44</v>
@@ -5505,7 +5831,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B5">
         <v>27</v>
@@ -5516,7 +5842,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B6">
         <v>46</v>
@@ -5527,7 +5853,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B7">
         <v>61</v>
@@ -5538,7 +5864,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B8">
         <v>47</v>
@@ -5549,7 +5875,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B9">
         <v>55</v>
@@ -5560,7 +5886,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -5571,7 +5897,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B11">
         <v>24</v>
@@ -5582,7 +5908,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B12">
         <v>45</v>
@@ -5593,7 +5919,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B13">
         <v>59</v>
@@ -5604,7 +5930,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -5615,12 +5941,12 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B16">
         <v>59</v>
@@ -5631,7 +5957,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -5642,7 +5968,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -5653,7 +5979,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B19">
         <v>52</v>
@@ -5664,7 +5990,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -5675,7 +6001,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B21">
         <v>49</v>
@@ -5686,7 +6012,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B22">
         <v>55</v>
@@ -5697,7 +6023,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B23">
         <v>69</v>
@@ -5708,7 +6034,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B24">
         <v>64</v>
@@ -5719,7 +6045,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B25">
         <v>17</v>
@@ -5730,12 +6056,12 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -5746,7 +6072,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B28">
         <v>30</v>
@@ -5757,7 +6083,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B29">
         <v>41</v>
@@ -5768,7 +6094,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B30">
         <v>36</v>
@@ -5779,7 +6105,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B31">
         <v>65</v>
@@ -5790,12 +6116,12 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B33">
         <v>25</v>
@@ -5806,7 +6132,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B34">
         <v>41</v>
@@ -5817,7 +6143,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B35">
         <v>11</v>
@@ -5828,12 +6154,12 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B37">
         <v>47</v>
@@ -5844,7 +6170,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B38">
         <v>34</v>
@@ -5855,7 +6181,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -5866,7 +6192,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B40">
         <v>46</v>
@@ -5877,7 +6203,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B41">
         <v>25</v>
@@ -5888,7 +6214,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B42">
         <v>9</v>
@@ -5899,7 +6225,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B43">
         <v>49</v>
@@ -5910,7 +6236,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B44">
         <v>21</v>
@@ -5921,7 +6247,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B45">
         <v>9</v>
@@ -5932,7 +6258,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B46">
         <v>10</v>
@@ -5943,7 +6269,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B47">
         <v>25</v>
@@ -5954,7 +6280,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B48">
         <v>48</v>
@@ -5965,7 +6291,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B49">
         <v>23</v>
@@ -5976,7 +6302,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B50">
         <v>25</v>
@@ -5999,6 +6325,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08D3B80-1D2B-41F2-9997-2425A74C9955}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView topLeftCell="A53" workbookViewId="0">
@@ -6923,6 +7250,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A799BE-9F84-4BAB-8CB9-C9B281CC6A64}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7039,6 +7367,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A92B752-814C-4C87-B89E-FD54022B7B26}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7066,7 +7395,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B2">
         <v>31</v>
@@ -7077,7 +7406,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B3">
         <v>33</v>
@@ -7088,7 +7417,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B4">
         <v>21</v>
@@ -7099,7 +7428,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -7110,7 +7439,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B6">
         <v>17</v>
@@ -7121,7 +7450,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B7">
         <v>28</v>
@@ -7132,7 +7461,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -7143,7 +7472,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B9">
         <v>31</v>
@@ -7154,7 +7483,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B10">
         <v>19</v>
@@ -7165,7 +7494,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -7176,7 +7505,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B12">
         <v>25</v>
@@ -7187,7 +7516,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B13">
         <v>29</v>
@@ -7198,7 +7527,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -7209,7 +7538,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B15">
         <v>18</v>
@@ -7220,7 +7549,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B16">
         <v>8</v>
@@ -7243,10 +7572,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078994BB-162C-4327-BF62-6D3636325352}">
-  <dimension ref="A1:J88"/>
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H87" sqref="H83:H87"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7271,7 +7601,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="41" t="s">
         <v>214</v>
       </c>
       <c r="B2" s="18"/>
@@ -7279,7 +7609,7 @@
       <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="43" t="s">
         <v>172</v>
       </c>
       <c r="B3" s="21">
@@ -7291,7 +7621,7 @@
       <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="41" t="s">
         <v>163</v>
       </c>
       <c r="B4" s="18"/>
@@ -7299,7 +7629,7 @@
       <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="44" t="s">
         <v>173</v>
       </c>
       <c r="B5" s="21">
@@ -7311,7 +7641,7 @@
       <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="41" t="s">
         <v>215</v>
       </c>
       <c r="B6" s="18"/>
@@ -7319,8 +7649,8 @@
       <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>240</v>
+      <c r="A7" s="44" t="s">
+        <v>239</v>
       </c>
       <c r="B7" s="21">
         <v>63</v>
@@ -7331,8 +7661,8 @@
       <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
-        <v>241</v>
+      <c r="A8" s="42" t="s">
+        <v>240</v>
       </c>
       <c r="B8" s="18">
         <v>103</v>
@@ -7343,7 +7673,7 @@
       <c r="D8" s="30"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="44" t="s">
         <v>176</v>
       </c>
       <c r="B9" s="21">
@@ -7355,7 +7685,7 @@
       <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="41" t="s">
         <v>216</v>
       </c>
       <c r="B10" s="18"/>
@@ -7363,8 +7693,8 @@
       <c r="D10" s="30"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>242</v>
+      <c r="A11" s="44" t="s">
+        <v>241</v>
       </c>
       <c r="B11" s="21">
         <v>42</v>
@@ -7375,8 +7705,8 @@
       <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>243</v>
+      <c r="A12" s="42" t="s">
+        <v>242</v>
       </c>
       <c r="B12" s="18">
         <v>111</v>
@@ -7387,7 +7717,7 @@
       <c r="D12" s="30"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="44" t="s">
         <v>179</v>
       </c>
       <c r="B13" s="21">
@@ -7399,7 +7729,7 @@
       <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="41" t="s">
         <v>217</v>
       </c>
       <c r="B14" s="18"/>
@@ -7407,8 +7737,8 @@
       <c r="D14" s="30"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
-        <v>244</v>
+      <c r="A15" s="44" t="s">
+        <v>243</v>
       </c>
       <c r="B15" s="21">
         <v>61</v>
@@ -7419,8 +7749,8 @@
       <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>245</v>
+      <c r="A16" s="42" t="s">
+        <v>244</v>
       </c>
       <c r="B16" s="18">
         <v>84</v>
@@ -7431,7 +7761,7 @@
       <c r="D16" s="30"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="40" t="s">
         <v>218</v>
       </c>
       <c r="B17" s="21"/>
@@ -7439,8 +7769,8 @@
       <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>246</v>
+      <c r="A18" s="42" t="s">
+        <v>245</v>
       </c>
       <c r="B18" s="18">
         <v>56</v>
@@ -7451,8 +7781,8 @@
       <c r="D18" s="30"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>247</v>
+      <c r="A19" s="44" t="s">
+        <v>246</v>
       </c>
       <c r="B19" s="21">
         <v>23</v>
@@ -7463,7 +7793,7 @@
       <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="41" t="s">
         <v>219</v>
       </c>
       <c r="B20" s="18"/>
@@ -7471,8 +7801,8 @@
       <c r="D20" s="30"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>248</v>
+      <c r="A21" s="44" t="s">
+        <v>247</v>
       </c>
       <c r="B21" s="21">
         <v>100</v>
@@ -7483,7 +7813,7 @@
       <c r="D21" s="31"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="42" t="s">
         <v>185</v>
       </c>
       <c r="B22" s="18">
@@ -7495,8 +7825,8 @@
       <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
-        <v>249</v>
+      <c r="A23" s="44" t="s">
+        <v>248</v>
       </c>
       <c r="B23" s="21">
         <v>50</v>
@@ -7507,7 +7837,7 @@
       <c r="D23" s="31"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="42" t="s">
         <v>220</v>
       </c>
       <c r="B24" s="18"/>
@@ -7515,8 +7845,8 @@
       <c r="D24" s="30"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>250</v>
+      <c r="A25" s="44" t="s">
+        <v>249</v>
       </c>
       <c r="B25" s="21">
         <v>25</v>
@@ -7527,7 +7857,7 @@
       <c r="D25" s="31"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="41" t="s">
         <v>221</v>
       </c>
       <c r="B26" s="18"/>
@@ -7535,8 +7865,8 @@
       <c r="D26" s="30"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>251</v>
+      <c r="A27" s="44" t="s">
+        <v>250</v>
       </c>
       <c r="B27" s="21">
         <v>41</v>
@@ -7547,8 +7877,8 @@
       <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>252</v>
+      <c r="A28" s="42" t="s">
+        <v>251</v>
       </c>
       <c r="B28" s="18">
         <v>77</v>
@@ -7559,8 +7889,8 @@
       <c r="D28" s="30"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
-        <v>253</v>
+      <c r="A29" s="44" t="s">
+        <v>252</v>
       </c>
       <c r="B29" s="21">
         <v>42</v>
@@ -7571,8 +7901,8 @@
       <c r="D29" s="31"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>254</v>
+      <c r="A30" s="42" t="s">
+        <v>253</v>
       </c>
       <c r="B30" s="18">
         <v>146</v>
@@ -7583,7 +7913,7 @@
       <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="40" t="s">
         <v>222</v>
       </c>
       <c r="B31" s="21"/>
@@ -7591,8 +7921,8 @@
       <c r="D31" s="31"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>255</v>
+      <c r="A32" s="42" t="s">
+        <v>254</v>
       </c>
       <c r="B32" s="18">
         <v>58</v>
@@ -7603,8 +7933,8 @@
       <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="20" t="s">
-        <v>256</v>
+      <c r="A33" s="44" t="s">
+        <v>255</v>
       </c>
       <c r="B33" s="21">
         <v>71</v>
@@ -7615,7 +7945,7 @@
       <c r="D33" s="31"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="41" t="s">
         <v>223</v>
       </c>
       <c r="B34" s="18"/>
@@ -7623,8 +7953,8 @@
       <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
-        <v>257</v>
+      <c r="A35" s="44" t="s">
+        <v>256</v>
       </c>
       <c r="B35" s="21">
         <v>41</v>
@@ -7635,8 +7965,8 @@
       <c r="D35" s="31"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
-        <v>258</v>
+      <c r="A36" s="42" t="s">
+        <v>257</v>
       </c>
       <c r="B36" s="18">
         <v>110</v>
@@ -7647,8 +7977,8 @@
       <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="20" t="s">
-        <v>259</v>
+      <c r="A37" s="44" t="s">
+        <v>258</v>
       </c>
       <c r="B37" s="21">
         <v>2</v>
@@ -7659,7 +7989,7 @@
       <c r="D37" s="31"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="41" t="s">
         <v>224</v>
       </c>
       <c r="B38" s="18"/>
@@ -7667,8 +7997,8 @@
       <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
-        <v>260</v>
+      <c r="A39" s="44" t="s">
+        <v>259</v>
       </c>
       <c r="B39" s="21">
         <v>54</v>
@@ -7679,8 +8009,8 @@
       <c r="D39" s="31"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>261</v>
+      <c r="A40" s="42" t="s">
+        <v>260</v>
       </c>
       <c r="B40" s="18">
         <v>71</v>
@@ -7691,7 +8021,7 @@
       <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="40" t="s">
         <v>225</v>
       </c>
       <c r="B41" s="21"/>
@@ -7699,8 +8029,8 @@
       <c r="D41" s="31"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
-        <v>262</v>
+      <c r="A42" s="42" t="s">
+        <v>261</v>
       </c>
       <c r="B42" s="18">
         <v>56</v>
@@ -7711,8 +8041,8 @@
       <c r="D42" s="30"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="20" t="s">
-        <v>263</v>
+      <c r="A43" s="44" t="s">
+        <v>262</v>
       </c>
       <c r="B43" s="21">
         <v>53</v>
@@ -7723,7 +8053,7 @@
       <c r="D43" s="31"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="41" t="s">
         <v>226</v>
       </c>
       <c r="B44" s="18"/>
@@ -7731,8 +8061,8 @@
       <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="20" t="s">
-        <v>264</v>
+      <c r="A45" s="44" t="s">
+        <v>263</v>
       </c>
       <c r="B45" s="21">
         <v>32</v>
@@ -7743,8 +8073,8 @@
       <c r="D45" s="31"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>265</v>
+      <c r="A46" s="42" t="s">
+        <v>264</v>
       </c>
       <c r="B46" s="18">
         <v>86</v>
@@ -7755,8 +8085,8 @@
       <c r="D46" s="30"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
-        <v>266</v>
+      <c r="A47" s="44" t="s">
+        <v>265</v>
       </c>
       <c r="B47" s="21">
         <v>20</v>
@@ -7767,7 +8097,7 @@
       <c r="D47" s="31"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="41" t="s">
         <v>227</v>
       </c>
       <c r="B48" s="18"/>
@@ -7775,7 +8105,7 @@
       <c r="D48" s="30"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="44" t="s">
         <v>190</v>
       </c>
       <c r="B49" s="21">
@@ -7787,7 +8117,7 @@
       <c r="D49" s="31"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="41" t="s">
         <v>228</v>
       </c>
       <c r="B50" s="18"/>
@@ -7795,8 +8125,8 @@
       <c r="D50" s="30"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="20" t="s">
-        <v>267</v>
+      <c r="A51" s="44" t="s">
+        <v>266</v>
       </c>
       <c r="B51" s="21">
         <v>26</v>
@@ -7807,8 +8137,8 @@
       <c r="D51" s="31"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="17" t="s">
-        <v>268</v>
+      <c r="A52" s="42" t="s">
+        <v>267</v>
       </c>
       <c r="B52" s="18">
         <v>75</v>
@@ -7819,7 +8149,7 @@
       <c r="D52" s="30"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="40" t="s">
         <v>229</v>
       </c>
       <c r="B53" s="21"/>
@@ -7827,8 +8157,8 @@
       <c r="D53" s="31"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="s">
-        <v>269</v>
+      <c r="A54" s="42" t="s">
+        <v>268</v>
       </c>
       <c r="B54" s="18">
         <v>53</v>
@@ -7839,8 +8169,8 @@
       <c r="D54" s="30"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="s">
-        <v>270</v>
+      <c r="A55" s="44" t="s">
+        <v>269</v>
       </c>
       <c r="B55" s="21">
         <v>62</v>
@@ -7851,7 +8181,7 @@
       <c r="D55" s="31"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="41" t="s">
         <v>230</v>
       </c>
       <c r="B56" s="18"/>
@@ -7859,8 +8189,8 @@
       <c r="D56" s="30"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="20" t="s">
-        <v>271</v>
+      <c r="A57" s="44" t="s">
+        <v>270</v>
       </c>
       <c r="B57" s="21">
         <v>97</v>
@@ -7871,7 +8201,7 @@
       <c r="D57" s="31"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="41" t="s">
         <v>231</v>
       </c>
       <c r="B58" s="18"/>
@@ -7879,8 +8209,8 @@
       <c r="D58" s="30"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="20" t="s">
-        <v>272</v>
+      <c r="A59" s="44" t="s">
+        <v>271</v>
       </c>
       <c r="B59" s="21">
         <v>33</v>
@@ -7891,8 +8221,8 @@
       <c r="D59" s="31"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="17" t="s">
-        <v>273</v>
+      <c r="A60" s="45" t="s">
+        <v>272</v>
       </c>
       <c r="B60" s="18">
         <v>69</v>
@@ -7903,8 +8233,8 @@
       <c r="D60" s="30"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="20" t="s">
-        <v>274</v>
+      <c r="A61" s="44" t="s">
+        <v>273</v>
       </c>
       <c r="B61" s="21">
         <v>4</v>
@@ -7915,7 +8245,7 @@
       <c r="D61" s="31"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="41" t="s">
         <v>232</v>
       </c>
       <c r="B62" s="18"/>
@@ -7923,8 +8253,8 @@
       <c r="D62" s="30"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="20" t="s">
-        <v>275</v>
+      <c r="A63" s="44" t="s">
+        <v>274</v>
       </c>
       <c r="B63" s="21">
         <v>51</v>
@@ -7935,8 +8265,8 @@
       <c r="D63" s="31"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
-        <v>276</v>
+      <c r="A64" s="42" t="s">
+        <v>275</v>
       </c>
       <c r="B64" s="18">
         <v>23</v>
@@ -7947,8 +8277,8 @@
       <c r="D64" s="30"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="20" t="s">
-        <v>277</v>
+      <c r="A65" s="44" t="s">
+        <v>276</v>
       </c>
       <c r="B65" s="21">
         <v>5</v>
@@ -7959,7 +8289,7 @@
       <c r="D65" s="31"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="41" t="s">
         <v>233</v>
       </c>
       <c r="B66" s="18"/>
@@ -7967,8 +8297,8 @@
       <c r="D66" s="30"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="20" t="s">
-        <v>278</v>
+      <c r="A67" s="44" t="s">
+        <v>277</v>
       </c>
       <c r="B67" s="21">
         <v>81</v>
@@ -7979,8 +8309,8 @@
       <c r="D67" s="31"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="17" t="s">
-        <v>279</v>
+      <c r="A68" s="42" t="s">
+        <v>278</v>
       </c>
       <c r="B68" s="18">
         <v>59</v>
@@ -7991,7 +8321,7 @@
       <c r="D68" s="30"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="20" t="s">
+      <c r="A69" s="40" t="s">
         <v>234</v>
       </c>
       <c r="B69" s="21"/>
@@ -7999,8 +8329,8 @@
       <c r="D69" s="31"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
-        <v>280</v>
+      <c r="A70" s="42" t="s">
+        <v>279</v>
       </c>
       <c r="B70" s="18">
         <v>22</v>
@@ -8011,8 +8341,8 @@
       <c r="D70" s="30"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="20" t="s">
-        <v>281</v>
+      <c r="A71" s="44" t="s">
+        <v>280</v>
       </c>
       <c r="B71" s="21">
         <v>64</v>
@@ -8023,7 +8353,7 @@
       <c r="D71" s="31"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="41" t="s">
         <v>235</v>
       </c>
       <c r="B72" s="18"/>
@@ -8031,8 +8361,8 @@
       <c r="D72" s="30"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="20" t="s">
-        <v>282</v>
+      <c r="A73" s="44" t="s">
+        <v>281</v>
       </c>
       <c r="B73" s="21">
         <v>98</v>
@@ -8043,7 +8373,7 @@
       <c r="D73" s="31"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="41" t="s">
         <v>236</v>
       </c>
       <c r="B74" s="18"/>
@@ -8051,8 +8381,8 @@
       <c r="D74" s="30"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="20" t="s">
-        <v>283</v>
+      <c r="A75" s="44" t="s">
+        <v>282</v>
       </c>
       <c r="B75" s="21">
         <v>75</v>
@@ -8063,157 +8393,149 @@
       <c r="D75" s="31"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="B76" s="21">
+        <v>29</v>
+      </c>
+      <c r="C76" s="21">
+        <v>56</v>
+      </c>
+      <c r="D76" s="31"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="41" t="s">
         <v>237</v>
       </c>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="30"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="20" t="s">
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="30"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="44" t="s">
         <v>284</v>
       </c>
-      <c r="B77" s="21">
-        <v>29</v>
-      </c>
-      <c r="C77" s="21">
-        <v>56</v>
-      </c>
-      <c r="D77" s="31"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="17" t="s">
+      <c r="B78" s="21">
+        <v>64</v>
+      </c>
+      <c r="C78" s="21">
+        <v>10</v>
+      </c>
+      <c r="D78" s="31"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="B79" s="18">
+        <v>78</v>
+      </c>
+      <c r="C79" s="18">
+        <v>7</v>
+      </c>
+      <c r="D79" s="30"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="40" t="s">
         <v>238</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="30"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="B79" s="21">
-        <v>64</v>
-      </c>
-      <c r="C79" s="21">
-        <v>10</v>
-      </c>
-      <c r="D79" s="31"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="B80" s="18">
-        <v>78</v>
-      </c>
-      <c r="C80" s="18">
-        <v>7</v>
-      </c>
-      <c r="D80" s="30"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="31"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A81" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="B81" s="21"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="31"/>
+      <c r="A81" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" s="18">
+        <v>40</v>
+      </c>
+      <c r="C81" s="18">
+        <v>16</v>
+      </c>
+      <c r="D81" s="30"/>
+      <c r="H81" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="I81" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="J81" s="27" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A82" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B82" s="18">
-        <v>40</v>
-      </c>
-      <c r="C82" s="18">
-        <v>16</v>
-      </c>
-      <c r="D82" s="30"/>
-      <c r="H82" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="I82" s="27" t="s">
-        <v>303</v>
-      </c>
-      <c r="J82" s="27" t="s">
-        <v>304</v>
+      <c r="A82" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="B82" s="7">
+        <v>46</v>
+      </c>
+      <c r="C82" s="7">
+        <v>34</v>
+      </c>
+      <c r="D82" s="29"/>
+      <c r="H82" s="27">
+        <v>48</v>
+      </c>
+      <c r="I82" s="27">
+        <v>39</v>
+      </c>
+      <c r="J82" s="27">
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B83" s="7">
-        <v>46</v>
-      </c>
-      <c r="C83" s="7">
-        <v>34</v>
-      </c>
-      <c r="D83" s="29"/>
-      <c r="H83" s="27">
-        <v>48</v>
-      </c>
-      <c r="I83" s="27">
-        <v>39</v>
-      </c>
-      <c r="J83" s="27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A84" s="25" t="str">
+      <c r="A83" s="25" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：48:39:04</v>
       </c>
+      <c r="H83" s="27">
+        <v>5</v>
+      </c>
+      <c r="I83" s="27">
+        <v>23</v>
+      </c>
+      <c r="J83" s="27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H84" s="27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I84" s="27">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J84" s="27">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H85" s="27">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="I85" s="27">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="J85" s="27">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H86" s="27">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="I86" s="27">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="J86" s="27">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H87" s="27">
-        <v>21</v>
-      </c>
-      <c r="I87" s="27">
-        <v>8</v>
-      </c>
-      <c r="J87" s="27">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G88" s="28" t="str">
+      <c r="G87" s="28" t="str">
         <f>TEXT(SUM(H:H)/24+SUM(I:I)/1440+SUM(J:J)/86400,"[h]:m:s")</f>
         <v>128:15:30</v>
       </c>
@@ -8229,7 +8551,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -9197,6 +9519,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA86E1BE-FCFE-4251-B0EC-E291DDB8C47B}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9353,10 +9676,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7AC606-BCBF-4838-A963-4BC4664217AA}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added notes for 05_JS_end:Ch01L01: Environment initialization
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F5BAEB-D5B1-4348-8C4A-05E85890F70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFBBAE1-A1B5-4E7D-BAA8-2CE912E03110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1710" windowWidth="20565" windowHeight="13140" firstSheet="4" activeTab="9" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="5115" yWindow="1710" windowWidth="20565" windowHeight="13140" firstSheet="4" activeTab="5" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -3068,7 +3068,9 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8549,10 +8551,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080A7672-DAE8-47CE-809E-69717AE44590}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8563,7 +8565,7 @@
     <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>35</v>
       </c>
@@ -8577,7 +8579,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -8591,7 +8593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
@@ -8605,7 +8607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
@@ -8619,7 +8621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
@@ -8633,7 +8635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
@@ -8647,7 +8649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
@@ -8661,7 +8663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>32</v>
       </c>
@@ -8674,8 +8676,12 @@
       <c r="D8" s="19">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="str">
+        <f>TEXT(SUM(B2:B8)/1440+SUM(C2:C8)/86400,"[h]:mm:ss")</f>
+        <v>3:46:29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>33</v>
       </c>
@@ -8689,7 +8695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>34</v>
       </c>
@@ -8703,7 +8709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>5</v>
       </c>
@@ -8717,7 +8723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>6</v>
       </c>
@@ -8731,7 +8737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>7</v>
       </c>
@@ -8745,7 +8751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>8</v>
       </c>
@@ -8758,8 +8764,12 @@
       <c r="D14" s="19">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F14" t="str">
+        <f>TEXT(SUM(B9:B14)/1440+SUM(C9:C14)/86400,"[h]:mm:ss")</f>
+        <v>3:33:23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>9</v>
       </c>
@@ -8773,7 +8783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>10</v>
       </c>
@@ -8787,7 +8797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>11</v>
       </c>
@@ -8801,7 +8811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>12</v>
       </c>
@@ -8815,7 +8825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>13</v>
       </c>
@@ -8829,7 +8839,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>14</v>
       </c>
@@ -8842,8 +8852,12 @@
       <c r="D20" s="19">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" t="str">
+        <f>TEXT(SUM(B15:B20)/1440+SUM(C15:C20)/86400,"[h]:mm:ss")</f>
+        <v>3:45:24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>15</v>
       </c>
@@ -8857,7 +8871,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>16</v>
       </c>
@@ -8871,7 +8885,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>17</v>
       </c>
@@ -8885,7 +8899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>18</v>
       </c>
@@ -8899,7 +8913,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>19</v>
       </c>
@@ -8912,8 +8926,12 @@
       <c r="D25" s="22">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25" t="str">
+        <f>TEXT(SUM(B21:B25)/1440+SUM(C21:C25)/86400,"[h]:mm:ss")</f>
+        <v>3:53:58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>20</v>
       </c>
@@ -8927,7 +8945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>21</v>
       </c>
@@ -8941,7 +8959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>22</v>
       </c>
@@ -8955,7 +8973,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>23</v>
       </c>
@@ -8969,7 +8987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>24</v>
       </c>
@@ -8983,7 +9001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>25</v>
       </c>
@@ -8997,7 +9015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>26</v>
       </c>
@@ -9010,8 +9028,12 @@
       <c r="D32" s="19">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F32" t="str">
+        <f>TEXT(SUM(B26:B31)/1440+SUM(C26:C31)/86400,"[h]:mm:ss")</f>
+        <v>4:08:02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>27</v>
       </c>
@@ -9025,7 +9047,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>28</v>
       </c>
@@ -9039,7 +9061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
         <v>29</v>
       </c>
@@ -9053,7 +9075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>30</v>
       </c>
@@ -9066,8 +9088,12 @@
       <c r="D36" s="23">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F36" t="str">
+        <f>TEXT(SUM(B33:B36)/1440+SUM(C33:C36)/86400,"[h]:mm:ss")</f>
+        <v>2:41:59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：22:14:57</v>

</xml_diff>

<commit_message>
Created blank notes for this 05_JS_end section
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFBBAE1-A1B5-4E7D-BAA8-2CE912E03110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE1B3B2-223E-4A8D-A9DF-494AC01214DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5115" yWindow="1710" windowWidth="20565" windowHeight="13140" firstSheet="4" activeTab="5" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -8553,8 +8553,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added notes for 05_JS_end:L29: JS Regular Expression
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE1B3B2-223E-4A8D-A9DF-494AC01214DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D005AF-4300-4387-B4F8-653AA9C1C18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1710" windowWidth="20565" windowHeight="13140" firstSheet="4" activeTab="5" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="8400" yWindow="1560" windowWidth="17280" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="4" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="601">
   <si>
     <t>1. 环境准备</t>
   </si>
@@ -1892,6 +1892,10 @@
   </si>
   <si>
     <t>5.尾声：学无止境</t>
+  </si>
+  <si>
+    <t>Ch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1999,7 +2003,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2018,8 +2022,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2108,13 +2118,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2256,11 +2315,189 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2271,6 +2508,58 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}" name="表1" displayName="表1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="10">
+  <autoFilter ref="A1:D14" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{17F2527D-78B5-4B06-A96C-9154CE44E0C2}" name="Title"/>
+    <tableColumn id="2" xr3:uid="{EE3C824F-40FF-4F88-B4B9-C5214BACA1F1}" name="Minutes"/>
+    <tableColumn id="3" xr3:uid="{230A3F53-7EAB-4152-BC42-0BA62C77BB5C}" name="Seconds"/>
+    <tableColumn id="4" xr3:uid="{F7B7FE7E-C186-4BD5-89FC-F90A3311F416}" name="Day"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="8">
+  <autoFilter ref="A1:D8" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{56E13753-3D18-4640-894E-A9862A8519E9}" name="Title"/>
+    <tableColumn id="2" xr3:uid="{79D6C646-1226-4C28-B1C9-44701A88F7AD}" name="Minutes"/>
+    <tableColumn id="3" xr3:uid="{D0893D73-54C6-4CE8-BA7E-4CA7DAFD42BB}" name="Seconds"/>
+    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="5">
+  <autoFilter ref="A1:D8" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{12D9D257-0720-4D69-92DB-DAB28C2BA457}" name="Title"/>
+    <tableColumn id="2" xr3:uid="{16E320F3-22A7-423A-B471-F02438A5F8A6}" name="Minutes"/>
+    <tableColumn id="3" xr3:uid="{64AD87D5-100E-459C-BDDA-2972741296A6}" name="Seconds"/>
+    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:D9" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A51B88B7-4A2F-4D5C-A477-AFA8072799E1}" name="Title"/>
+    <tableColumn id="2" xr3:uid="{4A08D9E2-7055-4737-913C-04F2C5ED46F0}" name="Minutes"/>
+    <tableColumn id="3" xr3:uid="{0EDD753B-5FBA-424C-9B63-06AEEA8E4D71}" name="Seconds"/>
+    <tableColumn id="4" xr3:uid="{35807557-36BB-4B11-8AC2-863BC91B2108}" name="Day"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2593,7 +2882,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
@@ -3068,8 +3357,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4353,255 +4642,568 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC9628E-F669-40A2-855C-BA931809CE20}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A2:A14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.625" customWidth="1"/>
+    <col min="3" max="3" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>41</v>
+      </c>
+      <c r="C9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>54</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>41</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>316</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：7:32:31</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176B4581-7942-4FCC-A12F-3EC4A3FA8D07}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A2:A8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>72</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>323</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：3:02:48</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B832BBF-CF90-430B-B2E0-B6425812829B}">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A2:A8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>82</v>
+      </c>
+      <c r="C2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>38</v>
+      </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>330</v>
+      </c>
+      <c r="B8">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：4:57:07</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00865C93-FCC5-4D30-A25D-4C01DD061FF8}">
   <sheetPr codeName="Sheet15"/>
-  <dimension ref="A2:A9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>54</v>
+      </c>
+      <c r="C2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>67</v>
+      </c>
+      <c r="C3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>91</v>
+      </c>
+      <c r="C8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>338</v>
+      </c>
+      <c r="B9">
+        <v>110</v>
+      </c>
+      <c r="C9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：7:34:27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4611,7 +5213,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4844,7 +5446,7 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -5371,7 +5973,7 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -6330,7 +6932,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="A65" workbookViewId="0">
       <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
@@ -7575,10 +8177,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078994BB-162C-4327-BF62-6D3636325352}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89:K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8446,7 +9048,7 @@
       <c r="C80" s="21"/>
       <c r="D80" s="31"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="42" t="s">
         <v>188</v>
       </c>
@@ -8466,8 +9068,11 @@
       <c r="J81" s="27" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81" s="27" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="46" t="s">
         <v>189</v>
       </c>
@@ -8479,67 +9084,266 @@
       </c>
       <c r="D82" s="29"/>
       <c r="H82" s="27">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="I82" s="27">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="J82" s="27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="K82" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="25" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：48:39:04</v>
       </c>
       <c r="H83" s="27">
+        <v>48</v>
+      </c>
+      <c r="I83" s="27">
+        <v>39</v>
+      </c>
+      <c r="J83" s="27">
+        <v>4</v>
+      </c>
+      <c r="K83" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H84" s="27">
+        <v>48</v>
+      </c>
+      <c r="I84" s="27">
+        <v>45</v>
+      </c>
+      <c r="J84" s="27">
+        <v>42</v>
+      </c>
+      <c r="K84" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H85" s="27">
+        <v>4</v>
+      </c>
+      <c r="I85" s="27">
+        <v>18</v>
+      </c>
+      <c r="J85" s="27">
+        <v>18</v>
+      </c>
+      <c r="K85" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H86" s="27">
         <v>5</v>
       </c>
-      <c r="I83" s="27">
+      <c r="I86" s="27">
         <v>23</v>
       </c>
-      <c r="J83" s="27">
+      <c r="J86" s="27">
         <v>34</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H84" s="27">
+      <c r="K86" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G87" s="28" t="str">
+        <f>TEXT(SUM(H82:H87)/24+SUM(I82:I87)/1440+SUM(J82:J87)/86400,"[h]:m:s")</f>
+        <v>150:30:27</v>
+      </c>
+      <c r="H87" s="27">
+        <v>22</v>
+      </c>
+      <c r="I87" s="27">
+        <v>14</v>
+      </c>
+      <c r="J87" s="27">
+        <v>57</v>
+      </c>
+      <c r="K87" s="27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H88" s="27">
+        <v>17</v>
+      </c>
+      <c r="I88" s="27">
         <v>4</v>
       </c>
-      <c r="I84" s="27">
+      <c r="J88" s="27">
+        <v>17</v>
+      </c>
+      <c r="K88" s="27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H89" s="27">
+        <v>6</v>
+      </c>
+      <c r="I89" s="27">
+        <v>56</v>
+      </c>
+      <c r="J89" s="27">
+        <v>56</v>
+      </c>
+      <c r="K89" s="27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H90" s="27">
+        <v>10</v>
+      </c>
+      <c r="I90" s="27">
+        <v>30</v>
+      </c>
+      <c r="J90" s="27">
+        <v>6</v>
+      </c>
+      <c r="K90" s="27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K91" s="27">
+        <v>10</v>
+      </c>
+      <c r="M91" s="27">
+        <v>79</v>
+      </c>
+      <c r="N91" s="27">
+        <v>3</v>
+      </c>
+      <c r="O91" s="27">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H92" s="27">
+        <v>4</v>
+      </c>
+      <c r="I92" s="27">
+        <v>23</v>
+      </c>
+      <c r="J92" s="27">
+        <v>29</v>
+      </c>
+      <c r="K92" s="27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H93" s="27">
+        <v>7</v>
+      </c>
+      <c r="I93" s="27">
+        <v>32</v>
+      </c>
+      <c r="J93" s="27">
+        <v>31</v>
+      </c>
+      <c r="K93" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H94" s="27">
+        <v>3</v>
+      </c>
+      <c r="I94" s="27">
+        <v>2</v>
+      </c>
+      <c r="J94" s="27">
+        <v>48</v>
+      </c>
+      <c r="K94" s="27">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H95" s="27">
+        <v>4</v>
+      </c>
+      <c r="I95" s="27">
+        <v>57</v>
+      </c>
+      <c r="J95" s="27">
+        <v>7</v>
+      </c>
+      <c r="K95" s="27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H96" s="27">
+        <v>7</v>
+      </c>
+      <c r="I96" s="27">
+        <v>34</v>
+      </c>
+      <c r="J96" s="27">
+        <v>27</v>
+      </c>
+      <c r="K96" s="27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="K97" s="53">
+        <v>16</v>
+      </c>
+      <c r="M97" s="27">
+        <v>8</v>
+      </c>
+      <c r="N97" s="27">
+        <v>7</v>
+      </c>
+      <c r="O97" s="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="H98" s="27">
+        <v>28</v>
+      </c>
+      <c r="I98" s="27">
+        <v>1</v>
+      </c>
+      <c r="J98" s="27">
+        <v>5</v>
+      </c>
+      <c r="K98" s="54">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="G99" s="28" t="str">
+        <f>TEXT(SUM(H88:H99)/24+SUM(I88:I99)/1440+SUM(J88:J99)/86400,"[h]:m:s")</f>
+        <v>106:33:30</v>
+      </c>
+      <c r="H99" s="27">
+        <v>16</v>
+      </c>
+      <c r="I99" s="27">
+        <v>30</v>
+      </c>
+      <c r="J99" s="27">
+        <v>44</v>
+      </c>
+      <c r="K99" s="54">
         <v>18</v>
-      </c>
-      <c r="J84" s="27">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H85" s="27">
-        <v>48</v>
-      </c>
-      <c r="I85" s="27">
-        <v>45</v>
-      </c>
-      <c r="J85" s="27">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H86" s="27">
-        <v>21</v>
-      </c>
-      <c r="I86" s="27">
-        <v>8</v>
-      </c>
-      <c r="J86" s="27">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G87" s="28" t="str">
-        <f>TEXT(SUM(H:H)/24+SUM(I:I)/1440+SUM(J:J)/86400,"[h]:m:s")</f>
-        <v>128:15:30</v>
       </c>
     </row>
   </sheetData>
@@ -8553,8 +9357,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9112,7 +9916,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -9706,7 +10510,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added notes for 06_JS_proj:L01:item scrolling effect
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D005AF-4300-4387-B4F8-653AA9C1C18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B33FF9-A124-4E9C-BBB2-46E1C34F6467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="1560" windowWidth="17280" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="4" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" firstSheet="6" activeTab="4" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -2318,7 +2318,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2345,39 +2345,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -2385,83 +2352,10 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -2497,6 +2391,112 @@
         </top>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2511,7 +2511,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}" name="表1" displayName="表1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}" name="表1" displayName="表1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:D14" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{17F2527D-78B5-4B06-A96C-9154CE44E0C2}" name="Title"/>
@@ -2524,7 +2524,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A1:D8" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{56E13753-3D18-4640-894E-A9862A8519E9}" name="Title"/>
@@ -2537,7 +2537,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:D8" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{12D9D257-0720-4D69-92DB-DAB28C2BA457}" name="Title"/>
@@ -2550,7 +2550,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:D9" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A51B88B7-4A2F-4D5C-A477-AFA8072799E1}" name="Title"/>
@@ -8180,7 +8180,7 @@
   <dimension ref="A1:O99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89:K89"/>
+      <selection activeCell="O89" sqref="O89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated README and overall progress in Excel
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B33FF9-A124-4E9C-BBB2-46E1C34F6467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0822B6BD-B901-4DE5-95D0-8527DD2EFE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" firstSheet="6" activeTab="4" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="6795" yWindow="1815" windowWidth="17280" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="4" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -1902,7 +1902,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1997,6 +1997,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -2173,7 +2181,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2337,6 +2345,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8180,7 +8206,7 @@
   <dimension ref="A1:O99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="O89" sqref="O89"/>
+      <selection activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9917,7 +9943,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9942,58 +9968,58 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="56">
         <v>3</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="56">
         <v>38</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="57">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="59">
         <v>40</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="59">
         <v>47</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="60">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="56">
         <v>32</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="56">
         <v>41</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="57">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="59">
         <v>34</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="59">
         <v>35</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="60">
         <v>2</v>
       </c>
     </row>
@@ -10166,30 +10192,30 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="56">
         <v>27</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="56">
         <v>53</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="57">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="59">
         <v>78</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="59">
         <v>51</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="60">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated progress in Excel
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0822B6BD-B901-4DE5-95D0-8527DD2EFE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEA79CE-7FEA-4288-B30C-11761DEF4F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="1815" windowWidth="17280" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="4" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" firstSheet="4" activeTab="7" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -3383,8 +3383,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4587,7 +4587,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4671,7 +4671,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8205,7 +8205,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
+    <sheetView topLeftCell="B74" workbookViewId="0">
       <selection activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
@@ -9942,8 +9942,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10024,170 +10024,170 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="56">
         <v>4</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="56">
         <v>0</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="57">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="59">
         <v>57</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="59">
         <v>37</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="60">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="56">
         <v>2</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="56">
         <v>9</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="57">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="59">
         <v>44</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="59">
         <v>51</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="60">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="56">
         <v>3</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="56">
         <v>29</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="57">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="59">
         <v>64</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="59">
         <v>5</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="60">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="56">
         <v>2</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="56">
         <v>16</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="57">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="59">
         <v>59</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="59">
         <v>15</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="60">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="56">
         <v>7</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="56">
         <v>40</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="57">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="59">
         <v>95</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="59">
         <v>44</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="60">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="56">
         <v>15</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="56">
         <v>23</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="57">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="59">
         <v>36</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="59">
         <v>10</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="60">
         <v>8</v>
       </c>
     </row>
@@ -10378,8 +10378,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10404,58 +10404,58 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="56">
         <v>58</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="56">
         <v>14</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="57">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="59">
         <v>56</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="59">
         <v>1</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="60">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="56">
         <v>67</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="56">
         <v>55</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="57">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="59">
         <v>49</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="59">
         <v>2</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="60">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added notes for 06_JS_proj:L12: gomoku game with vanilla JS
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEA79CE-7FEA-4288-B30C-11761DEF4F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F677A03-8076-4A3B-99E1-67E9A170E749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" firstSheet="4" activeTab="7" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="6" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -9942,8 +9942,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10220,86 +10220,86 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="56">
         <v>18</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="56">
         <v>50</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="57">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="59">
         <v>53</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="59">
         <v>2</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="60">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="56">
         <v>15</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="56">
         <v>43</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="57">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="59">
         <v>52</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="59">
         <v>38</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="60">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="56">
         <v>9</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="56">
         <v>48</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="57">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="59">
         <v>76</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="59">
         <v>39</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="60">
         <v>12</v>
       </c>
     </row>
@@ -10378,7 +10378,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added notes for 06_JS_proj:L13: Mind Reader Game with vanilla JS
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F677A03-8076-4A3B-99E1-67E9A170E749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCF5D84-82B3-403A-9BE9-EBA43D1935FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="6" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -9943,7 +9943,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10304,30 +10304,30 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="56">
         <v>36</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="56">
         <v>18</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="57">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="59">
         <v>51</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="59">
         <v>58</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="60">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated notes for 06_JS_proj:L13: Mind Reader Game with vanilla JS
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCF5D84-82B3-403A-9BE9-EBA43D1935FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21CD4DC-29C7-428D-9BB2-9A269B4AFB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="6" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -9943,7 +9943,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added notes for 06_JS_proj:L14: Draggable Image Validation
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21CD4DC-29C7-428D-9BB2-9A269B4AFB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAC51A0-6605-4325-8EC7-2A155146F9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="6" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -2181,7 +2181,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2363,6 +2363,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -9943,7 +9952,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10332,30 +10341,30 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="56">
         <v>22</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="56">
         <v>56</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="57">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="62">
         <v>75</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="62">
         <v>21</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="63">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
init blank notes & folders for section 07:HTML5 & CSS3
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAC51A0-6605-4325-8EC7-2A155146F9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAEFC96-1A90-4769-A472-6783EC0975C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="6" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="7" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -8215,7 +8215,7 @@
   <dimension ref="A1:O99"/>
   <sheetViews>
     <sheetView topLeftCell="B74" workbookViewId="0">
-      <selection activeCell="K89" sqref="K89"/>
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9365,8 +9365,8 @@
     </row>
     <row r="99" spans="7:15" x14ac:dyDescent="0.2">
       <c r="G99" s="28" t="str">
-        <f>TEXT(SUM(H88:H99)/24+SUM(I88:I99)/1440+SUM(J88:J99)/86400,"[h]:m:s")</f>
-        <v>106:33:30</v>
+        <f>TEXT(SUM(H89:H99)/24+SUM(I89:I99)/1440+SUM(J89:J99)/86400,"[h]:m:s")</f>
+        <v>89:29:13</v>
       </c>
       <c r="H99" s="27">
         <v>16</v>
@@ -9951,7 +9951,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -10387,7 +10387,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added notes for 08_JS_ES6_Plug:L01: overview
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C844A546-8118-4F42-9ABC-23C092F2AC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC7AAF2-DBAB-4850-B130-08D06DD6048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="7" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="8" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -9187,10 +9187,6 @@
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G87" s="27" t="str">
-        <f>TEXT(SUM(H82:H87)/24+SUM(I82:I87)/1440+SUM(J82:J87)/86400,"[h]:m:s")</f>
-        <v>150:30:27</v>
-      </c>
       <c r="H87" s="26">
         <v>22</v>
       </c>
@@ -9219,6 +9215,10 @@
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G89" s="27" t="str">
+        <f>TEXT(SUM(H82:H89)/24+SUM(I82:I89)/1440+SUM(J82:J89)/86400,"[h]:m:s")</f>
+        <v>174:31:40</v>
+      </c>
       <c r="H89" s="26">
         <v>6</v>
       </c>
@@ -9360,8 +9360,8 @@
     </row>
     <row r="99" spans="7:15" x14ac:dyDescent="0.2">
       <c r="G99" s="27" t="str">
-        <f>TEXT(SUM(H89:H99)/24+SUM(I89:I99)/1440+SUM(J89:J99)/86400,"[h]:m:s")</f>
-        <v>89:29:13</v>
+        <f>TEXT(SUM(H90:H99)/24+SUM(I90:I99)/1440+SUM(J90:J99)/86400,"[h]:m:s")</f>
+        <v>82:32:17</v>
       </c>
       <c r="H99" s="26">
         <v>16</v>
@@ -9946,7 +9946,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -10382,8 +10382,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10464,16 +10464,16 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="55">
         <v>63</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="55">
         <v>8</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="56">
         <v>3</v>
       </c>
     </row>
@@ -10506,16 +10506,16 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="61">
         <v>52</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="61">
         <v>53</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="62">
         <v>5</v>
       </c>
     </row>
@@ -10539,8 +10539,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10569,13 +10569,13 @@
       <c r="A2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="55">
         <v>34</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="55">
         <v>57</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="56">
         <v>1</v>
       </c>
     </row>
@@ -10583,13 +10583,13 @@
       <c r="A3" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="58">
         <v>60</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="58">
         <v>4</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="59">
         <v>1</v>
       </c>
     </row>
@@ -10597,13 +10597,13 @@
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="55">
         <v>67</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="55">
         <v>25</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="56">
         <v>2</v>
       </c>
     </row>
@@ -10611,13 +10611,13 @@
       <c r="A5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="58">
         <v>79</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="58">
         <v>22</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="59">
         <v>2</v>
       </c>
     </row>
@@ -10625,13 +10625,13 @@
       <c r="A6" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="55">
         <v>108</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="55">
         <v>28</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="56">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added notes for 08_JS_ES6_Plug:L05: JS Event Loop in Depth
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC7AAF2-DBAB-4850-B130-08D06DD6048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB503F0-90BB-4C40-A16F-AC49F7D118F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="4" activeTab="8" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="8" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -2176,7 +2176,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2244,9 +2244,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -3371,7 +3368,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="24" t="str">
+      <c r="A47" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：21:08:52</v>
       </c>
@@ -3409,12 +3406,12 @@
       <c r="D1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>389</v>
       </c>
     </row>
@@ -3452,7 +3449,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>392</v>
       </c>
     </row>
@@ -3512,7 +3509,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>398</v>
       </c>
     </row>
@@ -3649,7 +3646,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="32" t="s">
         <v>411</v>
       </c>
     </row>
@@ -3764,7 +3761,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="32" t="s">
         <v>422</v>
       </c>
     </row>
@@ -3857,7 +3854,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="32" t="s">
         <v>431</v>
       </c>
     </row>
@@ -3994,7 +3991,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="32" t="s">
         <v>444</v>
       </c>
     </row>
@@ -4109,7 +4106,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="33" t="s">
+      <c r="A69" s="32" t="s">
         <v>455</v>
       </c>
     </row>
@@ -4268,7 +4265,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="33" t="s">
+      <c r="A84" s="32" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4328,7 +4325,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="33" t="s">
+      <c r="A90" s="32" t="s">
         <v>476</v>
       </c>
     </row>
@@ -4443,7 +4440,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="33" t="s">
+      <c r="A101" s="32" t="s">
         <v>487</v>
       </c>
     </row>
@@ -4558,7 +4555,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="33" t="s">
+      <c r="A112" s="32" t="s">
         <v>498</v>
       </c>
     </row>
@@ -4574,7 +4571,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="35" t="str">
+      <c r="A114" s="34" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：79:03:38</v>
       </c>
@@ -4591,7 +4588,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4686,16 +4683,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4843,7 +4840,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="str">
+      <c r="A16" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：7:32:31</v>
       </c>
@@ -4875,16 +4872,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4966,7 +4963,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="str">
+      <c r="A10" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：3:02:48</v>
       </c>
@@ -4998,16 +4995,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5089,7 +5086,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="str">
+      <c r="A10" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：4:57:07</v>
       </c>
@@ -5121,16 +5118,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5223,7 +5220,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="str">
+      <c r="A11" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：7:34:27</v>
       </c>
@@ -5243,7 +5240,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5269,7 +5266,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>581</v>
       </c>
     </row>
@@ -5340,7 +5337,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>582</v>
       </c>
     </row>
@@ -5400,7 +5397,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="23" t="s">
         <v>583</v>
       </c>
     </row>
@@ -5460,7 +5457,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="38" t="str">
+      <c r="A21" s="37" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：8:07:22</v>
       </c>
@@ -5498,7 +5495,7 @@
       <c r="D1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>544</v>
       </c>
     </row>
@@ -5976,7 +5973,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="33" t="s">
         <v>543</v>
       </c>
       <c r="B45">
@@ -5987,7 +5984,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="36" t="str">
+      <c r="A46" s="35" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：28:01:05</v>
       </c>
@@ -6025,7 +6022,7 @@
       <c r="D1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>565</v>
       </c>
     </row>
@@ -6079,7 +6076,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>566</v>
       </c>
       <c r="B7">
@@ -6090,7 +6087,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>567</v>
       </c>
       <c r="B8">
@@ -6101,7 +6098,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>568</v>
       </c>
       <c r="B9">
@@ -6437,7 +6434,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>339</v>
       </c>
     </row>
@@ -6574,7 +6571,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>352</v>
       </c>
     </row>
@@ -6689,7 +6686,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="30" t="s">
         <v>363</v>
       </c>
     </row>
@@ -6749,7 +6746,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>369</v>
       </c>
     </row>
@@ -6787,7 +6784,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>373</v>
       </c>
     </row>
@@ -7871,7 +7868,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="24" t="str">
+      <c r="A89" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：48:45:42</v>
       </c>
@@ -7911,7 +7908,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>207</v>
       </c>
       <c r="B2">
@@ -7922,7 +7919,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>208</v>
       </c>
       <c r="B3">
@@ -7933,7 +7930,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>209</v>
       </c>
       <c r="B4">
@@ -7944,7 +7941,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>210</v>
       </c>
       <c r="B5">
@@ -7955,7 +7952,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>211</v>
       </c>
       <c r="B6">
@@ -7966,7 +7963,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>212</v>
       </c>
       <c r="B7">
@@ -7977,7 +7974,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>213</v>
       </c>
       <c r="B8">
@@ -7988,7 +7985,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="str">
+      <c r="A9" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：4:18:18</v>
       </c>
@@ -8028,7 +8025,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>286</v>
       </c>
       <c r="B2">
@@ -8039,7 +8036,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>287</v>
       </c>
       <c r="B3">
@@ -8050,7 +8047,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>288</v>
       </c>
       <c r="B4">
@@ -8061,7 +8058,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>289</v>
       </c>
       <c r="B5">
@@ -8072,7 +8069,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>290</v>
       </c>
       <c r="B6">
@@ -8083,7 +8080,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>291</v>
       </c>
       <c r="B7">
@@ -8094,7 +8091,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>292</v>
       </c>
       <c r="B8">
@@ -8105,7 +8102,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>293</v>
       </c>
       <c r="B9">
@@ -8116,7 +8113,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>294</v>
       </c>
       <c r="B10">
@@ -8127,7 +8124,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>295</v>
       </c>
       <c r="B11">
@@ -8138,7 +8135,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>296</v>
       </c>
       <c r="B12">
@@ -8149,7 +8146,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>297</v>
       </c>
       <c r="B13">
@@ -8160,7 +8157,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>298</v>
       </c>
       <c r="B14">
@@ -8171,7 +8168,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>299</v>
       </c>
       <c r="B15">
@@ -8182,7 +8179,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="24" t="s">
         <v>300</v>
       </c>
       <c r="B16">
@@ -8193,7 +8190,7 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="str">
+      <c r="A17" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：5:23:34</v>
       </c>
@@ -8235,15 +8232,15 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>214</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="29"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>172</v>
       </c>
       <c r="B3" s="20">
@@ -8252,18 +8249,18 @@
       <c r="C3" s="20">
         <v>32</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>163</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="29"/>
+      <c r="D4" s="28"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>173</v>
       </c>
       <c r="B5" s="20">
@@ -8272,18 +8269,18 @@
       <c r="C5" s="20">
         <v>51</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>215</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
-      <c r="D6" s="29"/>
+      <c r="D6" s="28"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>239</v>
       </c>
       <c r="B7" s="20">
@@ -8292,10 +8289,10 @@
       <c r="C7" s="20">
         <v>16</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>240</v>
       </c>
       <c r="B8" s="17">
@@ -8304,10 +8301,10 @@
       <c r="C8" s="17">
         <v>16</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="28"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>176</v>
       </c>
       <c r="B9" s="20">
@@ -8316,18 +8313,18 @@
       <c r="C9" s="20">
         <v>26</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>216</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
-      <c r="D10" s="29"/>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>241</v>
       </c>
       <c r="B11" s="20">
@@ -8336,10 +8333,10 @@
       <c r="C11" s="20">
         <v>4</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>242</v>
       </c>
       <c r="B12" s="17">
@@ -8348,10 +8345,10 @@
       <c r="C12" s="17">
         <v>20</v>
       </c>
-      <c r="D12" s="29"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>179</v>
       </c>
       <c r="B13" s="20">
@@ -8360,18 +8357,18 @@
       <c r="C13" s="20">
         <v>44</v>
       </c>
-      <c r="D13" s="30"/>
+      <c r="D13" s="29"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="39" t="s">
         <v>217</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="29"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>243</v>
       </c>
       <c r="B15" s="20">
@@ -8380,10 +8377,10 @@
       <c r="C15" s="20">
         <v>38</v>
       </c>
-      <c r="D15" s="30"/>
+      <c r="D15" s="29"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>244</v>
       </c>
       <c r="B16" s="17">
@@ -8392,18 +8389,18 @@
       <c r="C16" s="17">
         <v>34</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="28"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="38" t="s">
         <v>218</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
-      <c r="D17" s="30"/>
+      <c r="D17" s="29"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="40" t="s">
         <v>245</v>
       </c>
       <c r="B18" s="17">
@@ -8412,10 +8409,10 @@
       <c r="C18" s="17">
         <v>6</v>
       </c>
-      <c r="D18" s="29"/>
+      <c r="D18" s="28"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>246</v>
       </c>
       <c r="B19" s="20">
@@ -8424,18 +8421,18 @@
       <c r="C19" s="20">
         <v>32</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="29"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="39" t="s">
         <v>219</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
-      <c r="D20" s="29"/>
+      <c r="D20" s="28"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="42" t="s">
         <v>247</v>
       </c>
       <c r="B21" s="20">
@@ -8444,10 +8441,10 @@
       <c r="C21" s="20">
         <v>26</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" s="29"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="40" t="s">
         <v>185</v>
       </c>
       <c r="B22" s="17">
@@ -8456,10 +8453,10 @@
       <c r="C22" s="17">
         <v>15</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="28"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="42" t="s">
         <v>248</v>
       </c>
       <c r="B23" s="20">
@@ -8468,18 +8465,18 @@
       <c r="C23" s="20">
         <v>5</v>
       </c>
-      <c r="D23" s="30"/>
+      <c r="D23" s="29"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="40" t="s">
         <v>220</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
-      <c r="D24" s="29"/>
+      <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>249</v>
       </c>
       <c r="B25" s="20">
@@ -8488,18 +8485,18 @@
       <c r="C25" s="20">
         <v>21</v>
       </c>
-      <c r="D25" s="30"/>
+      <c r="D25" s="29"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="39" t="s">
         <v>221</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
-      <c r="D26" s="29"/>
+      <c r="D26" s="28"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="42" t="s">
         <v>250</v>
       </c>
       <c r="B27" s="20">
@@ -8508,10 +8505,10 @@
       <c r="C27" s="20">
         <v>51</v>
       </c>
-      <c r="D27" s="30"/>
+      <c r="D27" s="29"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="40" t="s">
         <v>251</v>
       </c>
       <c r="B28" s="17">
@@ -8520,10 +8517,10 @@
       <c r="C28" s="17">
         <v>38</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="42" t="s">
         <v>252</v>
       </c>
       <c r="B29" s="20">
@@ -8532,10 +8529,10 @@
       <c r="C29" s="20">
         <v>43</v>
       </c>
-      <c r="D29" s="30"/>
+      <c r="D29" s="29"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="40" t="s">
         <v>253</v>
       </c>
       <c r="B30" s="17">
@@ -8544,18 +8541,18 @@
       <c r="C30" s="17">
         <v>2</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="28"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="38" t="s">
         <v>222</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
-      <c r="D31" s="30"/>
+      <c r="D31" s="29"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="40" t="s">
         <v>254</v>
       </c>
       <c r="B32" s="17">
@@ -8564,10 +8561,10 @@
       <c r="C32" s="17">
         <v>21</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="28"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="42" t="s">
         <v>255</v>
       </c>
       <c r="B33" s="20">
@@ -8576,18 +8573,18 @@
       <c r="C33" s="20">
         <v>4</v>
       </c>
-      <c r="D33" s="30"/>
+      <c r="D33" s="29"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="39" t="s">
         <v>223</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
-      <c r="D34" s="29"/>
+      <c r="D34" s="28"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="42" t="s">
         <v>256</v>
       </c>
       <c r="B35" s="20">
@@ -8596,10 +8593,10 @@
       <c r="C35" s="20">
         <v>29</v>
       </c>
-      <c r="D35" s="30"/>
+      <c r="D35" s="29"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="40" t="s">
         <v>257</v>
       </c>
       <c r="B36" s="17">
@@ -8608,10 +8605,10 @@
       <c r="C36" s="17">
         <v>37</v>
       </c>
-      <c r="D36" s="29"/>
+      <c r="D36" s="28"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="42" t="s">
         <v>258</v>
       </c>
       <c r="B37" s="20">
@@ -8620,18 +8617,18 @@
       <c r="C37" s="20">
         <v>33</v>
       </c>
-      <c r="D37" s="30"/>
+      <c r="D37" s="29"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="39" t="s">
         <v>224</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
-      <c r="D38" s="29"/>
+      <c r="D38" s="28"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="42" t="s">
         <v>259</v>
       </c>
       <c r="B39" s="20">
@@ -8640,10 +8637,10 @@
       <c r="C39" s="20">
         <v>18</v>
       </c>
-      <c r="D39" s="30"/>
+      <c r="D39" s="29"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="40" t="s">
         <v>260</v>
       </c>
       <c r="B40" s="17">
@@ -8652,18 +8649,18 @@
       <c r="C40" s="17">
         <v>40</v>
       </c>
-      <c r="D40" s="29"/>
+      <c r="D40" s="28"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="38" t="s">
         <v>225</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
-      <c r="D41" s="30"/>
+      <c r="D41" s="29"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="40" t="s">
         <v>261</v>
       </c>
       <c r="B42" s="17">
@@ -8672,10 +8669,10 @@
       <c r="C42" s="17">
         <v>31</v>
       </c>
-      <c r="D42" s="29"/>
+      <c r="D42" s="28"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="42" t="s">
         <v>262</v>
       </c>
       <c r="B43" s="20">
@@ -8684,18 +8681,18 @@
       <c r="C43" s="20">
         <v>3</v>
       </c>
-      <c r="D43" s="30"/>
+      <c r="D43" s="29"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="39" t="s">
         <v>226</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
-      <c r="D44" s="29"/>
+      <c r="D44" s="28"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="42" t="s">
         <v>263</v>
       </c>
       <c r="B45" s="20">
@@ -8704,10 +8701,10 @@
       <c r="C45" s="20">
         <v>27</v>
       </c>
-      <c r="D45" s="30"/>
+      <c r="D45" s="29"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="40" t="s">
         <v>264</v>
       </c>
       <c r="B46" s="17">
@@ -8716,10 +8713,10 @@
       <c r="C46" s="17">
         <v>52</v>
       </c>
-      <c r="D46" s="29"/>
+      <c r="D46" s="28"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="42" t="s">
         <v>265</v>
       </c>
       <c r="B47" s="20">
@@ -8728,18 +8725,18 @@
       <c r="C47" s="20">
         <v>19</v>
       </c>
-      <c r="D47" s="30"/>
+      <c r="D47" s="29"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="40" t="s">
+      <c r="A48" s="39" t="s">
         <v>227</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
-      <c r="D48" s="29"/>
+      <c r="D48" s="28"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="42" t="s">
         <v>190</v>
       </c>
       <c r="B49" s="20">
@@ -8748,18 +8745,18 @@
       <c r="C49" s="20">
         <v>17</v>
       </c>
-      <c r="D49" s="30"/>
+      <c r="D49" s="29"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="40" t="s">
+      <c r="A50" s="39" t="s">
         <v>228</v>
       </c>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
-      <c r="D50" s="29"/>
+      <c r="D50" s="28"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="42" t="s">
         <v>266</v>
       </c>
       <c r="B51" s="20">
@@ -8768,10 +8765,10 @@
       <c r="C51" s="20">
         <v>51</v>
       </c>
-      <c r="D51" s="30"/>
+      <c r="D51" s="29"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="41" t="s">
+      <c r="A52" s="40" t="s">
         <v>267</v>
       </c>
       <c r="B52" s="17">
@@ -8780,18 +8777,18 @@
       <c r="C52" s="17">
         <v>3</v>
       </c>
-      <c r="D52" s="29"/>
+      <c r="D52" s="28"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="38" t="s">
         <v>229</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
-      <c r="D53" s="30"/>
+      <c r="D53" s="29"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="41" t="s">
+      <c r="A54" s="40" t="s">
         <v>268</v>
       </c>
       <c r="B54" s="17">
@@ -8800,10 +8797,10 @@
       <c r="C54" s="17">
         <v>31</v>
       </c>
-      <c r="D54" s="29"/>
+      <c r="D54" s="28"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="43" t="s">
+      <c r="A55" s="42" t="s">
         <v>269</v>
       </c>
       <c r="B55" s="20">
@@ -8812,18 +8809,18 @@
       <c r="C55" s="20">
         <v>46</v>
       </c>
-      <c r="D55" s="30"/>
+      <c r="D55" s="29"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="40" t="s">
+      <c r="A56" s="39" t="s">
         <v>230</v>
       </c>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
-      <c r="D56" s="29"/>
+      <c r="D56" s="28"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="43" t="s">
+      <c r="A57" s="42" t="s">
         <v>270</v>
       </c>
       <c r="B57" s="20">
@@ -8832,18 +8829,18 @@
       <c r="C57" s="20">
         <v>50</v>
       </c>
-      <c r="D57" s="30"/>
+      <c r="D57" s="29"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="40" t="s">
+      <c r="A58" s="39" t="s">
         <v>231</v>
       </c>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
-      <c r="D58" s="29"/>
+      <c r="D58" s="28"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="43" t="s">
+      <c r="A59" s="42" t="s">
         <v>271</v>
       </c>
       <c r="B59" s="20">
@@ -8852,10 +8849,10 @@
       <c r="C59" s="20">
         <v>38</v>
       </c>
-      <c r="D59" s="30"/>
+      <c r="D59" s="29"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="44" t="s">
+      <c r="A60" s="43" t="s">
         <v>272</v>
       </c>
       <c r="B60" s="17">
@@ -8864,10 +8861,10 @@
       <c r="C60" s="17">
         <v>48</v>
       </c>
-      <c r="D60" s="29"/>
+      <c r="D60" s="28"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="43" t="s">
+      <c r="A61" s="42" t="s">
         <v>273</v>
       </c>
       <c r="B61" s="20">
@@ -8876,18 +8873,18 @@
       <c r="C61" s="20">
         <v>31</v>
       </c>
-      <c r="D61" s="30"/>
+      <c r="D61" s="29"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="39" t="s">
         <v>232</v>
       </c>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
-      <c r="D62" s="29"/>
+      <c r="D62" s="28"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="42" t="s">
         <v>274</v>
       </c>
       <c r="B63" s="20">
@@ -8896,10 +8893,10 @@
       <c r="C63" s="20">
         <v>33</v>
       </c>
-      <c r="D63" s="30"/>
+      <c r="D63" s="29"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="40" t="s">
         <v>275</v>
       </c>
       <c r="B64" s="17">
@@ -8908,10 +8905,10 @@
       <c r="C64" s="17">
         <v>1</v>
       </c>
-      <c r="D64" s="29"/>
+      <c r="D64" s="28"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="42" t="s">
         <v>276</v>
       </c>
       <c r="B65" s="20">
@@ -8920,18 +8917,18 @@
       <c r="C65" s="20">
         <v>33</v>
       </c>
-      <c r="D65" s="30"/>
+      <c r="D65" s="29"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="40" t="s">
+      <c r="A66" s="39" t="s">
         <v>233</v>
       </c>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
-      <c r="D66" s="29"/>
+      <c r="D66" s="28"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="42" t="s">
         <v>277</v>
       </c>
       <c r="B67" s="20">
@@ -8940,10 +8937,10 @@
       <c r="C67" s="20">
         <v>3</v>
       </c>
-      <c r="D67" s="30"/>
+      <c r="D67" s="29"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="41" t="s">
+      <c r="A68" s="40" t="s">
         <v>278</v>
       </c>
       <c r="B68" s="17">
@@ -8952,18 +8949,18 @@
       <c r="C68" s="17">
         <v>9</v>
       </c>
-      <c r="D68" s="29"/>
+      <c r="D68" s="28"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="39" t="s">
+      <c r="A69" s="38" t="s">
         <v>234</v>
       </c>
       <c r="B69" s="20"/>
       <c r="C69" s="20"/>
-      <c r="D69" s="30"/>
+      <c r="D69" s="29"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="40" t="s">
         <v>279</v>
       </c>
       <c r="B70" s="17">
@@ -8972,10 +8969,10 @@
       <c r="C70" s="17">
         <v>36</v>
       </c>
-      <c r="D70" s="29"/>
+      <c r="D70" s="28"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="42" t="s">
         <v>280</v>
       </c>
       <c r="B71" s="20">
@@ -8984,18 +8981,18 @@
       <c r="C71" s="20">
         <v>12</v>
       </c>
-      <c r="D71" s="30"/>
+      <c r="D71" s="29"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="40" t="s">
+      <c r="A72" s="39" t="s">
         <v>235</v>
       </c>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
-      <c r="D72" s="29"/>
+      <c r="D72" s="28"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="43" t="s">
+      <c r="A73" s="42" t="s">
         <v>281</v>
       </c>
       <c r="B73" s="20">
@@ -9004,18 +9001,18 @@
       <c r="C73" s="20">
         <v>21</v>
       </c>
-      <c r="D73" s="30"/>
+      <c r="D73" s="29"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="40" t="s">
+      <c r="A74" s="39" t="s">
         <v>236</v>
       </c>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
-      <c r="D74" s="29"/>
+      <c r="D74" s="28"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="43" t="s">
+      <c r="A75" s="42" t="s">
         <v>282</v>
       </c>
       <c r="B75" s="20">
@@ -9024,10 +9021,10 @@
       <c r="C75" s="20">
         <v>24</v>
       </c>
-      <c r="D75" s="30"/>
+      <c r="D75" s="29"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="43" t="s">
+      <c r="A76" s="42" t="s">
         <v>283</v>
       </c>
       <c r="B76" s="20">
@@ -9036,18 +9033,18 @@
       <c r="C76" s="20">
         <v>56</v>
       </c>
-      <c r="D76" s="30"/>
+      <c r="D76" s="29"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="40" t="s">
+      <c r="A77" s="39" t="s">
         <v>237</v>
       </c>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
-      <c r="D77" s="29"/>
+      <c r="D77" s="28"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="43" t="s">
+      <c r="A78" s="42" t="s">
         <v>284</v>
       </c>
       <c r="B78" s="20">
@@ -9056,10 +9053,10 @@
       <c r="C78" s="20">
         <v>10</v>
       </c>
-      <c r="D78" s="30"/>
+      <c r="D78" s="29"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="40" t="s">
         <v>285</v>
       </c>
       <c r="B79" s="17">
@@ -9068,18 +9065,18 @@
       <c r="C79" s="17">
         <v>7</v>
       </c>
-      <c r="D79" s="29"/>
+      <c r="D79" s="28"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="39" t="s">
+      <c r="A80" s="38" t="s">
         <v>238</v>
       </c>
       <c r="B80" s="20"/>
       <c r="C80" s="20"/>
-      <c r="D80" s="30"/>
+      <c r="D80" s="29"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A81" s="41" t="s">
+      <c r="A81" s="40" t="s">
         <v>188</v>
       </c>
       <c r="B81" s="17">
@@ -9088,22 +9085,22 @@
       <c r="C81" s="17">
         <v>16</v>
       </c>
-      <c r="D81" s="29"/>
-      <c r="H81" s="26" t="s">
+      <c r="D81" s="28"/>
+      <c r="H81" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="I81" s="26" t="s">
+      <c r="I81" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="J81" s="26" t="s">
+      <c r="J81" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="K81" s="26" t="s">
+      <c r="K81" s="25" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A82" s="45" t="s">
+      <c r="A82" s="44" t="s">
         <v>189</v>
       </c>
       <c r="B82" s="7">
@@ -9112,267 +9109,267 @@
       <c r="C82" s="7">
         <v>34</v>
       </c>
-      <c r="D82" s="28"/>
-      <c r="H82" s="26">
+      <c r="D82" s="27"/>
+      <c r="H82" s="25">
         <v>21</v>
       </c>
-      <c r="I82" s="26">
+      <c r="I82" s="25">
         <v>8</v>
       </c>
-      <c r="J82" s="26">
+      <c r="J82" s="25">
         <v>52</v>
       </c>
-      <c r="K82" s="26">
+      <c r="K82" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A83" s="24" t="str">
+      <c r="A83" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：48:39:04</v>
       </c>
-      <c r="H83" s="26">
+      <c r="H83" s="25">
         <v>48</v>
       </c>
-      <c r="I83" s="26">
+      <c r="I83" s="25">
         <v>39</v>
       </c>
-      <c r="J83" s="26">
+      <c r="J83" s="25">
         <v>4</v>
       </c>
-      <c r="K83" s="26">
+      <c r="K83" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H84" s="26">
+      <c r="H84" s="25">
         <v>48</v>
       </c>
-      <c r="I84" s="26">
+      <c r="I84" s="25">
         <v>45</v>
       </c>
-      <c r="J84" s="26">
+      <c r="J84" s="25">
         <v>42</v>
       </c>
-      <c r="K84" s="26">
+      <c r="K84" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H85" s="26">
+      <c r="H85" s="25">
         <v>4</v>
       </c>
-      <c r="I85" s="26">
+      <c r="I85" s="25">
         <v>18</v>
       </c>
-      <c r="J85" s="26">
+      <c r="J85" s="25">
         <v>18</v>
       </c>
-      <c r="K85" s="26">
+      <c r="K85" s="25">
         <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H86" s="26">
+      <c r="H86" s="25">
         <v>5</v>
       </c>
-      <c r="I86" s="26">
+      <c r="I86" s="25">
         <v>23</v>
       </c>
-      <c r="J86" s="26">
+      <c r="J86" s="25">
         <v>34</v>
       </c>
-      <c r="K86" s="26">
+      <c r="K86" s="25">
         <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H87" s="26">
+      <c r="H87" s="25">
         <v>22</v>
       </c>
-      <c r="I87" s="26">
+      <c r="I87" s="25">
         <v>14</v>
       </c>
-      <c r="J87" s="26">
+      <c r="J87" s="25">
         <v>57</v>
       </c>
-      <c r="K87" s="26">
+      <c r="K87" s="25">
         <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H88" s="26">
+      <c r="H88" s="25">
         <v>17</v>
       </c>
-      <c r="I88" s="26">
+      <c r="I88" s="25">
         <v>4</v>
       </c>
-      <c r="J88" s="26">
+      <c r="J88" s="25">
         <v>17</v>
       </c>
-      <c r="K88" s="26">
+      <c r="K88" s="25">
         <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G89" s="27" t="str">
+      <c r="G89" s="26" t="str">
         <f>TEXT(SUM(H82:H89)/24+SUM(I82:I89)/1440+SUM(J82:J89)/86400,"[h]:m:s")</f>
         <v>174:31:40</v>
       </c>
-      <c r="H89" s="26">
+      <c r="H89" s="25">
         <v>6</v>
       </c>
-      <c r="I89" s="26">
+      <c r="I89" s="25">
         <v>56</v>
       </c>
-      <c r="J89" s="26">
+      <c r="J89" s="25">
         <v>56</v>
       </c>
-      <c r="K89" s="26">
+      <c r="K89" s="25">
         <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H90" s="26">
+      <c r="H90" s="25">
         <v>10</v>
       </c>
-      <c r="I90" s="26">
+      <c r="I90" s="25">
         <v>30</v>
       </c>
-      <c r="J90" s="26">
+      <c r="J90" s="25">
         <v>6</v>
       </c>
-      <c r="K90" s="26">
+      <c r="K90" s="25">
         <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="K91" s="26">
+      <c r="K91" s="25">
         <v>10</v>
       </c>
-      <c r="M91" s="26">
+      <c r="M91" s="25">
         <v>79</v>
       </c>
-      <c r="N91" s="26">
+      <c r="N91" s="25">
         <v>3</v>
       </c>
-      <c r="O91" s="26">
+      <c r="O91" s="25">
         <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H92" s="26">
+      <c r="H92" s="25">
         <v>4</v>
       </c>
-      <c r="I92" s="26">
+      <c r="I92" s="25">
         <v>23</v>
       </c>
-      <c r="J92" s="26">
+      <c r="J92" s="25">
         <v>29</v>
       </c>
-      <c r="K92" s="26">
+      <c r="K92" s="25">
         <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H93" s="26">
+      <c r="H93" s="25">
         <v>7</v>
       </c>
-      <c r="I93" s="26">
+      <c r="I93" s="25">
         <v>32</v>
       </c>
-      <c r="J93" s="26">
+      <c r="J93" s="25">
         <v>31</v>
       </c>
-      <c r="K93" s="26">
+      <c r="K93" s="25">
         <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H94" s="26">
+      <c r="H94" s="25">
         <v>3</v>
       </c>
-      <c r="I94" s="26">
+      <c r="I94" s="25">
         <v>2</v>
       </c>
-      <c r="J94" s="26">
+      <c r="J94" s="25">
         <v>48</v>
       </c>
-      <c r="K94" s="26">
+      <c r="K94" s="25">
         <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H95" s="26">
+      <c r="H95" s="25">
         <v>4</v>
       </c>
-      <c r="I95" s="26">
+      <c r="I95" s="25">
         <v>57</v>
       </c>
-      <c r="J95" s="26">
+      <c r="J95" s="25">
         <v>7</v>
       </c>
-      <c r="K95" s="26">
+      <c r="K95" s="25">
         <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H96" s="26">
+      <c r="H96" s="25">
         <v>7</v>
       </c>
-      <c r="I96" s="26">
+      <c r="I96" s="25">
         <v>34</v>
       </c>
-      <c r="J96" s="26">
+      <c r="J96" s="25">
         <v>27</v>
       </c>
-      <c r="K96" s="26">
+      <c r="K96" s="25">
         <v>15</v>
       </c>
     </row>
     <row r="97" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="K97" s="52">
+      <c r="K97" s="51">
         <v>16</v>
       </c>
-      <c r="M97" s="26">
+      <c r="M97" s="25">
         <v>8</v>
       </c>
-      <c r="N97" s="26">
+      <c r="N97" s="25">
         <v>7</v>
       </c>
-      <c r="O97" s="26">
+      <c r="O97" s="25">
         <v>22</v>
       </c>
     </row>
     <row r="98" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="H98" s="26">
+      <c r="H98" s="25">
         <v>28</v>
       </c>
-      <c r="I98" s="26">
+      <c r="I98" s="25">
         <v>1</v>
       </c>
-      <c r="J98" s="26">
+      <c r="J98" s="25">
         <v>5</v>
       </c>
-      <c r="K98" s="53">
+      <c r="K98" s="52">
         <v>17</v>
       </c>
     </row>
     <row r="99" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="G99" s="27" t="str">
+      <c r="G99" s="26" t="str">
         <f>TEXT(SUM(H90:H99)/24+SUM(I90:I99)/1440+SUM(J90:J99)/86400,"[h]:m:s")</f>
         <v>82:32:17</v>
       </c>
-      <c r="H99" s="26">
+      <c r="H99" s="25">
         <v>16</v>
       </c>
-      <c r="I99" s="26">
+      <c r="I99" s="25">
         <v>30</v>
       </c>
-      <c r="J99" s="26">
+      <c r="J99" s="25">
         <v>44</v>
       </c>
-      <c r="K99" s="53">
+      <c r="K99" s="52">
         <v>18</v>
       </c>
     </row>
@@ -9972,394 +9969,394 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="54">
         <v>3</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="54">
         <v>38</v>
       </c>
-      <c r="D2" s="56">
+      <c r="D2" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="57">
         <v>40</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="57">
         <v>47</v>
       </c>
-      <c r="D3" s="59">
+      <c r="D3" s="58">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4" s="54">
         <v>32</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="54">
         <v>41</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="55">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="57">
         <v>34</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="57">
         <v>35</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="58">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="54">
         <v>4</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="54">
         <v>0</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="55">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="57">
         <v>57</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="57">
         <v>37</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="58">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="55">
+      <c r="B8" s="54">
         <v>2</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="54">
         <v>9</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="55">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="58">
+      <c r="B9" s="57">
         <v>44</v>
       </c>
-      <c r="C9" s="58">
+      <c r="C9" s="57">
         <v>51</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="58">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="54">
         <v>3</v>
       </c>
-      <c r="C10" s="55">
+      <c r="C10" s="54">
         <v>29</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="55">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="57">
         <v>64</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="57">
         <v>5</v>
       </c>
-      <c r="D11" s="59">
+      <c r="D11" s="58">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="55">
+      <c r="B12" s="54">
         <v>2</v>
       </c>
-      <c r="C12" s="55">
+      <c r="C12" s="54">
         <v>16</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="55">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="58">
+      <c r="B13" s="57">
         <v>59</v>
       </c>
-      <c r="C13" s="58">
+      <c r="C13" s="57">
         <v>15</v>
       </c>
-      <c r="D13" s="59">
+      <c r="D13" s="58">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="55">
+      <c r="B14" s="54">
         <v>7</v>
       </c>
-      <c r="C14" s="55">
+      <c r="C14" s="54">
         <v>40</v>
       </c>
-      <c r="D14" s="56">
+      <c r="D14" s="55">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="58">
+      <c r="B15" s="57">
         <v>95</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="57">
         <v>44</v>
       </c>
-      <c r="D15" s="59">
+      <c r="D15" s="58">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="55">
+      <c r="B16" s="54">
         <v>15</v>
       </c>
-      <c r="C16" s="55">
+      <c r="C16" s="54">
         <v>23</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="55">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="58">
+      <c r="B17" s="57">
         <v>36</v>
       </c>
-      <c r="C17" s="58">
+      <c r="C17" s="57">
         <v>10</v>
       </c>
-      <c r="D17" s="59">
+      <c r="D17" s="58">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="55">
+      <c r="B18" s="54">
         <v>27</v>
       </c>
-      <c r="C18" s="55">
+      <c r="C18" s="54">
         <v>53</v>
       </c>
-      <c r="D18" s="56">
+      <c r="D18" s="55">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="58">
+      <c r="B19" s="57">
         <v>78</v>
       </c>
-      <c r="C19" s="58">
+      <c r="C19" s="57">
         <v>51</v>
       </c>
-      <c r="D19" s="59">
+      <c r="D19" s="58">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="55">
+      <c r="B20" s="54">
         <v>18</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="54">
         <v>50</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="55">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="58">
+      <c r="B21" s="57">
         <v>53</v>
       </c>
-      <c r="C21" s="58">
+      <c r="C21" s="57">
         <v>2</v>
       </c>
-      <c r="D21" s="59">
+      <c r="D21" s="58">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="55">
+      <c r="B22" s="54">
         <v>15</v>
       </c>
-      <c r="C22" s="55">
+      <c r="C22" s="54">
         <v>43</v>
       </c>
-      <c r="D22" s="56">
+      <c r="D22" s="55">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="58">
+      <c r="B23" s="57">
         <v>52</v>
       </c>
-      <c r="C23" s="58">
+      <c r="C23" s="57">
         <v>38</v>
       </c>
-      <c r="D23" s="59">
+      <c r="D23" s="58">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="55">
+      <c r="B24" s="54">
         <v>9</v>
       </c>
-      <c r="C24" s="55">
+      <c r="C24" s="54">
         <v>48</v>
       </c>
-      <c r="D24" s="56">
+      <c r="D24" s="55">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="58">
+      <c r="B25" s="57">
         <v>76</v>
       </c>
-      <c r="C25" s="58">
+      <c r="C25" s="57">
         <v>39</v>
       </c>
-      <c r="D25" s="59">
+      <c r="D25" s="58">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="55">
+      <c r="B26" s="54">
         <v>36</v>
       </c>
-      <c r="C26" s="55">
+      <c r="C26" s="54">
         <v>18</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D26" s="55">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="58">
+      <c r="B27" s="57">
         <v>51</v>
       </c>
-      <c r="C27" s="58">
+      <c r="C27" s="57">
         <v>58</v>
       </c>
-      <c r="D27" s="59">
+      <c r="D27" s="58">
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="55">
+      <c r="B28" s="54">
         <v>22</v>
       </c>
-      <c r="C28" s="55">
+      <c r="C28" s="54">
         <v>56</v>
       </c>
-      <c r="D28" s="56">
+      <c r="D28" s="55">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="61">
+      <c r="B29" s="60">
         <v>75</v>
       </c>
-      <c r="C29" s="61">
+      <c r="C29" s="60">
         <v>21</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="61">
         <v>14</v>
       </c>
     </row>
@@ -10408,114 +10405,114 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="54">
         <v>58</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="54">
         <v>14</v>
       </c>
-      <c r="D2" s="56">
+      <c r="D2" s="55">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="57">
         <v>56</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="57">
         <v>1</v>
       </c>
-      <c r="D3" s="59">
+      <c r="D3" s="58">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4" s="54">
         <v>67</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="54">
         <v>55</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="55">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="57">
         <v>49</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="57">
         <v>2</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="58">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="54">
         <v>63</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="54">
         <v>8</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="55">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="57">
         <v>30</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="57">
         <v>54</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="58">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="55">
+      <c r="B8" s="54">
         <v>38</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="54">
         <v>49</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="55">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="61">
+      <c r="B9" s="60">
         <v>52</v>
       </c>
-      <c r="C9" s="61">
+      <c r="C9" s="60">
         <v>53</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="61">
         <v>5</v>
       </c>
     </row>
@@ -10540,7 +10537,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10569,13 +10566,13 @@
       <c r="A2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="54">
         <v>34</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="54">
         <v>57</v>
       </c>
-      <c r="D2" s="56">
+      <c r="D2" s="55">
         <v>1</v>
       </c>
     </row>
@@ -10583,13 +10580,13 @@
       <c r="A3" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="57">
         <v>60</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="57">
         <v>4</v>
       </c>
-      <c r="D3" s="59">
+      <c r="D3" s="58">
         <v>1</v>
       </c>
     </row>
@@ -10597,13 +10594,13 @@
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4" s="54">
         <v>67</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="54">
         <v>25</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="55">
         <v>2</v>
       </c>
     </row>
@@ -10611,13 +10608,13 @@
       <c r="A5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="57">
         <v>79</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="57">
         <v>22</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="58">
         <v>2</v>
       </c>
     </row>
@@ -10625,13 +10622,13 @@
       <c r="A6" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="54">
         <v>108</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="54">
         <v>28</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="55">
         <v>3</v>
       </c>
     </row>
@@ -10639,13 +10636,13 @@
       <c r="A7" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="57">
         <v>71</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="57">
         <v>22</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="58">
         <v>4</v>
       </c>
     </row>
@@ -10653,13 +10650,13 @@
       <c r="A8" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="54">
         <v>63</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="54">
         <v>25</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="55">
         <v>5</v>
       </c>
     </row>
@@ -10667,13 +10664,13 @@
       <c r="A9" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="57">
         <v>45</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="57">
         <v>56</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="58">
         <v>6</v>
       </c>
     </row>
@@ -10681,13 +10678,13 @@
       <c r="A10" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="54">
         <v>38</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="54">
         <v>7</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="55">
         <v>6</v>
       </c>
     </row>
@@ -10695,13 +10692,13 @@
       <c r="A11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="60">
         <v>61</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="60">
         <v>0</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="61">
         <v>7</v>
       </c>
     </row>
@@ -10714,5 +10711,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added notes for 09_Programming_thoughts:L01: Scrolling lyrics
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB503F0-90BB-4C40-A16F-AC49F7D118F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14988FE-4B84-4CD0-96F5-173C4A327A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="8" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="10" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -4587,8 +4587,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10536,7 +10536,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added notes for 09_Programming_thoughts:L03: Customized Cascading Addr Dropdown Menu
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14988FE-4B84-4CD0-96F5-173C4A327A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA30EEE0-F7D4-46A9-B398-2E43C05D9E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="10" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="14" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -2370,7 +2370,35 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b/>
+        <family val="3"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="3"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="3"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="3"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -2538,52 +2566,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}" name="表1" displayName="表1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}" name="表1" displayName="表1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A1:D14" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{17F2527D-78B5-4B06-A96C-9154CE44E0C2}" name="Title"/>
     <tableColumn id="2" xr3:uid="{EE3C824F-40FF-4F88-B4B9-C5214BACA1F1}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{230A3F53-7EAB-4152-BC42-0BA62C77BB5C}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{F7B7FE7E-C186-4BD5-89FC-F90A3311F416}" name="Day"/>
+    <tableColumn id="4" xr3:uid="{F7B7FE7E-C186-4BD5-89FC-F90A3311F416}" name="Day" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A1:D8" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{56E13753-3D18-4640-894E-A9862A8519E9}" name="Title"/>
     <tableColumn id="2" xr3:uid="{79D6C646-1226-4C28-B1C9-44701A88F7AD}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{D0893D73-54C6-4CE8-BA7E-4CA7DAFD42BB}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day"/>
+    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A1:D8" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{12D9D257-0720-4D69-92DB-DAB28C2BA457}" name="Title"/>
     <tableColumn id="2" xr3:uid="{16E320F3-22A7-423A-B471-F02438A5F8A6}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{64AD87D5-100E-459C-BDDA-2972741296A6}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day"/>
+    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:D9" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A51B88B7-4A2F-4D5C-A477-AFA8072799E1}" name="Title"/>
     <tableColumn id="2" xr3:uid="{4A08D9E2-7055-4737-913C-04F2C5ED46F0}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{0EDD753B-5FBA-424C-9B63-06AEEA8E4D71}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{35807557-36BB-4B11-8AC2-863BC91B2108}" name="Day"/>
+    <tableColumn id="4" xr3:uid="{35807557-36BB-4B11-8AC2-863BC91B2108}" name="Day" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4587,7 +4615,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -4672,7 +4700,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4706,6 +4734,9 @@
       <c r="C2">
         <v>40</v>
       </c>
+      <c r="D2" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -4717,6 +4748,9 @@
       <c r="C3">
         <v>35</v>
       </c>
+      <c r="D3" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -4728,6 +4762,9 @@
       <c r="C4">
         <v>56</v>
       </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4739,6 +4776,9 @@
       <c r="C5">
         <v>46</v>
       </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -4750,6 +4790,9 @@
       <c r="C6">
         <v>56</v>
       </c>
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4761,6 +4804,9 @@
       <c r="C7">
         <v>24</v>
       </c>
+      <c r="D7" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -4772,6 +4818,9 @@
       <c r="C8">
         <v>21</v>
       </c>
+      <c r="D8" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -4783,6 +4832,9 @@
       <c r="C9">
         <v>39</v>
       </c>
+      <c r="D9" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -4794,6 +4846,9 @@
       <c r="C10">
         <v>0</v>
       </c>
+      <c r="D10" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -4805,6 +4860,9 @@
       <c r="C11">
         <v>4</v>
       </c>
+      <c r="D11" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -4816,6 +4874,9 @@
       <c r="C12">
         <v>3</v>
       </c>
+      <c r="D12" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -4827,6 +4888,9 @@
       <c r="C13">
         <v>16</v>
       </c>
+      <c r="D13" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -4838,12 +4902,18 @@
       <c r="C14">
         <v>51</v>
       </c>
+      <c r="D14" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="str">
+      <c r="A16" s="1" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：7:32:31</v>
       </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4860,7 +4930,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4895,6 +4965,9 @@
       <c r="C2">
         <v>20</v>
       </c>
+      <c r="D2" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -4906,6 +4979,9 @@
       <c r="C3">
         <v>8</v>
       </c>
+      <c r="D3" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -4917,6 +4993,9 @@
       <c r="C4">
         <v>39</v>
       </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4928,6 +5007,9 @@
       <c r="C5">
         <v>13</v>
       </c>
+      <c r="D5" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -4939,6 +5021,9 @@
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4950,6 +5035,9 @@
       <c r="C7">
         <v>7</v>
       </c>
+      <c r="D7" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -4960,6 +5048,9 @@
       </c>
       <c r="C8">
         <v>19</v>
+      </c>
+      <c r="D8" s="25">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4983,7 +5074,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D7" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5018,6 +5109,9 @@
       <c r="C2">
         <v>31</v>
       </c>
+      <c r="D2" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -5029,6 +5123,9 @@
       <c r="C3">
         <v>25</v>
       </c>
+      <c r="D3" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -5040,6 +5137,9 @@
       <c r="C4">
         <v>6</v>
       </c>
+      <c r="D4" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -5051,6 +5151,9 @@
       <c r="C5">
         <v>29</v>
       </c>
+      <c r="D5" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -5062,6 +5165,9 @@
       <c r="C6">
         <v>28</v>
       </c>
+      <c r="D6" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -5073,6 +5179,9 @@
       <c r="C7">
         <v>3</v>
       </c>
+      <c r="D7" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -5083,6 +5192,9 @@
       </c>
       <c r="C8">
         <v>5</v>
+      </c>
+      <c r="D8" s="25">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5105,8 +5217,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5141,6 +5253,9 @@
       <c r="C2">
         <v>26</v>
       </c>
+      <c r="D2" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -5152,6 +5267,9 @@
       <c r="C3">
         <v>59</v>
       </c>
+      <c r="D3" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -5163,6 +5281,9 @@
       <c r="C4">
         <v>18</v>
       </c>
+      <c r="D4" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -5174,6 +5295,9 @@
       <c r="C5">
         <v>3</v>
       </c>
+      <c r="D5" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -5185,6 +5309,9 @@
       <c r="C6">
         <v>47</v>
       </c>
+      <c r="D6" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -5196,6 +5323,9 @@
       <c r="C7">
         <v>12</v>
       </c>
+      <c r="D7" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -5207,6 +5337,9 @@
       <c r="C8">
         <v>57</v>
       </c>
+      <c r="D8" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -5217,6 +5350,9 @@
       </c>
       <c r="C9">
         <v>45</v>
+      </c>
+      <c r="D9" s="25">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added notes for 11_Networks:L01: Network introduction
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA30EEE0-F7D4-46A9-B398-2E43C05D9E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DED760A-F6DD-449F-9D27-E94D01C674FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="14" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="11" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -2176,7 +2176,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2366,6 +2366,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2379,17 +2382,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <family val="3"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <family val="3"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2440,6 +2469,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <family val="3"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -2480,43 +2516,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
+        <family val="3"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2572,40 +2575,40 @@
     <tableColumn id="1" xr3:uid="{17F2527D-78B5-4B06-A96C-9154CE44E0C2}" name="Title"/>
     <tableColumn id="2" xr3:uid="{EE3C824F-40FF-4F88-B4B9-C5214BACA1F1}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{230A3F53-7EAB-4152-BC42-0BA62C77BB5C}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{F7B7FE7E-C186-4BD5-89FC-F90A3311F416}" name="Day" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F7B7FE7E-C186-4BD5-89FC-F90A3311F416}" name="Day" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:D8" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{56E13753-3D18-4640-894E-A9862A8519E9}" name="Title"/>
     <tableColumn id="2" xr3:uid="{79D6C646-1226-4C28-B1C9-44701A88F7AD}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{D0893D73-54C6-4CE8-BA7E-4CA7DAFD42BB}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A1:D8" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{12D9D257-0720-4D69-92DB-DAB28C2BA457}" name="Title"/>
     <tableColumn id="2" xr3:uid="{16E320F3-22A7-423A-B471-F02438A5F8A6}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{64AD87D5-100E-459C-BDDA-2972741296A6}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:D9" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A51B88B7-4A2F-4D5C-A477-AFA8072799E1}" name="Title"/>
@@ -3412,8 +3415,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4699,8 +4702,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4725,16 +4728,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="63" t="s">
         <v>304</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="63">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="63">
         <v>40</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="51">
         <v>1</v>
       </c>
     </row>
@@ -5217,7 +5220,7 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added notes for 11_Networks:L08: Browser loading process
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DED760A-F6DD-449F-9D27-E94D01C674FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B9956F-4509-4B12-918F-63F74C4DD7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="11" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -995,22 +995,6 @@
     <t>06. 基本概念-http-part2</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">07. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF262626"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>关于 Apifox 的使用</t>
-    </r>
-  </si>
-  <si>
     <t>08. 浏览器页面处理流程</t>
   </si>
   <si>
@@ -1896,13 +1880,16 @@
   <si>
     <t>Ch</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07. 关于 Apifox 的使用</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1956,14 +1943,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF262626"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -2267,10 +2246,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2285,7 +2264,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="22"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2300,7 +2279,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2336,37 +2315,37 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3438,12 +3417,12 @@
         <v>53</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3459,7 +3438,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B4">
         <v>81</v>
@@ -3470,7 +3449,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -3481,12 +3460,12 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -3497,7 +3476,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B8">
         <v>65</v>
@@ -3508,7 +3487,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B9">
         <v>52</v>
@@ -3519,7 +3498,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B10">
         <v>85</v>
@@ -3530,7 +3509,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B11">
         <v>69</v>
@@ -3541,12 +3520,12 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B13">
         <v>37</v>
@@ -3557,7 +3536,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B14">
         <v>58</v>
@@ -3568,7 +3547,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -3579,7 +3558,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B16">
         <v>45</v>
@@ -3590,7 +3569,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B17">
         <v>45</v>
@@ -3601,7 +3580,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B18">
         <v>54</v>
@@ -3612,7 +3591,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -3623,7 +3602,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B20">
         <v>7</v>
@@ -3634,7 +3613,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B21">
         <v>31</v>
@@ -3645,7 +3624,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B22">
         <v>73</v>
@@ -3656,7 +3635,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B23">
         <v>52</v>
@@ -3667,7 +3646,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B24">
         <v>18</v>
@@ -3678,12 +3657,12 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B26">
         <v>19</v>
@@ -3694,7 +3673,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B27">
         <v>42</v>
@@ -3705,7 +3684,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B28">
         <v>36</v>
@@ -3716,7 +3695,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B29">
         <v>7</v>
@@ -3727,7 +3706,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B30">
         <v>50</v>
@@ -3738,7 +3717,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B31">
         <v>43</v>
@@ -3749,7 +3728,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B32">
         <v>40</v>
@@ -3760,7 +3739,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B33">
         <v>96</v>
@@ -3771,7 +3750,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B34">
         <v>23</v>
@@ -3782,7 +3761,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B35">
         <v>69</v>
@@ -3793,12 +3772,12 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B37">
         <v>74</v>
@@ -3809,7 +3788,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B38">
         <v>60</v>
@@ -3820,7 +3799,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B39">
         <v>41</v>
@@ -3831,7 +3810,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B40">
         <v>61</v>
@@ -3842,7 +3821,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B41">
         <v>38</v>
@@ -3853,7 +3832,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B42">
         <v>57</v>
@@ -3864,7 +3843,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B43">
         <v>37</v>
@@ -3875,7 +3854,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B44">
         <v>63</v>
@@ -3886,12 +3865,12 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B46">
         <v>68</v>
@@ -3902,7 +3881,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B47">
         <v>60</v>
@@ -3913,7 +3892,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3924,7 +3903,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B49">
         <v>77</v>
@@ -3935,7 +3914,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B50">
         <v>39</v>
@@ -3946,7 +3925,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B51">
         <v>12</v>
@@ -3957,7 +3936,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B52">
         <v>59</v>
@@ -3968,7 +3947,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B53">
         <v>37</v>
@@ -3979,7 +3958,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B54">
         <v>60</v>
@@ -3990,7 +3969,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B55">
         <v>66</v>
@@ -4001,7 +3980,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B56">
         <v>60</v>
@@ -4012,7 +3991,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B57">
         <v>59</v>
@@ -4023,12 +4002,12 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="32" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B59">
         <v>39</v>
@@ -4039,7 +4018,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B60">
         <v>67</v>
@@ -4050,7 +4029,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B61">
         <v>16</v>
@@ -4061,7 +4040,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B62">
         <v>54</v>
@@ -4072,7 +4051,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B63">
         <v>49</v>
@@ -4083,7 +4062,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B64">
         <v>55</v>
@@ -4094,7 +4073,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B65">
         <v>45</v>
@@ -4105,7 +4084,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B66">
         <v>20</v>
@@ -4116,7 +4095,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B67">
         <v>58</v>
@@ -4127,7 +4106,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B68">
         <v>33</v>
@@ -4138,12 +4117,12 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="32" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B70">
         <v>22</v>
@@ -4154,7 +4133,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B71">
         <v>36</v>
@@ -4165,7 +4144,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B72">
         <v>53</v>
@@ -4176,7 +4155,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B73">
         <v>35</v>
@@ -4187,7 +4166,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B74">
         <v>61</v>
@@ -4198,7 +4177,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B75">
         <v>79</v>
@@ -4209,7 +4188,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B76">
         <v>20</v>
@@ -4220,7 +4199,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B77">
         <v>21</v>
@@ -4231,7 +4210,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B78">
         <v>35</v>
@@ -4242,7 +4221,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B79">
         <v>51</v>
@@ -4253,7 +4232,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B80">
         <v>45</v>
@@ -4264,7 +4243,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B81">
         <v>14</v>
@@ -4275,7 +4254,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B82">
         <v>60</v>
@@ -4286,7 +4265,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B83">
         <v>49</v>
@@ -4297,12 +4276,12 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="32" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B85">
         <v>36</v>
@@ -4313,7 +4292,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B86">
         <v>21</v>
@@ -4324,7 +4303,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B87">
         <v>105</v>
@@ -4335,7 +4314,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B88">
         <v>41</v>
@@ -4346,7 +4325,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B89">
         <v>62</v>
@@ -4357,12 +4336,12 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="32" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B91">
         <v>69</v>
@@ -4373,7 +4352,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B92">
         <v>69</v>
@@ -4384,7 +4363,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B93">
         <v>62</v>
@@ -4395,7 +4374,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B94">
         <v>76</v>
@@ -4406,7 +4385,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B95">
         <v>64</v>
@@ -4417,7 +4396,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B96">
         <v>42</v>
@@ -4428,7 +4407,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B97">
         <v>44</v>
@@ -4439,7 +4418,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B98">
         <v>39</v>
@@ -4450,7 +4429,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B99">
         <v>31</v>
@@ -4461,7 +4440,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B100">
         <v>21</v>
@@ -4472,12 +4451,12 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="32" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B102">
         <v>67</v>
@@ -4488,7 +4467,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B103">
         <v>51</v>
@@ -4499,7 +4478,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B104">
         <v>29</v>
@@ -4510,7 +4489,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B105">
         <v>30</v>
@@ -4521,7 +4500,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B106">
         <v>44</v>
@@ -4532,7 +4511,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B107">
         <v>60</v>
@@ -4543,7 +4522,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B108">
         <v>55</v>
@@ -4554,7 +4533,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B109">
         <v>63</v>
@@ -4565,7 +4544,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B110">
         <v>60</v>
@@ -4576,7 +4555,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B111">
         <v>87</v>
@@ -4587,12 +4566,12 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="32" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B113">
         <v>11</v>
@@ -4703,7 +4682,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4742,120 +4721,120 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="63" t="s">
         <v>305</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="63">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="63">
         <v>35</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="63" t="s">
         <v>306</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="63">
         <v>39</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="63">
         <v>56</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="63" t="s">
         <v>307</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="63">
         <v>25</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="63">
         <v>46</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="63" t="s">
         <v>308</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="63">
         <v>41</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="63">
         <v>56</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="63" t="s">
         <v>309</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="63">
         <v>39</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="63">
         <v>24</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="63" t="s">
+        <v>600</v>
+      </c>
+      <c r="B8" s="63">
+        <v>18</v>
+      </c>
+      <c r="C8" s="63">
+        <v>21</v>
+      </c>
+      <c r="D8" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="63" t="s">
         <v>310</v>
       </c>
-      <c r="B8">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>21</v>
-      </c>
-      <c r="D8" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" s="63">
+        <v>41</v>
+      </c>
+      <c r="C9" s="63">
+        <v>39</v>
+      </c>
+      <c r="D9" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="B9">
-        <v>41</v>
-      </c>
-      <c r="C9">
-        <v>39</v>
-      </c>
-      <c r="D9" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>312</v>
-      </c>
-      <c r="B10">
+      <c r="B10" s="63">
         <v>54</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="63">
         <v>0</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B11">
         <v>41</v>
@@ -4869,7 +4848,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B12">
         <v>55</v>
@@ -4883,7 +4862,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B13">
         <v>49</v>
@@ -4897,7 +4876,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B14">
         <v>24</v>
@@ -4921,8 +4900,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4933,7 +4913,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4960,7 +4940,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B2">
         <v>72</v>
@@ -4974,7 +4954,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B3">
         <v>41</v>
@@ -4988,7 +4968,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -5002,7 +4982,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -5016,7 +4996,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -5030,7 +5010,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -5044,7 +5024,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B8">
         <v>16</v>
@@ -5104,7 +5084,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B2">
         <v>82</v>
@@ -5118,7 +5098,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -5132,7 +5112,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4">
         <v>18</v>
@@ -5146,7 +5126,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5">
         <v>38</v>
@@ -5160,7 +5140,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6">
         <v>43</v>
@@ -5174,7 +5154,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7">
         <v>69</v>
@@ -5188,7 +5168,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8">
         <v>37</v>
@@ -5248,7 +5228,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B2">
         <v>54</v>
@@ -5262,7 +5242,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B3">
         <v>67</v>
@@ -5276,7 +5256,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B4">
         <v>41</v>
@@ -5290,7 +5270,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B5">
         <v>48</v>
@@ -5304,7 +5284,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B6">
         <v>23</v>
@@ -5318,7 +5298,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -5332,7 +5312,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B8">
         <v>91</v>
@@ -5346,7 +5326,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B9">
         <v>110</v>
@@ -5406,12 +5386,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B3">
         <v>30</v>
@@ -5422,7 +5402,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -5433,7 +5413,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B5">
         <v>55</v>
@@ -5444,7 +5424,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5455,7 +5435,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B7">
         <v>55</v>
@@ -5466,7 +5446,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B8">
         <v>58</v>
@@ -5477,12 +5457,12 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B10">
         <v>24</v>
@@ -5493,7 +5473,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B11">
         <v>29</v>
@@ -5504,7 +5484,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B12">
         <v>17</v>
@@ -5515,7 +5495,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -5526,7 +5506,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B14">
         <v>24</v>
@@ -5537,12 +5517,12 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B16">
         <v>41</v>
@@ -5553,7 +5533,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B17">
         <v>20</v>
@@ -5564,7 +5544,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B18">
         <v>46</v>
@@ -5575,7 +5555,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B19">
         <v>25</v>
@@ -5586,7 +5566,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -5635,12 +5615,12 @@
         <v>53</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B2">
         <v>23</v>
@@ -5651,7 +5631,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B3">
         <v>22</v>
@@ -5662,7 +5642,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B4">
         <v>48</v>
@@ -5673,7 +5653,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -5684,7 +5664,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -5695,7 +5675,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B7">
         <v>47</v>
@@ -5706,7 +5686,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B8">
         <v>38</v>
@@ -5717,7 +5697,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B9">
         <v>84</v>
@@ -5728,7 +5708,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B10">
         <v>17</v>
@@ -5739,7 +5719,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B11">
         <v>112</v>
@@ -5750,7 +5730,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B12">
         <v>33</v>
@@ -5761,7 +5741,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B13">
         <v>54</v>
@@ -5772,7 +5752,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B14">
         <v>71</v>
@@ -5783,7 +5763,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B15">
         <v>57</v>
@@ -5794,7 +5774,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B16">
         <v>34</v>
@@ -5805,7 +5785,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B17">
         <v>44</v>
@@ -5816,7 +5796,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B18">
         <v>41</v>
@@ -5827,7 +5807,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B19">
         <v>34</v>
@@ -5838,7 +5818,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B20">
         <v>41</v>
@@ -5849,7 +5829,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -5860,7 +5840,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B22">
         <v>27</v>
@@ -5871,7 +5851,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B23">
         <v>26</v>
@@ -5882,7 +5862,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B24">
         <v>94</v>
@@ -5893,7 +5873,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -5904,7 +5884,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B26">
         <v>39</v>
@@ -5915,7 +5895,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B27">
         <v>43</v>
@@ -5926,7 +5906,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B28">
         <v>48</v>
@@ -5937,7 +5917,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -5948,7 +5928,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B30">
         <v>40</v>
@@ -5959,7 +5939,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B31">
         <v>37</v>
@@ -5970,7 +5950,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B32">
         <v>10</v>
@@ -5981,7 +5961,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B33">
         <v>39</v>
@@ -5992,7 +5972,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B34">
         <v>46</v>
@@ -6003,7 +5983,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B35">
         <v>98</v>
@@ -6014,7 +5994,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B36">
         <v>23</v>
@@ -6025,7 +6005,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B37">
         <v>14</v>
@@ -6036,7 +6016,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B38">
         <v>12</v>
@@ -6047,7 +6027,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B39">
         <v>17</v>
@@ -6058,7 +6038,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B40">
         <v>14</v>
@@ -6069,7 +6049,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B41">
         <v>55</v>
@@ -6080,7 +6060,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B42">
         <v>23</v>
@@ -6091,7 +6071,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B43">
         <v>6</v>
@@ -6102,7 +6082,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B44">
         <v>5</v>
@@ -6113,7 +6093,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B45">
         <v>32</v>
@@ -6162,12 +6142,12 @@
         <v>53</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B2">
         <v>19</v>
@@ -6178,7 +6158,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -6189,7 +6169,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -6200,7 +6180,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -6211,12 +6191,12 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B7">
         <v>15</v>
@@ -6227,7 +6207,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B8">
         <v>58</v>
@@ -6238,7 +6218,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B9">
         <v>17</v>
@@ -6249,7 +6229,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B10">
         <v>62</v>
@@ -6260,7 +6240,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B11">
         <v>46</v>
@@ -6271,7 +6251,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B12">
         <v>58</v>
@@ -6282,7 +6262,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B13">
         <v>40</v>
@@ -6293,7 +6273,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B14">
         <v>57</v>
@@ -6304,7 +6284,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B15">
         <v>78</v>
@@ -6315,7 +6295,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B16">
         <v>43</v>
@@ -6326,7 +6306,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B17">
         <v>79</v>
@@ -6337,7 +6317,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B18">
         <v>15</v>
@@ -6348,7 +6328,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B19">
         <v>75</v>
@@ -6359,7 +6339,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B20">
         <v>14</v>
@@ -6370,7 +6350,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B21">
         <v>35</v>
@@ -6381,12 +6361,12 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -6397,7 +6377,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B24">
         <v>17</v>
@@ -6408,7 +6388,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -6419,7 +6399,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B26">
         <v>13</v>
@@ -6430,7 +6410,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B27">
         <v>23</v>
@@ -6441,7 +6421,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -6452,7 +6432,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B29">
         <v>18</v>
@@ -6463,7 +6443,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -6474,7 +6454,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -6485,7 +6465,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B32">
         <v>22</v>
@@ -6496,7 +6476,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -6507,12 +6487,12 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B35">
         <v>23</v>
@@ -6523,7 +6503,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B36">
         <v>26</v>
@@ -6574,12 +6554,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -6590,7 +6570,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B4">
         <v>44</v>
@@ -6601,7 +6581,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B5">
         <v>27</v>
@@ -6612,7 +6592,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B6">
         <v>46</v>
@@ -6623,7 +6603,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B7">
         <v>61</v>
@@ -6634,7 +6614,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B8">
         <v>47</v>
@@ -6645,7 +6625,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B9">
         <v>55</v>
@@ -6656,7 +6636,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -6667,7 +6647,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B11">
         <v>24</v>
@@ -6678,7 +6658,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B12">
         <v>45</v>
@@ -6689,7 +6669,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B13">
         <v>59</v>
@@ -6700,7 +6680,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -6711,12 +6691,12 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B16">
         <v>59</v>
@@ -6727,7 +6707,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B17">
         <v>50</v>
@@ -6738,7 +6718,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -6749,7 +6729,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B19">
         <v>52</v>
@@ -6760,7 +6740,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -6771,7 +6751,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B21">
         <v>49</v>
@@ -6782,7 +6762,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B22">
         <v>55</v>
@@ -6793,7 +6773,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B23">
         <v>69</v>
@@ -6804,7 +6784,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B24">
         <v>64</v>
@@ -6815,7 +6795,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B25">
         <v>17</v>
@@ -6826,12 +6806,12 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -6842,7 +6822,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B28">
         <v>30</v>
@@ -6853,7 +6833,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B29">
         <v>41</v>
@@ -6864,7 +6844,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B30">
         <v>36</v>
@@ -6875,7 +6855,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B31">
         <v>65</v>
@@ -6886,12 +6866,12 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B33">
         <v>25</v>
@@ -6902,7 +6882,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B34">
         <v>41</v>
@@ -6913,7 +6893,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B35">
         <v>11</v>
@@ -6924,12 +6904,12 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B37">
         <v>47</v>
@@ -6940,7 +6920,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B38">
         <v>34</v>
@@ -6951,7 +6931,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -6962,7 +6942,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B40">
         <v>46</v>
@@ -6973,7 +6953,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B41">
         <v>25</v>
@@ -6984,7 +6964,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B42">
         <v>9</v>
@@ -6995,7 +6975,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B43">
         <v>49</v>
@@ -7006,7 +6986,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B44">
         <v>21</v>
@@ -7017,7 +6997,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B45">
         <v>9</v>
@@ -7028,7 +7008,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B46">
         <v>10</v>
@@ -7039,7 +7019,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B47">
         <v>25</v>
@@ -7050,7 +7030,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B48">
         <v>48</v>
@@ -7061,7 +7041,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B49">
         <v>23</v>
@@ -7072,7 +7052,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B50">
         <v>25</v>
@@ -9235,7 +9215,7 @@
         <v>303</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added notes for 11_Networks:L11: Chatbot project: register & login page
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B9956F-4509-4B12-918F-63F74C4DD7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A45FDD6-7486-4056-A0C7-95CDDE31AD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="990" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="11" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3315" yWindow="690" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="13" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -4681,8 +4681,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4833,58 +4833,58 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="63" t="s">
         <v>312</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="63">
         <v>41</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="63">
         <v>4</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="51">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="63" t="s">
         <v>313</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="63">
         <v>55</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="63">
         <v>3</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="51">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="63" t="s">
         <v>314</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="63">
         <v>49</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="63">
         <v>16</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="51">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="63" t="s">
         <v>315</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="63">
         <v>24</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="63">
         <v>51</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="51">
         <v>4</v>
       </c>
     </row>
@@ -4913,7 +4913,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5056,8 +5056,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added notes for 13_Third_library:L01: jQuery introduction
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A45FDD6-7486-4056-A0C7-95CDDE31AD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F317E4-2427-4206-9592-02E607041064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="690" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="13" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -2352,53 +2352,78 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="19">
     <dxf>
       <font>
-        <b/>
-        <family val="3"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="0"/>
+        <color rgb="FFFF0000"/>
         <name val="等线"/>
-        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2495,6 +2520,46 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <family val="3"/>
@@ -2548,52 +2613,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}" name="表1" displayName="表1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}" name="表1" displayName="表1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A1:D14" xr:uid="{C70CFAA9-A0E5-4E03-9547-5F59A01E3F79}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{17F2527D-78B5-4B06-A96C-9154CE44E0C2}" name="Title"/>
     <tableColumn id="2" xr3:uid="{EE3C824F-40FF-4F88-B4B9-C5214BACA1F1}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{230A3F53-7EAB-4152-BC42-0BA62C77BB5C}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{F7B7FE7E-C186-4BD5-89FC-F90A3311F416}" name="Day" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{F7B7FE7E-C186-4BD5-89FC-F90A3311F416}" name="Day" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="0" headerRowBorderDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A1:D8" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{56E13753-3D18-4640-894E-A9862A8519E9}" name="Title"/>
-    <tableColumn id="2" xr3:uid="{79D6C646-1226-4C28-B1C9-44701A88F7AD}" name="Minutes"/>
-    <tableColumn id="3" xr3:uid="{D0893D73-54C6-4CE8-BA7E-4CA7DAFD42BB}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{56E13753-3D18-4640-894E-A9862A8519E9}" name="Title" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{79D6C646-1226-4C28-B1C9-44701A88F7AD}" name="Minutes" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{D0893D73-54C6-4CE8-BA7E-4CA7DAFD42BB}" name="Seconds" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A1:D8" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{12D9D257-0720-4D69-92DB-DAB28C2BA457}" name="Title"/>
     <tableColumn id="2" xr3:uid="{16E320F3-22A7-423A-B471-F02438A5F8A6}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{64AD87D5-100E-459C-BDDA-2972741296A6}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A1:D9" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A51B88B7-4A2F-4D5C-A477-AFA8072799E1}" name="Title"/>
     <tableColumn id="2" xr3:uid="{4A08D9E2-7055-4737-913C-04F2C5ED46F0}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{0EDD753B-5FBA-424C-9B63-06AEEA8E4D71}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{35807557-36BB-4B11-8AC2-863BC91B2108}" name="Day" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{35807557-36BB-4B11-8AC2-863BC91B2108}" name="Day" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4913,7 +4978,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4939,100 +5004,100 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="63" t="s">
         <v>316</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="63">
         <v>72</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="63">
         <v>20</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="63" t="s">
         <v>317</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="63">
         <v>41</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="63">
         <v>8</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="63" t="s">
         <v>318</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="63">
         <v>24</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="63">
         <v>39</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="63" t="s">
         <v>319</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="63">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="63">
         <v>13</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="63" t="s">
         <v>320</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="63">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="63">
         <v>2</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="63" t="s">
         <v>321</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="63">
         <v>16</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="63">
         <v>7</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="63" t="s">
         <v>322</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="63">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="63">
         <v>19</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="51">
         <v>2</v>
       </c>
     </row>
@@ -5057,7 +5122,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5083,58 +5148,58 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="63" t="s">
         <v>323</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="63">
         <v>82</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="63">
         <v>31</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="63" t="s">
         <v>324</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="63">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="63">
         <v>25</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="63" t="s">
         <v>325</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="63">
         <v>18</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="63">
         <v>6</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="63" t="s">
         <v>326</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="63">
         <v>38</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="63">
         <v>29</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="51">
         <v>2</v>
       </c>
     </row>
@@ -5201,7 +5266,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D9" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added notes for 13_Third_library:L04: Axios introduction
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F317E4-2427-4206-9592-02E607041064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECE6AC7-923D-4E0A-A7D8-C38FA608074B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="690" windowWidth="19200" windowHeight="13140" tabRatio="768" firstSheet="8" activeTab="13" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3315" yWindow="690" windowWidth="19200" windowHeight="13140" tabRatio="722" firstSheet="10" activeTab="13" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -2155,7 +2155,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2348,83 +2348,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="32"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2520,11 +2451,83 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2626,39 +2629,39 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="0" headerRowBorderDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}" name="表2" displayName="表2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A1:D8" xr:uid="{B03604A7-54BB-40E4-A753-F066A9EE57CD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{56E13753-3D18-4640-894E-A9862A8519E9}" name="Title" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{79D6C646-1226-4C28-B1C9-44701A88F7AD}" name="Minutes" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{D0893D73-54C6-4CE8-BA7E-4CA7DAFD42BB}" name="Seconds" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{56E13753-3D18-4640-894E-A9862A8519E9}" name="Title" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{79D6C646-1226-4C28-B1C9-44701A88F7AD}" name="Minutes" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{D0893D73-54C6-4CE8-BA7E-4CA7DAFD42BB}" name="Seconds" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{359B13F2-EBE0-4293-9CC1-460C29E0A781}" name="Day" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}" name="表3" displayName="表3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A1:D8" xr:uid="{86FD78AE-DBFC-4D13-9AEB-87ABB2BA44ED}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{12D9D257-0720-4D69-92DB-DAB28C2BA457}" name="Title"/>
     <tableColumn id="2" xr3:uid="{16E320F3-22A7-423A-B471-F02438A5F8A6}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{64AD87D5-100E-459C-BDDA-2972741296A6}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{B0B5AFC3-8899-495B-B393-B698A292457B}" name="Day" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}" name="表4" displayName="表4" ref="A1:D9" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:D9" xr:uid="{3A07BEBD-9576-4B15-B502-7AC05840FF62}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A51B88B7-4A2F-4D5C-A477-AFA8072799E1}" name="Title"/>
     <tableColumn id="2" xr3:uid="{4A08D9E2-7055-4737-913C-04F2C5ED46F0}" name="Minutes"/>
     <tableColumn id="3" xr3:uid="{0EDD753B-5FBA-424C-9B63-06AEEA8E4D71}" name="Seconds"/>
-    <tableColumn id="4" xr3:uid="{35807557-36BB-4B11-8AC2-863BC91B2108}" name="Day" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{35807557-36BB-4B11-8AC2-863BC91B2108}" name="Day" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5122,7 +5125,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5204,44 +5207,44 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="63" t="s">
         <v>327</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="63">
         <v>43</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="63">
         <v>28</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="63" t="s">
         <v>328</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="63">
         <v>69</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="63">
         <v>3</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="51">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="63" t="s">
         <v>329</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="63">
         <v>37</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="63">
         <v>5</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="51">
         <v>3</v>
       </c>
     </row>
@@ -5266,7 +5269,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D2:D9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5404,7 +5407,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="str">
+      <c r="A11" s="64" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：7:34:27</v>
       </c>

</xml_diff>

<commit_message>
added notes for 13_Third_library:L06: Moment.js
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECE6AC7-923D-4E0A-A7D8-C38FA608074B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4762AC02-1D22-43D4-A58F-818C0D132CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="690" windowWidth="19200" windowHeight="13140" tabRatio="722" firstSheet="10" activeTab="13" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3315" yWindow="690" windowWidth="19200" windowHeight="13140" tabRatio="722" firstSheet="13" activeTab="19" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="17Vue_intro" sheetId="15" r:id="rId17"/>
     <sheet name="18Vue_comp" sheetId="16" r:id="rId18"/>
     <sheet name="19Miniapp" sheetId="17" r:id="rId19"/>
+    <sheet name="20Echarts" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="653">
   <si>
     <t>1. 环境准备</t>
   </si>
@@ -1883,6 +1884,162 @@
   </si>
   <si>
     <t>07. 关于 Apifox 的使用</t>
+  </si>
+  <si>
+    <t>01-echarts介绍</t>
+  </si>
+  <si>
+    <t>02-第一个Ecarts例子</t>
+  </si>
+  <si>
+    <t>03-title组件</t>
+  </si>
+  <si>
+    <t>04-legend组件1</t>
+  </si>
+  <si>
+    <t>05-legend组件2</t>
+  </si>
+  <si>
+    <t>06-网格</t>
+  </si>
+  <si>
+    <t>07-坐标轴1</t>
+  </si>
+  <si>
+    <t>08-坐标轴2</t>
+  </si>
+  <si>
+    <t>09-极坐标系</t>
+  </si>
+  <si>
+    <t>10-雷达坐标系</t>
+  </si>
+  <si>
+    <t>11-区域缩放1</t>
+  </si>
+  <si>
+    <t>12-区域缩放2</t>
+  </si>
+  <si>
+    <t>13-视觉映射组件-1</t>
+  </si>
+  <si>
+    <t>14-视觉映射组件-2</t>
+  </si>
+  <si>
+    <t>15-视觉映射组件-3</t>
+  </si>
+  <si>
+    <t>16-提示框组件</t>
+  </si>
+  <si>
+    <t>17-坐标轴指示器组件</t>
+  </si>
+  <si>
+    <t>18-工具栏</t>
+  </si>
+  <si>
+    <t>19-区域选择1</t>
+  </si>
+  <si>
+    <t>20-区域选择2</t>
+  </si>
+  <si>
+    <t>21-地理坐标系1</t>
+  </si>
+  <si>
+    <t>22-地理坐标系2</t>
+  </si>
+  <si>
+    <t>23-平行坐标系</t>
+  </si>
+  <si>
+    <t>24-单轴</t>
+  </si>
+  <si>
+    <t>25-时间轴</t>
+  </si>
+  <si>
+    <t>26-图形元素1</t>
+  </si>
+  <si>
+    <t>27-图形元素2</t>
+  </si>
+  <si>
+    <t>28-日历坐标系</t>
+  </si>
+  <si>
+    <t>29-数据集1-存储</t>
+  </si>
+  <si>
+    <t>30-数据集2-映射</t>
+  </si>
+  <si>
+    <t>31-折线图</t>
+  </si>
+  <si>
+    <t>32-柱状图</t>
+  </si>
+  <si>
+    <t>33-饼图</t>
+  </si>
+  <si>
+    <t>34-气泡图</t>
+  </si>
+  <si>
+    <t>35-涟漪气泡图</t>
+  </si>
+  <si>
+    <t>36-雷达图</t>
+  </si>
+  <si>
+    <t>37-树图</t>
+  </si>
+  <si>
+    <t>38-矩形树图1</t>
+  </si>
+  <si>
+    <t>39-矩形树图2</t>
+  </si>
+  <si>
+    <t>40-旭日图</t>
+  </si>
+  <si>
+    <t>41-盒须图</t>
+  </si>
+  <si>
+    <t>42-K线图</t>
+  </si>
+  <si>
+    <t>43-热力图</t>
+  </si>
+  <si>
+    <t>44-平行坐标图</t>
+  </si>
+  <si>
+    <t>45-线图</t>
+  </si>
+  <si>
+    <t>46-关系图</t>
+  </si>
+  <si>
+    <t>47-桑基图</t>
+  </si>
+  <si>
+    <t>48-漏斗图</t>
+  </si>
+  <si>
+    <t>49-仪表盘</t>
+  </si>
+  <si>
+    <t>50-象形柱图</t>
+  </si>
+  <si>
+    <t>51-河流图</t>
+  </si>
+  <si>
+    <t>52-课程总结</t>
   </si>
 </sst>
 </file>
@@ -2155,7 +2312,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2350,6 +2507,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="32"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="16"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5124,7 +5284,7 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -6597,8 +6757,8 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8058,6 +8218,616 @@
       <c r="A89" s="23" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：48:45:42</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E8140B-BC28-463F-83D4-E613D48B68A9}">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>601</v>
+      </c>
+      <c r="B2">
+        <v>46</v>
+      </c>
+      <c r="C2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>602</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>603</v>
+      </c>
+      <c r="B4">
+        <v>46</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>604</v>
+      </c>
+      <c r="B5">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>605</v>
+      </c>
+      <c r="B6">
+        <v>71</v>
+      </c>
+      <c r="C6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>606</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>607</v>
+      </c>
+      <c r="B8">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>608</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>609</v>
+      </c>
+      <c r="B10">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>610</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>611</v>
+      </c>
+      <c r="B12">
+        <v>62</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>612</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>613</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>614</v>
+      </c>
+      <c r="B15">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>615</v>
+      </c>
+      <c r="B16">
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>616</v>
+      </c>
+      <c r="B17">
+        <v>73</v>
+      </c>
+      <c r="C17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>617</v>
+      </c>
+      <c r="B18">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>618</v>
+      </c>
+      <c r="B19">
+        <v>62</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>619</v>
+      </c>
+      <c r="B20">
+        <v>55</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>620</v>
+      </c>
+      <c r="B21">
+        <v>29</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>621</v>
+      </c>
+      <c r="B22">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>622</v>
+      </c>
+      <c r="B23">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>623</v>
+      </c>
+      <c r="B24">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>624</v>
+      </c>
+      <c r="B25">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>625</v>
+      </c>
+      <c r="B26">
+        <v>60</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>626</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+      <c r="C27">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>627</v>
+      </c>
+      <c r="B28">
+        <v>49</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>628</v>
+      </c>
+      <c r="B29">
+        <v>51</v>
+      </c>
+      <c r="C29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>629</v>
+      </c>
+      <c r="B30">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>630</v>
+      </c>
+      <c r="B31">
+        <v>24</v>
+      </c>
+      <c r="C31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>631</v>
+      </c>
+      <c r="B32">
+        <v>83</v>
+      </c>
+      <c r="C32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>632</v>
+      </c>
+      <c r="B33">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>633</v>
+      </c>
+      <c r="B34">
+        <v>44</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>634</v>
+      </c>
+      <c r="B35">
+        <v>77</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>635</v>
+      </c>
+      <c r="B36">
+        <v>57</v>
+      </c>
+      <c r="C36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>636</v>
+      </c>
+      <c r="B37">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>637</v>
+      </c>
+      <c r="B38">
+        <v>40</v>
+      </c>
+      <c r="C38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>638</v>
+      </c>
+      <c r="B39">
+        <v>63</v>
+      </c>
+      <c r="C39">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>639</v>
+      </c>
+      <c r="B40">
+        <v>66</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>640</v>
+      </c>
+      <c r="B41">
+        <v>51</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>641</v>
+      </c>
+      <c r="B42">
+        <v>47</v>
+      </c>
+      <c r="C42">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>642</v>
+      </c>
+      <c r="B43">
+        <v>78</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>643</v>
+      </c>
+      <c r="B44">
+        <v>41</v>
+      </c>
+      <c r="C44">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>644</v>
+      </c>
+      <c r="B45">
+        <v>64</v>
+      </c>
+      <c r="C45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>645</v>
+      </c>
+      <c r="B46">
+        <v>79</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>646</v>
+      </c>
+      <c r="B47">
+        <v>93</v>
+      </c>
+      <c r="C47">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>647</v>
+      </c>
+      <c r="B48">
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>648</v>
+      </c>
+      <c r="B49">
+        <v>42</v>
+      </c>
+      <c r="C49">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>649</v>
+      </c>
+      <c r="B50">
+        <v>68</v>
+      </c>
+      <c r="C50">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>650</v>
+      </c>
+      <c r="B51">
+        <v>75</v>
+      </c>
+      <c r="C51">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>651</v>
+      </c>
+      <c r="B52">
+        <v>25</v>
+      </c>
+      <c r="C52">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>652</v>
+      </c>
+      <c r="B53">
+        <v>9</v>
+      </c>
+      <c r="C53">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="65" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：42:01:10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated notes for 14_fe_engineering:L01: CommonJS module system
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4762AC02-1D22-43D4-A58F-818C0D132CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2E80E2-0982-47BE-8A7D-8F44B7DA1D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="690" windowWidth="19200" windowHeight="13140" tabRatio="722" firstSheet="13" activeTab="19" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13140" tabRatio="722" firstSheet="13" activeTab="14" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -5428,8 +5428,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5455,30 +5455,30 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="63" t="s">
         <v>330</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="63">
         <v>54</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="63">
         <v>26</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="51">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="63" t="s">
         <v>331</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="63">
         <v>67</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="63">
         <v>59</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="51">
         <v>1</v>
       </c>
     </row>
@@ -8230,7 +8230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E8140B-BC28-463F-83D4-E613D48B68A9}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
added notes for 14_fe_engineering:L04: Less
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2E80E2-0982-47BE-8A7D-8F44B7DA1D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AB2C09-073E-46FA-8E7B-812BF6424BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13140" tabRatio="722" firstSheet="13" activeTab="14" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -5429,7 +5429,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5483,58 +5483,58 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="63" t="s">
         <v>332</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="63">
         <v>41</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="63">
         <v>18</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="63" t="s">
         <v>333</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="63">
         <v>48</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="63">
         <v>3</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="63" t="s">
         <v>334</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="63">
         <v>23</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="63">
         <v>47</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="51">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="63" t="s">
         <v>335</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="63">
         <v>16</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="63">
         <v>12</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="51">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added notes for 14_fe_engineering:L05: build tools intruduction
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AB2C09-073E-46FA-8E7B-812BF6424BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3BA088-F4DF-4484-A4A4-E0DCB8B22844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13140" tabRatio="722" firstSheet="13" activeTab="14" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -5429,7 +5429,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5539,16 +5539,16 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="63" t="s">
         <v>336</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="63">
         <v>91</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="63">
         <v>57</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="51">
         <v>3</v>
       </c>
     </row>
@@ -5575,8 +5575,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added notes for 14_fe_engineering:L06: integrated proj: movie-list
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3BA088-F4DF-4484-A4A4-E0DCB8B22844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9B8CD1-491E-400F-B582-BAB04735742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13140" tabRatio="722" firstSheet="13" activeTab="14" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -5429,7 +5429,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5553,16 +5553,16 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="63" t="s">
         <v>337</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="63">
         <v>110</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="63">
         <v>45</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="51">
         <v>4</v>
       </c>
     </row>
@@ -5588,7 +5588,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added notes for 14_Vue_intro:L01: background for the front-end frameworks
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9B8CD1-491E-400F-B582-BAB04735742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83459D1-3363-4E00-8614-2EE0D55DBE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13140" tabRatio="722" firstSheet="13" activeTab="14" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13440" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="18Vue_comp" sheetId="16" r:id="rId18"/>
     <sheet name="19Miniapp" sheetId="17" r:id="rId19"/>
     <sheet name="20Echarts" sheetId="20" r:id="rId20"/>
+    <sheet name="21Webpack" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="720">
   <si>
     <t>1. 环境准备</t>
   </si>
@@ -2040,6 +2041,209 @@
   </si>
   <si>
     <t>52-课程总结</t>
+  </si>
+  <si>
+    <t>1.Webpack核心功能</t>
+  </si>
+  <si>
+    <t>1-1. 如何在浏览器端实现模块化</t>
+  </si>
+  <si>
+    <t>1-2. webpack的安装和使用</t>
+  </si>
+  <si>
+    <t>1-3. 模块化兼容性</t>
+  </si>
+  <si>
+    <t>1-4. [练习]酷炫的数字查找特效</t>
+  </si>
+  <si>
+    <t>1-5. 编译结果分析</t>
+  </si>
+  <si>
+    <t>1-6. 配置文件</t>
+  </si>
+  <si>
+    <t>1-7. devtool配置</t>
+  </si>
+  <si>
+    <t>1-8. 编译过程</t>
+  </si>
+  <si>
+    <t>1-9. 入口和出口</t>
+  </si>
+  <si>
+    <t>1-10. 入口和出口的最佳实践</t>
+  </si>
+  <si>
+    <t>1-11. loader</t>
+  </si>
+  <si>
+    <t>1-12. [练习]处理样式</t>
+  </si>
+  <si>
+    <t>1-13. [练习]处理图片</t>
+  </si>
+  <si>
+    <t>1-14. plugin</t>
+  </si>
+  <si>
+    <t>1-15. [练习]添加文件列表</t>
+  </si>
+  <si>
+    <t>1-16. 区分环境</t>
+  </si>
+  <si>
+    <t>1-17. 其他细节配置</t>
+  </si>
+  <si>
+    <t>2.常用扩展</t>
+  </si>
+  <si>
+    <t>2-1. 清除输出目录</t>
+  </si>
+  <si>
+    <t>2-2. 自动生成页面</t>
+  </si>
+  <si>
+    <t>2-3. 复制静态资源</t>
+  </si>
+  <si>
+    <t>2-4. 开发服务器</t>
+  </si>
+  <si>
+    <t>2-5. 普通文件处理</t>
+  </si>
+  <si>
+    <t>2-6. 解决路径问题</t>
+  </si>
+  <si>
+    <t>2-7. webpack内置插件</t>
+  </si>
+  <si>
+    <t>2-8. [练习]区域查询</t>
+  </si>
+  <si>
+    <t>3. CSS工程化</t>
+  </si>
+  <si>
+    <t>3-1. css工程化概述</t>
+  </si>
+  <si>
+    <t>3-2. 利用webpack拆分css</t>
+  </si>
+  <si>
+    <t>3-3. BEM</t>
+  </si>
+  <si>
+    <t>3-4. css-in-js</t>
+  </si>
+  <si>
+    <t>3-5. css module</t>
+  </si>
+  <si>
+    <t>3-6. 预编译器less</t>
+  </si>
+  <si>
+    <t>3-7. 在webpack中使用less</t>
+  </si>
+  <si>
+    <t>3-8. PostCss</t>
+  </si>
+  <si>
+    <t>3-9.在webpack中使用postcss</t>
+  </si>
+  <si>
+    <t>3-10.抽离css文件</t>
+  </si>
+  <si>
+    <t>4. js兼容性</t>
+  </si>
+  <si>
+    <t>4-1. babel的安装和使用</t>
+  </si>
+  <si>
+    <t>4-2. babel预设</t>
+  </si>
+  <si>
+    <t>4-3. babel插件</t>
+  </si>
+  <si>
+    <t>4-4. 在webpack中使用babel</t>
+  </si>
+  <si>
+    <t>4-5. [扩展]对类的转换</t>
+  </si>
+  <si>
+    <t>4-6. [扩展]async和await的转换</t>
+  </si>
+  <si>
+    <t>5. 性能优化</t>
+  </si>
+  <si>
+    <t>5-1. 性能优化概述</t>
+  </si>
+  <si>
+    <t>5-2. 减少模块解析</t>
+  </si>
+  <si>
+    <t>5-3. 优化loader性能</t>
+  </si>
+  <si>
+    <t>5-4. 热替换</t>
+  </si>
+  <si>
+    <t>5-5. 手动分包</t>
+  </si>
+  <si>
+    <t>5-6. 自动分包</t>
+  </si>
+  <si>
+    <t>5-7. 代码压缩</t>
+  </si>
+  <si>
+    <t>5-8. tree shaking</t>
+  </si>
+  <si>
+    <t>5-9. 懒加载</t>
+  </si>
+  <si>
+    <t>5-10. ESLint</t>
+  </si>
+  <si>
+    <t>5-11. bundle analyzer</t>
+  </si>
+  <si>
+    <t>5-12. gzip</t>
+  </si>
+  <si>
+    <t>6. 补充和案例</t>
+  </si>
+  <si>
+    <t>6-1. [扩展]不确定的动态依赖</t>
+  </si>
+  <si>
+    <t>6-2. 搭建多页应用</t>
+  </si>
+  <si>
+    <t>6-3. [扩展]搭建vue单页应用</t>
+  </si>
+  <si>
+    <t>6-4. [扩展]搭建React单页应用</t>
+  </si>
+  <si>
+    <t>6-5. [扩展]搭建Node应用</t>
+  </si>
+  <si>
+    <t>6-6. 搭建全栈应用</t>
+  </si>
+  <si>
+    <t>1-5-1. 学习可以很轻松</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>webpack-课程前导</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2312,7 +2516,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2510,6 +2714,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="16"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5428,7 +5635,7 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -5588,7 +5795,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5821,8 +6028,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5857,6 +6064,9 @@
       <c r="C2">
         <v>57</v>
       </c>
+      <c r="D2" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -5868,6 +6078,9 @@
       <c r="C3">
         <v>5</v>
       </c>
+      <c r="D3" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -5879,6 +6092,9 @@
       <c r="C4">
         <v>15</v>
       </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -5890,6 +6106,9 @@
       <c r="C5">
         <v>9</v>
       </c>
+      <c r="D5" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -5901,6 +6120,9 @@
       <c r="C6">
         <v>46</v>
       </c>
+      <c r="D6" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -5912,6 +6134,9 @@
       <c r="C7">
         <v>50</v>
       </c>
+      <c r="D7" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -5923,6 +6148,9 @@
       <c r="C8">
         <v>26</v>
       </c>
+      <c r="D8" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -5934,6 +6162,9 @@
       <c r="C9">
         <v>18</v>
       </c>
+      <c r="D9" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -5945,6 +6176,9 @@
       <c r="C10">
         <v>25</v>
       </c>
+      <c r="D10" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5956,6 +6190,9 @@
       <c r="C11">
         <v>57</v>
       </c>
+      <c r="D11" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -5967,6 +6204,9 @@
       <c r="C12">
         <v>49</v>
       </c>
+      <c r="D12" s="25">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -5978,6 +6218,9 @@
       <c r="C13">
         <v>9</v>
       </c>
+      <c r="D13" s="25">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -5989,6 +6232,9 @@
       <c r="C14">
         <v>2</v>
       </c>
+      <c r="D14" s="25">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -6000,6 +6246,9 @@
       <c r="C15">
         <v>59</v>
       </c>
+      <c r="D15" s="25">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -6011,8 +6260,11 @@
       <c r="C16">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>514</v>
       </c>
@@ -6022,8 +6274,11 @@
       <c r="C17">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>515</v>
       </c>
@@ -6033,8 +6288,11 @@
       <c r="C18">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>516</v>
       </c>
@@ -6044,8 +6302,11 @@
       <c r="C19">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>517</v>
       </c>
@@ -6055,8 +6316,11 @@
       <c r="C20">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>518</v>
       </c>
@@ -6066,8 +6330,11 @@
       <c r="C21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>519</v>
       </c>
@@ -6077,8 +6344,9 @@
       <c r="C22">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="25"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>520</v>
       </c>
@@ -6088,8 +6356,9 @@
       <c r="C23">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>521</v>
       </c>
@@ -6099,8 +6368,9 @@
       <c r="C24">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>522</v>
       </c>
@@ -6110,8 +6380,9 @@
       <c r="C25">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>523</v>
       </c>
@@ -6121,8 +6392,9 @@
       <c r="C26">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="25"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>524</v>
       </c>
@@ -6132,8 +6404,9 @@
       <c r="C27">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" s="25"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>525</v>
       </c>
@@ -6143,8 +6416,9 @@
       <c r="C28">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>526</v>
       </c>
@@ -6154,8 +6428,9 @@
       <c r="C29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>527</v>
       </c>
@@ -6165,8 +6440,9 @@
       <c r="C30">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>528</v>
       </c>
@@ -6176,8 +6452,9 @@
       <c r="C31">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>529</v>
       </c>
@@ -6187,8 +6464,9 @@
       <c r="C32">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="25"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>530</v>
       </c>
@@ -6198,8 +6476,9 @@
       <c r="C33">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>531</v>
       </c>
@@ -6209,8 +6488,9 @@
       <c r="C34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="25"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>532</v>
       </c>
@@ -6220,8 +6500,9 @@
       <c r="C35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" s="25"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>533</v>
       </c>
@@ -6231,8 +6512,9 @@
       <c r="C36">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="25"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>534</v>
       </c>
@@ -6242,8 +6524,9 @@
       <c r="C37">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="25"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>535</v>
       </c>
@@ -6253,8 +6536,9 @@
       <c r="C38">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="25"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>536</v>
       </c>
@@ -6264,8 +6548,9 @@
       <c r="C39">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" s="25"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>537</v>
       </c>
@@ -6275,8 +6560,9 @@
       <c r="C40">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" s="25"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>538</v>
       </c>
@@ -6286,8 +6572,9 @@
       <c r="C41">
         <v>43</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" s="25"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>539</v>
       </c>
@@ -6297,8 +6584,9 @@
       <c r="C42">
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" s="25"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>540</v>
       </c>
@@ -6308,8 +6596,9 @@
       <c r="C43">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" s="25"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>541</v>
       </c>
@@ -6319,8 +6608,9 @@
       <c r="C44">
         <v>27</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" s="25"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
         <v>542</v>
       </c>
@@ -6330,8 +6620,9 @@
       <c r="C45">
         <v>30</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" s="25"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：28:01:05</v>
@@ -6348,8 +6639,8 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8231,7 +8522,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E8140B-BC28-463F-83D4-E613D48B68A9}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8829,6 +9122,747 @@
       <c r="A54" s="65" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：42:01:10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97C62C-B5D1-4E72-812F-7EA03DA117C7}">
+  <dimension ref="A1:D69"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="66" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>719</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>655</v>
+      </c>
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>656</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>657</v>
+      </c>
+      <c r="B7">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>658</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>718</v>
+      </c>
+      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>659</v>
+      </c>
+      <c r="B10">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>660</v>
+      </c>
+      <c r="B11">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>661</v>
+      </c>
+      <c r="B12">
+        <v>51</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>662</v>
+      </c>
+      <c r="B13">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>663</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>664</v>
+      </c>
+      <c r="B15">
+        <v>44</v>
+      </c>
+      <c r="C15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>665</v>
+      </c>
+      <c r="B16">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>666</v>
+      </c>
+      <c r="B17">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>667</v>
+      </c>
+      <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>668</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>669</v>
+      </c>
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>670</v>
+      </c>
+      <c r="B21">
+        <v>68</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="66" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>672</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>673</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>674</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>675</v>
+      </c>
+      <c r="B26">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>676</v>
+      </c>
+      <c r="B27">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>677</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>678</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>679</v>
+      </c>
+      <c r="B30">
+        <v>47</v>
+      </c>
+      <c r="C30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="66" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>681</v>
+      </c>
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>682</v>
+      </c>
+      <c r="B33">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>683</v>
+      </c>
+      <c r="B34">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>684</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>685</v>
+      </c>
+      <c r="B36">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>686</v>
+      </c>
+      <c r="B37">
+        <v>52</v>
+      </c>
+      <c r="C37">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>687</v>
+      </c>
+      <c r="B38">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>688</v>
+      </c>
+      <c r="B39">
+        <v>69</v>
+      </c>
+      <c r="C39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>689</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>690</v>
+      </c>
+      <c r="B41">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="66" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>692</v>
+      </c>
+      <c r="B43">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>693</v>
+      </c>
+      <c r="B44">
+        <v>22</v>
+      </c>
+      <c r="C44">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>694</v>
+      </c>
+      <c r="B45">
+        <v>24</v>
+      </c>
+      <c r="C45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>695</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>696</v>
+      </c>
+      <c r="B47">
+        <v>31</v>
+      </c>
+      <c r="C47">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>697</v>
+      </c>
+      <c r="B48">
+        <v>40</v>
+      </c>
+      <c r="C48">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="66" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>699</v>
+      </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>700</v>
+      </c>
+      <c r="B51">
+        <v>23</v>
+      </c>
+      <c r="C51">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>701</v>
+      </c>
+      <c r="B52">
+        <v>33</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>702</v>
+      </c>
+      <c r="B53">
+        <v>22</v>
+      </c>
+      <c r="C53">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>703</v>
+      </c>
+      <c r="B54">
+        <v>45</v>
+      </c>
+      <c r="C54">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>704</v>
+      </c>
+      <c r="B55">
+        <v>51</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>705</v>
+      </c>
+      <c r="B56">
+        <v>32</v>
+      </c>
+      <c r="C56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>706</v>
+      </c>
+      <c r="B57">
+        <v>54</v>
+      </c>
+      <c r="C57">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>707</v>
+      </c>
+      <c r="B58">
+        <v>11</v>
+      </c>
+      <c r="C58">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>708</v>
+      </c>
+      <c r="B59">
+        <v>31</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>709</v>
+      </c>
+      <c r="B60">
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>710</v>
+      </c>
+      <c r="B61">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="66" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>712</v>
+      </c>
+      <c r="B63">
+        <v>24</v>
+      </c>
+      <c r="C63">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>713</v>
+      </c>
+      <c r="B64">
+        <v>19</v>
+      </c>
+      <c r="C64">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>714</v>
+      </c>
+      <c r="B65">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>715</v>
+      </c>
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>716</v>
+      </c>
+      <c r="B67">
+        <v>16</v>
+      </c>
+      <c r="C67">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>717</v>
+      </c>
+      <c r="B68">
+        <v>14</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="35" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：28:35:01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added notes for 14_Vue_intro:L07:component events
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83459D1-3363-4E00-8614-2EE0D55DBE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB745C1-F3B7-4304-B360-DEA70254D8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13440" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6029,7 +6029,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6058,13 +6058,13 @@
       <c r="A2" t="s">
         <v>499</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="63">
         <v>23</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="63">
         <v>57</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="51">
         <v>1</v>
       </c>
     </row>
@@ -6072,13 +6072,13 @@
       <c r="A3" t="s">
         <v>500</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="63">
         <v>22</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="63">
         <v>5</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="51">
         <v>1</v>
       </c>
     </row>
@@ -6086,13 +6086,13 @@
       <c r="A4" t="s">
         <v>501</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="63">
         <v>48</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="63">
         <v>15</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="51">
         <v>1</v>
       </c>
     </row>
@@ -6100,13 +6100,13 @@
       <c r="A5" t="s">
         <v>502</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="63">
         <v>40</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="63">
         <v>9</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="51">
         <v>2</v>
       </c>
     </row>
@@ -6114,13 +6114,13 @@
       <c r="A6" t="s">
         <v>503</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="63">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="63">
         <v>46</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="51">
         <v>2</v>
       </c>
     </row>
@@ -6128,13 +6128,13 @@
       <c r="A7" t="s">
         <v>504</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="63">
         <v>47</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="63">
         <v>50</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="51">
         <v>2</v>
       </c>
     </row>
@@ -6142,13 +6142,13 @@
       <c r="A8" t="s">
         <v>505</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="63">
         <v>38</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="63">
         <v>26</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="51">
         <v>2</v>
       </c>
     </row>
@@ -6156,13 +6156,13 @@
       <c r="A9" t="s">
         <v>506</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="63">
         <v>84</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="63">
         <v>18</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="51">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added notes for 14_Vue_intro:L08: project structure optimization
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB745C1-F3B7-4304-B360-DEA70254D8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D39E6C-FFB1-4AF5-AA37-14D025B2448E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13440" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6029,7 +6029,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6170,13 +6170,13 @@
       <c r="A10" t="s">
         <v>507</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="63">
         <v>17</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="63">
         <v>25</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="51">
         <v>4</v>
       </c>
     </row>
@@ -6184,13 +6184,13 @@
       <c r="A11" t="s">
         <v>508</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="63">
         <v>112</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="63">
         <v>57</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="51">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added notes for 14_Vue_intro:L09: implemented Empty, ImageLoader & Contact (ContactItem)
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D39E6C-FFB1-4AF5-AA37-14D025B2448E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C30F07E-B080-43DD-B388-8D7209260177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13440" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -5795,7 +5795,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6028,8 +6028,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9134,9 +9134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97C62C-B5D1-4E72-812F-7EA03DA117C7}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
added notes for 14_Vue_intro:L15: Main page implementation (Part 1/3)
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C30F07E-B080-43DD-B388-8D7209260177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7180EB23-47B0-48D4-8FCD-765133F9CC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="690" windowWidth="19995" windowHeight="13440" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="6855" yWindow="915" windowWidth="19995" windowHeight="13440" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -6028,8 +6028,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6198,13 +6198,13 @@
       <c r="A12" t="s">
         <v>509</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="63">
         <v>33</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="63">
         <v>49</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="51">
         <v>5</v>
       </c>
     </row>
@@ -6212,13 +6212,13 @@
       <c r="A13" t="s">
         <v>510</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="63">
         <v>54</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="63">
         <v>9</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="51">
         <v>5</v>
       </c>
     </row>
@@ -6226,13 +6226,13 @@
       <c r="A14" t="s">
         <v>511</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="63">
         <v>71</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="63">
         <v>2</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="51">
         <v>6</v>
       </c>
     </row>
@@ -6240,13 +6240,13 @@
       <c r="A15" t="s">
         <v>512</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="63">
         <v>57</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="63">
         <v>59</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="51">
         <v>6</v>
       </c>
     </row>
@@ -6254,13 +6254,13 @@
       <c r="A16" t="s">
         <v>513</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="63">
         <v>34</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="63">
         <v>48</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="51">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L18: Vue 2.x custom directives in action
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7180EB23-47B0-48D4-8FCD-765133F9CC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAF3C0B-E8C4-48FD-807A-2A83F7EACB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6855" yWindow="915" windowWidth="19995" windowHeight="13440" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6028,8 +6028,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6268,13 +6268,13 @@
       <c r="A17" t="s">
         <v>514</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="63">
         <v>44</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="63">
         <v>14</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="51">
         <v>7</v>
       </c>
     </row>
@@ -6282,13 +6282,13 @@
       <c r="A18" t="s">
         <v>515</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="63">
         <v>41</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="63">
         <v>25</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="51">
         <v>7</v>
       </c>
     </row>
@@ -6296,13 +6296,13 @@
       <c r="A19" t="s">
         <v>516</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="63">
         <v>34</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="63">
         <v>9</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="51">
         <v>8</v>
       </c>
     </row>
@@ -6310,41 +6310,43 @@
       <c r="A20" t="s">
         <v>517</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="63">
         <v>41</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="63">
         <v>54</v>
       </c>
-      <c r="D20" s="25">
-        <v>8</v>
+      <c r="D20" s="51">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>518</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="63">
         <v>12</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="63">
         <v>19</v>
       </c>
-      <c r="D21" s="25">
-        <v>8</v>
+      <c r="D21" s="51">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>519</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="63">
         <v>27</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="63">
         <v>31</v>
       </c>
-      <c r="D22" s="25"/>
+      <c r="D22" s="51">
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -6631,6 +6633,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add notes for 15_Vue_intro:L2: 1st Vue App
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAF3C0B-E8C4-48FD-807A-2A83F7EACB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51610645-DECE-4B45-BF04-A61D27A404C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6855" yWindow="915" windowWidth="19995" windowHeight="13440" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="21" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="19Miniapp" sheetId="17" r:id="rId19"/>
     <sheet name="20Echarts" sheetId="20" r:id="rId20"/>
     <sheet name="21Webpack" sheetId="21" r:id="rId21"/>
+    <sheet name="22BPMN" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="741">
   <si>
     <t>1. 环境准备</t>
   </si>
@@ -2244,13 +2245,76 @@
   <si>
     <t>webpack-课程前导</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01.课程导读</t>
+  </si>
+  <si>
+    <t>02.认识BPMN</t>
+  </si>
+  <si>
+    <t>03.工作流引擎的简单介绍</t>
+  </si>
+  <si>
+    <t>04.bpmn.js基础使用</t>
+  </si>
+  <si>
+    <t>05.bpmn.js常见功能处理</t>
+  </si>
+  <si>
+    <t>06.了解bpmn.js的底层实现</t>
+  </si>
+  <si>
+    <t>07.简单引入自定义Palette处理</t>
+  </si>
+  <si>
+    <t>08.自定义Palette模块实现</t>
+  </si>
+  <si>
+    <t>09.自定义Modeler替换</t>
+  </si>
+  <si>
+    <t>10.自定义renderer</t>
+  </si>
+  <si>
+    <t>11.自定义ContextPad</t>
+  </si>
+  <si>
+    <t>12.使用仓库保存节点数据</t>
+  </si>
+  <si>
+    <t>13.自定义封装处理-1</t>
+  </si>
+  <si>
+    <t>14.自定义封装处理-2</t>
+  </si>
+  <si>
+    <t>15.bpmn properties</t>
+  </si>
+  <si>
+    <t>16.moddleExtension描述文件</t>
+  </si>
+  <si>
+    <t>17.自定义PropertiesPanelExtension扩展</t>
+  </si>
+  <si>
+    <t>18.完全自定义PropertiesPanel</t>
+  </si>
+  <si>
+    <t>19.flowable工作流引擎处理</t>
+  </si>
+  <si>
+    <t>20.通过flowable相关API实现工作流处理</t>
+  </si>
+  <si>
+    <t>BPMN可视化与工作流实践 - 闫虹志</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2355,6 +2419,21 @@
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF262626"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -2516,7 +2595,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2717,6 +2796,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6028,7 +6113,7 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -9137,7 +9222,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97C62C-B5D1-4E72-812F-7EA03DA117C7}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9864,6 +9951,270 @@
       <c r="A69" s="35" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：28:35:01</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94422AE2-1435-4D63-A4A0-EC2A97CE768E}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="68" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="67" t="s">
+        <v>720</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="67" t="s">
+        <v>721</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="67" t="s">
+        <v>722</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="67" t="s">
+        <v>723</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="67" t="s">
+        <v>724</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="67" t="s">
+        <v>725</v>
+      </c>
+      <c r="B8">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="67" t="s">
+        <v>726</v>
+      </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="67" t="s">
+        <v>727</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="67" t="s">
+        <v>728</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="67" t="s">
+        <v>729</v>
+      </c>
+      <c r="B12">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="67" t="s">
+        <v>730</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="67" t="s">
+        <v>731</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="67" t="s">
+        <v>732</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="67" t="s">
+        <v>733</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="67" t="s">
+        <v>734</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="67" t="s">
+        <v>735</v>
+      </c>
+      <c r="B18">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="67" t="s">
+        <v>736</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="67" t="s">
+        <v>737</v>
+      </c>
+      <c r="B20">
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="67" t="s">
+        <v>738</v>
+      </c>
+      <c r="B21">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="67" t="s">
+        <v>739</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：7:45:18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated notes for 15_Vue_intro:L04:Vue components,L04_05:vue cli version
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51610645-DECE-4B45-BF04-A61D27A404C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2959DFF-B07E-4C44-95FC-B002E507668E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="21" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="3660" yWindow="2100" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -2595,7 +2595,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2802,6 +2802,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6113,8 +6116,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6192,7 +6195,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -6206,7 +6209,7 @@
         <v>46</v>
       </c>
       <c r="D6" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -6219,7 +6222,7 @@
       <c r="C7" s="63">
         <v>50</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="69">
         <v>2</v>
       </c>
     </row>
@@ -6233,7 +6236,7 @@
       <c r="C8" s="63">
         <v>26</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="69">
         <v>2</v>
       </c>
     </row>
@@ -6247,7 +6250,7 @@
       <c r="C9" s="63">
         <v>18</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="69">
         <v>3</v>
       </c>
     </row>
@@ -6261,7 +6264,7 @@
       <c r="C10" s="63">
         <v>25</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="69">
         <v>4</v>
       </c>
     </row>
@@ -6275,7 +6278,7 @@
       <c r="C11" s="63">
         <v>57</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="69">
         <v>4</v>
       </c>
     </row>
@@ -6289,7 +6292,7 @@
       <c r="C12" s="63">
         <v>49</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="69">
         <v>5</v>
       </c>
     </row>
@@ -6303,7 +6306,7 @@
       <c r="C13" s="63">
         <v>9</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="69">
         <v>5</v>
       </c>
     </row>
@@ -6317,7 +6320,7 @@
       <c r="C14" s="63">
         <v>2</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="69">
         <v>6</v>
       </c>
     </row>
@@ -6331,7 +6334,7 @@
       <c r="C15" s="63">
         <v>59</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="69">
         <v>6</v>
       </c>
     </row>
@@ -6345,7 +6348,7 @@
       <c r="C16" s="63">
         <v>48</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="69">
         <v>7</v>
       </c>
     </row>
@@ -6359,7 +6362,7 @@
       <c r="C17" s="63">
         <v>14</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="69">
         <v>7</v>
       </c>
     </row>
@@ -6373,7 +6376,7 @@
       <c r="C18" s="63">
         <v>25</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="69">
         <v>7</v>
       </c>
     </row>
@@ -6387,7 +6390,7 @@
       <c r="C19" s="63">
         <v>9</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="69">
         <v>8</v>
       </c>
     </row>
@@ -6401,7 +6404,7 @@
       <c r="C20" s="63">
         <v>54</v>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="69">
         <v>9</v>
       </c>
     </row>
@@ -6415,7 +6418,7 @@
       <c r="C21" s="63">
         <v>19</v>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="69">
         <v>9</v>
       </c>
     </row>
@@ -6429,7 +6432,7 @@
       <c r="C22" s="63">
         <v>31</v>
       </c>
-      <c r="D22" s="51">
+      <c r="D22" s="69">
         <v>9</v>
       </c>
     </row>
@@ -9963,7 +9966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94422AE2-1435-4D63-A4A0-EC2A97CE768E}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated notes for 15_Vue_intro:L06-L08
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2959DFF-B07E-4C44-95FC-B002E507668E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39D68AC-F54B-4111-8C03-BA5CB7162FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2100" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6117,7 +6117,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6222,7 +6222,7 @@
       <c r="C7" s="63">
         <v>50</v>
       </c>
-      <c r="D7" s="69">
+      <c r="D7" s="51">
         <v>2</v>
       </c>
     </row>
@@ -6236,8 +6236,8 @@
       <c r="C8" s="63">
         <v>26</v>
       </c>
-      <c r="D8" s="69">
-        <v>2</v>
+      <c r="D8" s="51">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -6250,7 +6250,7 @@
       <c r="C9" s="63">
         <v>18</v>
       </c>
-      <c r="D9" s="69">
+      <c r="D9" s="51">
         <v>3</v>
       </c>
     </row>
@@ -6264,8 +6264,8 @@
       <c r="C10" s="63">
         <v>25</v>
       </c>
-      <c r="D10" s="69">
-        <v>4</v>
+      <c r="D10" s="51">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated notes for 15_Vue_intro:L09-L12
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39D68AC-F54B-4111-8C03-BA5CB7162FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F52EF88-46FA-4231-BD02-185730DCE3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2100" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6116,8 +6116,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6278,7 +6278,7 @@
       <c r="C11" s="63">
         <v>57</v>
       </c>
-      <c r="D11" s="69">
+      <c r="D11" s="51">
         <v>4</v>
       </c>
     </row>
@@ -6292,7 +6292,7 @@
       <c r="C12" s="63">
         <v>49</v>
       </c>
-      <c r="D12" s="69">
+      <c r="D12" s="51">
         <v>5</v>
       </c>
     </row>
@@ -6306,7 +6306,7 @@
       <c r="C13" s="63">
         <v>9</v>
       </c>
-      <c r="D13" s="69">
+      <c r="D13" s="51">
         <v>5</v>
       </c>
     </row>
@@ -6320,8 +6320,8 @@
       <c r="C14" s="63">
         <v>2</v>
       </c>
-      <c r="D14" s="69">
-        <v>6</v>
+      <c r="D14" s="51">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
reviewed notes for 15_Vue_intro:L13-L14
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F52EF88-46FA-4231-BD02-185730DCE3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7756DB5C-D7DC-4911-A007-F392E855680B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2100" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6117,7 +6117,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6334,7 +6334,7 @@
       <c r="C15" s="63">
         <v>59</v>
       </c>
-      <c r="D15" s="69">
+      <c r="D15" s="51">
         <v>6</v>
       </c>
     </row>
@@ -6348,8 +6348,8 @@
       <c r="C16" s="63">
         <v>48</v>
       </c>
-      <c r="D16" s="69">
-        <v>7</v>
+      <c r="D16" s="51">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated notes for 15_Vue_intro:L15-L19
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7756DB5C-D7DC-4911-A007-F392E855680B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105BB307-9859-4232-A729-7ACC697DF6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2100" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -2438,7 +2438,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2460,6 +2460,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C0A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2595,7 +2601,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2804,6 +2810,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6116,8 +6125,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6278,7 +6287,7 @@
       <c r="C11" s="63">
         <v>57</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="70">
         <v>4</v>
       </c>
     </row>
@@ -6362,7 +6371,7 @@
       <c r="C17" s="63">
         <v>14</v>
       </c>
-      <c r="D17" s="69">
+      <c r="D17" s="51">
         <v>7</v>
       </c>
     </row>
@@ -6376,7 +6385,7 @@
       <c r="C18" s="63">
         <v>25</v>
       </c>
-      <c r="D18" s="69">
+      <c r="D18" s="51">
         <v>7</v>
       </c>
     </row>
@@ -6390,8 +6399,8 @@
       <c r="C19" s="63">
         <v>9</v>
       </c>
-      <c r="D19" s="69">
-        <v>8</v>
+      <c r="D19" s="51">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -6404,8 +6413,8 @@
       <c r="C20" s="63">
         <v>54</v>
       </c>
-      <c r="D20" s="69">
-        <v>9</v>
+      <c r="D20" s="51">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -6418,8 +6427,8 @@
       <c r="C21" s="63">
         <v>19</v>
       </c>
-      <c r="D21" s="69">
-        <v>9</v>
+      <c r="D21" s="51">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated notes for 15_Vue_intro:L21-L22
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105BB307-9859-4232-A729-7ACC697DF6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B62885B-5238-45A6-AAD6-0C822D50F2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -2601,7 +2601,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2808,9 +2808,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6126,7 +6123,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D22" sqref="D22:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6287,7 +6284,7 @@
       <c r="C11" s="63">
         <v>57</v>
       </c>
-      <c r="D11" s="70">
+      <c r="D11" s="69">
         <v>4</v>
       </c>
     </row>
@@ -6441,8 +6438,8 @@
       <c r="C22" s="63">
         <v>31</v>
       </c>
-      <c r="D22" s="69">
-        <v>9</v>
+      <c r="D22" s="51">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -6455,7 +6452,9 @@
       <c r="C23">
         <v>43</v>
       </c>
-      <c r="D23" s="25"/>
+      <c r="D23" s="51">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -6467,7 +6466,9 @@
       <c r="C24">
         <v>32</v>
       </c>
-      <c r="D24" s="25"/>
+      <c r="D24" s="51">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L23: blog detail preparations
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B62885B-5238-45A6-AAD6-0C822D50F2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCB4E65-F918-4547-9593-9CB3E53F5482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -2601,7 +2601,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2811,6 +2811,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6122,8 +6125,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6446,10 +6449,10 @@
       <c r="A23" t="s">
         <v>520</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="70">
         <v>26</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="70">
         <v>43</v>
       </c>
       <c r="D23" s="51">
@@ -6460,10 +6463,10 @@
       <c r="A24" t="s">
         <v>521</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="70">
         <v>94</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="70">
         <v>32</v>
       </c>
       <c r="D24" s="51">
@@ -6474,13 +6477,15 @@
       <c r="A25" t="s">
         <v>522</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="63">
         <v>24</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="63">
         <v>19</v>
       </c>
-      <c r="D25" s="25"/>
+      <c r="D25" s="51">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L24: Blog detail page & TOC interactions
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCB4E65-F918-4547-9593-9CB3E53F5482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D812512-311B-4CBC-AD23-5AA259CB12FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6126,7 +6126,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6491,13 +6491,15 @@
       <c r="A26" t="s">
         <v>523</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="63">
         <v>39</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="63">
         <v>22</v>
       </c>
-      <c r="D26" s="25"/>
+      <c r="D26" s="51">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -7156,7 +7158,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L26: implemented BlogComment section
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D812512-311B-4CBC-AD23-5AA259CB12FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A267595E-0831-46F8-9FB1-B19FF8E63F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6125,8 +6125,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6505,49 +6505,57 @@
       <c r="A27" t="s">
         <v>524</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="70">
         <v>43</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="70">
         <v>7</v>
       </c>
-      <c r="D27" s="25"/>
+      <c r="D27" s="51">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>525</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="63">
         <v>48</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="63">
         <v>12</v>
       </c>
-      <c r="D28" s="25"/>
+      <c r="D28" s="51">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>526</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="70">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="70">
         <v>28</v>
       </c>
-      <c r="D29" s="25"/>
+      <c r="D29" s="25">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>527</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="70">
         <v>40</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="70">
         <v>26</v>
       </c>
-      <c r="D30" s="25"/>
+      <c r="D30" s="25">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L29: incremental bottom loading
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A267595E-0831-46F8-9FB1-B19FF8E63F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919F73A3-90F4-4811-81D0-1E9CFA0CD498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6125,8 +6125,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6539,7 +6539,7 @@
       <c r="C29" s="70">
         <v>28</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="51">
         <v>12</v>
       </c>
     </row>
@@ -6553,7 +6553,7 @@
       <c r="C30" s="70">
         <v>26</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="51">
         <v>12</v>
       </c>
     </row>
@@ -6561,25 +6561,29 @@
       <c r="A31" t="s">
         <v>528</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="70">
         <v>37</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="70">
         <v>59</v>
       </c>
-      <c r="D31" s="25"/>
+      <c r="D31" s="25">
+        <v>13</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>529</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="70">
         <v>10</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="70">
         <v>22</v>
       </c>
-      <c r="D32" s="25"/>
+      <c r="D32" s="25">
+        <v>13</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L30: extract same event bus logics into mixins
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919F73A3-90F4-4811-81D0-1E9CFA0CD498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F586CE51-75F7-4810-9526-8BC8DFA0314F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6126,7 +6126,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B33" sqref="B33:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6567,7 +6567,7 @@
       <c r="C31" s="70">
         <v>59</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="51">
         <v>13</v>
       </c>
     </row>
@@ -6581,7 +6581,7 @@
       <c r="C32" s="70">
         <v>22</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="51">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated notes for 15_Vue_intro:L30: completed ToTop preview component
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F586CE51-75F7-4810-9526-8BC8DFA0314F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0678B49B-8660-4530-A06D-2ECB9665E490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6126,7 +6126,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:C33"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6589,25 +6589,29 @@
       <c r="A33" t="s">
         <v>530</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="70">
         <v>39</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="70">
         <v>40</v>
       </c>
-      <c r="D33" s="25"/>
+      <c r="D33" s="25">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>531</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="70">
         <v>46</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="70">
         <v>33</v>
       </c>
-      <c r="D34" s="25"/>
+      <c r="D34" s="25">
+        <v>14</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L31: image lazy loading via customized v-lazy directive
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0678B49B-8660-4530-A06D-2ECB9665E490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B9C2ED-93E6-41CC-BD0A-F713E86696BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6126,7 +6126,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6595,7 +6595,7 @@
       <c r="C33" s="70">
         <v>40</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="51">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L32: data sharing with Vuex
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B9C2ED-93E6-41CC-BD0A-F713E86696BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2FB614-A2F9-4201-B2E6-91888888446B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6126,7 +6126,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6609,7 +6609,7 @@
       <c r="C34" s="70">
         <v>33</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="51">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated notes for 15_Vue_intro:L32: learning Vuex 3.x official docs
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2FB614-A2F9-4201-B2E6-91888888446B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB500CAE-3154-4949-AFE8-394BAD9BA9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6126,7 +6126,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6617,13 +6617,15 @@
       <c r="A35" t="s">
         <v>532</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="70">
         <v>98</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="70">
         <v>10</v>
       </c>
-      <c r="D35" s="25"/>
+      <c r="D35" s="25">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L34: Vuex in action: updated Home & SiteAside for my-site project
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB500CAE-3154-4949-AFE8-394BAD9BA9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE73BD0-D5C4-4A8C-984D-BDFAACC409E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2445" windowWidth="21600" windowHeight="11385" tabRatio="722" firstSheet="14" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6125,8 +6125,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6617,13 +6617,13 @@
       <c r="A35" t="s">
         <v>532</v>
       </c>
-      <c r="B35" s="70">
+      <c r="B35" s="63">
         <v>98</v>
       </c>
-      <c r="C35" s="70">
+      <c r="C35" s="63">
         <v>10</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="51">
         <v>15</v>
       </c>
     </row>
@@ -6631,13 +6631,15 @@
       <c r="A36" t="s">
         <v>533</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="63">
         <v>23</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="63">
         <v>50</v>
       </c>
-      <c r="D36" s="25"/>
+      <c r="D36" s="51">
+        <v>16</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L37: Project page
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99341259-0E82-458B-A48C-FDE4733E10D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623DE2A8-14DF-49CC-BA9B-86D61A656101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="16" activeTab="22" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="15" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -3021,7 +3021,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3252,9 +3252,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="34"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="24"/>
@@ -5574,13 +5571,12 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="79" t="str">
+      <c r="A16" s="78" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：7:32:31</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="77"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6036,7 +6032,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B3" sqref="B3:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6269,11 +6265,11 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomRight" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6854,7 +6850,7 @@
       <c r="C41" s="63">
         <v>43</v>
       </c>
-      <c r="D41" s="25">
+      <c r="D41" s="45">
         <v>16</v>
       </c>
     </row>
@@ -9682,7 +9678,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
@@ -10716,7 +10712,7 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -11913,7 +11909,7 @@
       <c r="D1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="79" t="s">
         <v>740</v>
       </c>
     </row>
@@ -14793,13 +14789,12 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="78" t="str">
+      <c r="A10" s="77" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：6:56:56</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="77"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L39: Bundle optimizations
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623DE2A8-14DF-49CC-BA9B-86D61A656101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC09414-01C8-4764-B6D5-43032F7070AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="15" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6269,7 +6269,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6851,7 +6851,7 @@
         <v>43</v>
       </c>
       <c r="D41" s="45">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added notes for 15_Vue_intro:L41: handling empty scenarios
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC09414-01C8-4764-B6D5-43032F7070AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8F153A-4465-422A-9518-139985468170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="15" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6269,7 +6269,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6858,34 +6858,38 @@
       <c r="A42" t="s">
         <v>539</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="63">
         <v>23</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="63">
         <v>43</v>
       </c>
-      <c r="D42" s="25"/>
+      <c r="D42" s="45">
+        <v>18</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>540</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="63">
         <v>6</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="63">
         <v>9</v>
       </c>
-      <c r="D43" s="25"/>
+      <c r="D43" s="45">
+        <v>18</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>541</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="63">
         <v>5</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="63">
         <v>27</v>
       </c>
       <c r="D44" s="25"/>
@@ -6894,10 +6898,10 @@
       <c r="A45" s="33" t="s">
         <v>542</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="63">
         <v>32</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="63">
         <v>30</v>
       </c>
       <c r="D45" s="25"/>

</xml_diff>

<commit_message>
added README & notes for L01: Vue introduction
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8F153A-4465-422A-9518-139985468170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244248A5-E8CD-47CE-A1C6-01F721F660B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="15" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="13" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -28,8 +28,8 @@
     <sheet name="13Git" sheetId="12" r:id="rId13"/>
     <sheet name="14ThirdLib" sheetId="13" r:id="rId14"/>
     <sheet name="15Build" sheetId="14" r:id="rId15"/>
-    <sheet name="16Vue_scratch" sheetId="19" r:id="rId16"/>
-    <sheet name="17Vue_intro" sheetId="15" r:id="rId17"/>
+    <sheet name="16Vue_intro" sheetId="15" r:id="rId16"/>
+    <sheet name="17Vue_scratch" sheetId="19" r:id="rId17"/>
     <sheet name="18Vue_comp" sheetId="16" r:id="rId18"/>
     <sheet name="19Vue3" sheetId="23" r:id="rId19"/>
     <sheet name="20Vue3_new" sheetId="24" r:id="rId20"/>
@@ -6027,12 +6027,675 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AF8CD0-73B6-411F-82CC-0DBAA39229A0}">
+  <sheetPr codeName="Sheet17"/>
+  <dimension ref="A1:F46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F45" sqref="F45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>499</v>
+      </c>
+      <c r="B2" s="57">
+        <v>23</v>
+      </c>
+      <c r="C2" s="57">
+        <v>57</v>
+      </c>
+      <c r="D2" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B3" s="57">
+        <v>22</v>
+      </c>
+      <c r="C3" s="57">
+        <v>5</v>
+      </c>
+      <c r="D3" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>501</v>
+      </c>
+      <c r="B4" s="57">
+        <v>48</v>
+      </c>
+      <c r="C4" s="57">
+        <v>15</v>
+      </c>
+      <c r="D4" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>502</v>
+      </c>
+      <c r="B5" s="57">
+        <v>40</v>
+      </c>
+      <c r="C5" s="57">
+        <v>9</v>
+      </c>
+      <c r="D5" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>503</v>
+      </c>
+      <c r="B6" s="57">
+        <v>7</v>
+      </c>
+      <c r="C6" s="57">
+        <v>46</v>
+      </c>
+      <c r="D6" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B7" s="57">
+        <v>47</v>
+      </c>
+      <c r="C7" s="57">
+        <v>50</v>
+      </c>
+      <c r="D7" s="45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>505</v>
+      </c>
+      <c r="B8" s="57">
+        <v>38</v>
+      </c>
+      <c r="C8" s="57">
+        <v>26</v>
+      </c>
+      <c r="D8" s="45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>506</v>
+      </c>
+      <c r="B9" s="57">
+        <v>84</v>
+      </c>
+      <c r="C9" s="57">
+        <v>18</v>
+      </c>
+      <c r="D9" s="45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>507</v>
+      </c>
+      <c r="B10" s="57">
+        <v>17</v>
+      </c>
+      <c r="C10" s="57">
+        <v>25</v>
+      </c>
+      <c r="D10" s="45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>508</v>
+      </c>
+      <c r="B11" s="57">
+        <v>112</v>
+      </c>
+      <c r="C11" s="57">
+        <v>57</v>
+      </c>
+      <c r="D11" s="62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>509</v>
+      </c>
+      <c r="B12" s="57">
+        <v>33</v>
+      </c>
+      <c r="C12" s="57">
+        <v>49</v>
+      </c>
+      <c r="D12" s="45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>510</v>
+      </c>
+      <c r="B13" s="57">
+        <v>54</v>
+      </c>
+      <c r="C13" s="57">
+        <v>9</v>
+      </c>
+      <c r="D13" s="45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>511</v>
+      </c>
+      <c r="B14" s="57">
+        <v>71</v>
+      </c>
+      <c r="C14" s="57">
+        <v>2</v>
+      </c>
+      <c r="D14" s="45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>512</v>
+      </c>
+      <c r="B15" s="57">
+        <v>57</v>
+      </c>
+      <c r="C15" s="57">
+        <v>59</v>
+      </c>
+      <c r="D15" s="45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>513</v>
+      </c>
+      <c r="B16" s="57">
+        <v>34</v>
+      </c>
+      <c r="C16" s="57">
+        <v>48</v>
+      </c>
+      <c r="D16" s="45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>514</v>
+      </c>
+      <c r="B17" s="57">
+        <v>44</v>
+      </c>
+      <c r="C17" s="57">
+        <v>14</v>
+      </c>
+      <c r="D17" s="45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>515</v>
+      </c>
+      <c r="B18" s="57">
+        <v>41</v>
+      </c>
+      <c r="C18" s="57">
+        <v>25</v>
+      </c>
+      <c r="D18" s="45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>516</v>
+      </c>
+      <c r="B19" s="57">
+        <v>34</v>
+      </c>
+      <c r="C19" s="57">
+        <v>9</v>
+      </c>
+      <c r="D19" s="45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>517</v>
+      </c>
+      <c r="B20" s="57">
+        <v>41</v>
+      </c>
+      <c r="C20" s="57">
+        <v>54</v>
+      </c>
+      <c r="D20" s="45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>518</v>
+      </c>
+      <c r="B21" s="57">
+        <v>12</v>
+      </c>
+      <c r="C21" s="57">
+        <v>19</v>
+      </c>
+      <c r="D21" s="45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>519</v>
+      </c>
+      <c r="B22" s="57">
+        <v>27</v>
+      </c>
+      <c r="C22" s="57">
+        <v>31</v>
+      </c>
+      <c r="D22" s="45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>520</v>
+      </c>
+      <c r="B23" s="63">
+        <v>26</v>
+      </c>
+      <c r="C23" s="63">
+        <v>43</v>
+      </c>
+      <c r="D23" s="45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>521</v>
+      </c>
+      <c r="B24" s="63">
+        <v>94</v>
+      </c>
+      <c r="C24" s="63">
+        <v>32</v>
+      </c>
+      <c r="D24" s="45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>522</v>
+      </c>
+      <c r="B25" s="57">
+        <v>24</v>
+      </c>
+      <c r="C25" s="57">
+        <v>19</v>
+      </c>
+      <c r="D25" s="45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>523</v>
+      </c>
+      <c r="B26" s="57">
+        <v>39</v>
+      </c>
+      <c r="C26" s="57">
+        <v>22</v>
+      </c>
+      <c r="D26" s="45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>524</v>
+      </c>
+      <c r="B27" s="63">
+        <v>43</v>
+      </c>
+      <c r="C27" s="63">
+        <v>7</v>
+      </c>
+      <c r="D27" s="45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>525</v>
+      </c>
+      <c r="B28" s="57">
+        <v>48</v>
+      </c>
+      <c r="C28" s="57">
+        <v>12</v>
+      </c>
+      <c r="D28" s="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>526</v>
+      </c>
+      <c r="B29" s="63">
+        <v>28</v>
+      </c>
+      <c r="C29" s="63">
+        <v>28</v>
+      </c>
+      <c r="D29" s="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>527</v>
+      </c>
+      <c r="B30" s="63">
+        <v>40</v>
+      </c>
+      <c r="C30" s="63">
+        <v>26</v>
+      </c>
+      <c r="D30" s="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>528</v>
+      </c>
+      <c r="B31" s="63">
+        <v>37</v>
+      </c>
+      <c r="C31" s="63">
+        <v>59</v>
+      </c>
+      <c r="D31" s="45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>529</v>
+      </c>
+      <c r="B32" s="63">
+        <v>10</v>
+      </c>
+      <c r="C32" s="63">
+        <v>22</v>
+      </c>
+      <c r="D32" s="45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>530</v>
+      </c>
+      <c r="B33" s="63">
+        <v>39</v>
+      </c>
+      <c r="C33" s="63">
+        <v>40</v>
+      </c>
+      <c r="D33" s="45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>531</v>
+      </c>
+      <c r="B34" s="63">
+        <v>46</v>
+      </c>
+      <c r="C34" s="63">
+        <v>33</v>
+      </c>
+      <c r="D34" s="45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>532</v>
+      </c>
+      <c r="B35" s="57">
+        <v>98</v>
+      </c>
+      <c r="C35" s="57">
+        <v>10</v>
+      </c>
+      <c r="D35" s="45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>533</v>
+      </c>
+      <c r="B36" s="57">
+        <v>23</v>
+      </c>
+      <c r="C36" s="57">
+        <v>50</v>
+      </c>
+      <c r="D36" s="45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>534</v>
+      </c>
+      <c r="B37" s="57">
+        <v>14</v>
+      </c>
+      <c r="C37" s="57">
+        <v>43</v>
+      </c>
+      <c r="D37" s="45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>535</v>
+      </c>
+      <c r="B38" s="63">
+        <v>12</v>
+      </c>
+      <c r="C38" s="63">
+        <v>36</v>
+      </c>
+      <c r="D38" s="45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>536</v>
+      </c>
+      <c r="B39" s="57">
+        <v>17</v>
+      </c>
+      <c r="C39" s="57">
+        <v>11</v>
+      </c>
+      <c r="D39" s="45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>537</v>
+      </c>
+      <c r="B40" s="57">
+        <v>14</v>
+      </c>
+      <c r="C40" s="57">
+        <v>53</v>
+      </c>
+      <c r="D40" s="45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>538</v>
+      </c>
+      <c r="B41" s="63">
+        <v>55</v>
+      </c>
+      <c r="C41" s="63">
+        <v>43</v>
+      </c>
+      <c r="D41" s="45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>539</v>
+      </c>
+      <c r="B42" s="63">
+        <v>23</v>
+      </c>
+      <c r="C42" s="63">
+        <v>43</v>
+      </c>
+      <c r="D42" s="45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>540</v>
+      </c>
+      <c r="B43" s="63">
+        <v>6</v>
+      </c>
+      <c r="C43" s="63">
+        <v>9</v>
+      </c>
+      <c r="D43" s="45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>541</v>
+      </c>
+      <c r="B44" s="63">
+        <v>5</v>
+      </c>
+      <c r="C44" s="63">
+        <v>27</v>
+      </c>
+      <c r="D44" s="45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="33" t="s">
+        <v>542</v>
+      </c>
+      <c r="B45" s="63">
+        <v>32</v>
+      </c>
+      <c r="C45" s="63">
+        <v>30</v>
+      </c>
+      <c r="D45" s="45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：28:01:05</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D093D58B-B7D0-4ABE-B71F-06475D33804E}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6066,44 +6729,56 @@
       <c r="A3" t="s">
         <v>583</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="57">
         <v>30</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="57">
         <v>52</v>
+      </c>
+      <c r="D3" s="45">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>584</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="57">
         <v>24</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="57">
         <v>7</v>
+      </c>
+      <c r="D4" s="45">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>585</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="57">
         <v>55</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="57">
         <v>35</v>
+      </c>
+      <c r="D5" s="45">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>586</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="57">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="57">
         <v>43</v>
+      </c>
+      <c r="D6" s="45">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6116,6 +6791,7 @@
       <c r="C7">
         <v>51</v>
       </c>
+      <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -6127,11 +6803,13 @@
       <c r="C8">
         <v>52</v>
       </c>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>581</v>
       </c>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -6143,6 +6821,7 @@
       <c r="C10">
         <v>38</v>
       </c>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -6154,6 +6833,7 @@
       <c r="C11">
         <v>51</v>
       </c>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -6165,6 +6845,7 @@
       <c r="C12">
         <v>57</v>
       </c>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -6176,6 +6857,7 @@
       <c r="C13">
         <v>28</v>
       </c>
+      <c r="D13" s="25"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -6187,11 +6869,13 @@
       <c r="C14">
         <v>21</v>
       </c>
+      <c r="D14" s="25"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>582</v>
       </c>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -6203,8 +6887,9 @@
       <c r="C16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>595</v>
       </c>
@@ -6214,8 +6899,9 @@
       <c r="C17">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>596</v>
       </c>
@@ -6225,8 +6911,9 @@
       <c r="C18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>597</v>
       </c>
@@ -6236,8 +6923,9 @@
       <c r="C19">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="25"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>598</v>
       </c>
@@ -6247,669 +6935,12 @@
       <c r="C20">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="37" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：8:07:22</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AF8CD0-73B6-411F-82CC-0DBAA39229A0}">
-  <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1:F46"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>499</v>
-      </c>
-      <c r="B2" s="57">
-        <v>23</v>
-      </c>
-      <c r="C2" s="57">
-        <v>57</v>
-      </c>
-      <c r="D2" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>500</v>
-      </c>
-      <c r="B3" s="57">
-        <v>22</v>
-      </c>
-      <c r="C3" s="57">
-        <v>5</v>
-      </c>
-      <c r="D3" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>501</v>
-      </c>
-      <c r="B4" s="57">
-        <v>48</v>
-      </c>
-      <c r="C4" s="57">
-        <v>15</v>
-      </c>
-      <c r="D4" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>502</v>
-      </c>
-      <c r="B5" s="57">
-        <v>40</v>
-      </c>
-      <c r="C5" s="57">
-        <v>9</v>
-      </c>
-      <c r="D5" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>503</v>
-      </c>
-      <c r="B6" s="57">
-        <v>7</v>
-      </c>
-      <c r="C6" s="57">
-        <v>46</v>
-      </c>
-      <c r="D6" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>504</v>
-      </c>
-      <c r="B7" s="57">
-        <v>47</v>
-      </c>
-      <c r="C7" s="57">
-        <v>50</v>
-      </c>
-      <c r="D7" s="45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>505</v>
-      </c>
-      <c r="B8" s="57">
-        <v>38</v>
-      </c>
-      <c r="C8" s="57">
-        <v>26</v>
-      </c>
-      <c r="D8" s="45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>506</v>
-      </c>
-      <c r="B9" s="57">
-        <v>84</v>
-      </c>
-      <c r="C9" s="57">
-        <v>18</v>
-      </c>
-      <c r="D9" s="45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>507</v>
-      </c>
-      <c r="B10" s="57">
-        <v>17</v>
-      </c>
-      <c r="C10" s="57">
-        <v>25</v>
-      </c>
-      <c r="D10" s="45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>508</v>
-      </c>
-      <c r="B11" s="57">
-        <v>112</v>
-      </c>
-      <c r="C11" s="57">
-        <v>57</v>
-      </c>
-      <c r="D11" s="62">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>509</v>
-      </c>
-      <c r="B12" s="57">
-        <v>33</v>
-      </c>
-      <c r="C12" s="57">
-        <v>49</v>
-      </c>
-      <c r="D12" s="45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>510</v>
-      </c>
-      <c r="B13" s="57">
-        <v>54</v>
-      </c>
-      <c r="C13" s="57">
-        <v>9</v>
-      </c>
-      <c r="D13" s="45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>511</v>
-      </c>
-      <c r="B14" s="57">
-        <v>71</v>
-      </c>
-      <c r="C14" s="57">
-        <v>2</v>
-      </c>
-      <c r="D14" s="45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>512</v>
-      </c>
-      <c r="B15" s="57">
-        <v>57</v>
-      </c>
-      <c r="C15" s="57">
-        <v>59</v>
-      </c>
-      <c r="D15" s="45">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>513</v>
-      </c>
-      <c r="B16" s="57">
-        <v>34</v>
-      </c>
-      <c r="C16" s="57">
-        <v>48</v>
-      </c>
-      <c r="D16" s="45">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>514</v>
-      </c>
-      <c r="B17" s="57">
-        <v>44</v>
-      </c>
-      <c r="C17" s="57">
-        <v>14</v>
-      </c>
-      <c r="D17" s="45">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>515</v>
-      </c>
-      <c r="B18" s="57">
-        <v>41</v>
-      </c>
-      <c r="C18" s="57">
-        <v>25</v>
-      </c>
-      <c r="D18" s="45">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>516</v>
-      </c>
-      <c r="B19" s="57">
-        <v>34</v>
-      </c>
-      <c r="C19" s="57">
-        <v>9</v>
-      </c>
-      <c r="D19" s="45">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>517</v>
-      </c>
-      <c r="B20" s="57">
-        <v>41</v>
-      </c>
-      <c r="C20" s="57">
-        <v>54</v>
-      </c>
-      <c r="D20" s="45">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>518</v>
-      </c>
-      <c r="B21" s="57">
-        <v>12</v>
-      </c>
-      <c r="C21" s="57">
-        <v>19</v>
-      </c>
-      <c r="D21" s="45">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>519</v>
-      </c>
-      <c r="B22" s="57">
-        <v>27</v>
-      </c>
-      <c r="C22" s="57">
-        <v>31</v>
-      </c>
-      <c r="D22" s="45">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>520</v>
-      </c>
-      <c r="B23" s="63">
-        <v>26</v>
-      </c>
-      <c r="C23" s="63">
-        <v>43</v>
-      </c>
-      <c r="D23" s="45">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>521</v>
-      </c>
-      <c r="B24" s="63">
-        <v>94</v>
-      </c>
-      <c r="C24" s="63">
-        <v>32</v>
-      </c>
-      <c r="D24" s="45">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>522</v>
-      </c>
-      <c r="B25" s="57">
-        <v>24</v>
-      </c>
-      <c r="C25" s="57">
-        <v>19</v>
-      </c>
-      <c r="D25" s="45">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>523</v>
-      </c>
-      <c r="B26" s="57">
-        <v>39</v>
-      </c>
-      <c r="C26" s="57">
-        <v>22</v>
-      </c>
-      <c r="D26" s="45">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>524</v>
-      </c>
-      <c r="B27" s="63">
-        <v>43</v>
-      </c>
-      <c r="C27" s="63">
-        <v>7</v>
-      </c>
-      <c r="D27" s="45">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>525</v>
-      </c>
-      <c r="B28" s="57">
-        <v>48</v>
-      </c>
-      <c r="C28" s="57">
-        <v>12</v>
-      </c>
-      <c r="D28" s="45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>526</v>
-      </c>
-      <c r="B29" s="63">
-        <v>28</v>
-      </c>
-      <c r="C29" s="63">
-        <v>28</v>
-      </c>
-      <c r="D29" s="45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>527</v>
-      </c>
-      <c r="B30" s="63">
-        <v>40</v>
-      </c>
-      <c r="C30" s="63">
-        <v>26</v>
-      </c>
-      <c r="D30" s="45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>528</v>
-      </c>
-      <c r="B31" s="63">
-        <v>37</v>
-      </c>
-      <c r="C31" s="63">
-        <v>59</v>
-      </c>
-      <c r="D31" s="45">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>529</v>
-      </c>
-      <c r="B32" s="63">
-        <v>10</v>
-      </c>
-      <c r="C32" s="63">
-        <v>22</v>
-      </c>
-      <c r="D32" s="45">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>530</v>
-      </c>
-      <c r="B33" s="63">
-        <v>39</v>
-      </c>
-      <c r="C33" s="63">
-        <v>40</v>
-      </c>
-      <c r="D33" s="45">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>531</v>
-      </c>
-      <c r="B34" s="63">
-        <v>46</v>
-      </c>
-      <c r="C34" s="63">
-        <v>33</v>
-      </c>
-      <c r="D34" s="45">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>532</v>
-      </c>
-      <c r="B35" s="57">
-        <v>98</v>
-      </c>
-      <c r="C35" s="57">
-        <v>10</v>
-      </c>
-      <c r="D35" s="45">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>533</v>
-      </c>
-      <c r="B36" s="57">
-        <v>23</v>
-      </c>
-      <c r="C36" s="57">
-        <v>50</v>
-      </c>
-      <c r="D36" s="45">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>534</v>
-      </c>
-      <c r="B37" s="57">
-        <v>14</v>
-      </c>
-      <c r="C37" s="57">
-        <v>43</v>
-      </c>
-      <c r="D37" s="45">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>535</v>
-      </c>
-      <c r="B38" s="63">
-        <v>12</v>
-      </c>
-      <c r="C38" s="63">
-        <v>36</v>
-      </c>
-      <c r="D38" s="45">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>536</v>
-      </c>
-      <c r="B39" s="57">
-        <v>17</v>
-      </c>
-      <c r="C39" s="57">
-        <v>11</v>
-      </c>
-      <c r="D39" s="45">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>537</v>
-      </c>
-      <c r="B40" s="57">
-        <v>14</v>
-      </c>
-      <c r="C40" s="57">
-        <v>53</v>
-      </c>
-      <c r="D40" s="45">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>538</v>
-      </c>
-      <c r="B41" s="63">
-        <v>55</v>
-      </c>
-      <c r="C41" s="63">
-        <v>43</v>
-      </c>
-      <c r="D41" s="45">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>539</v>
-      </c>
-      <c r="B42" s="63">
-        <v>23</v>
-      </c>
-      <c r="C42" s="63">
-        <v>43</v>
-      </c>
-      <c r="D42" s="45">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>540</v>
-      </c>
-      <c r="B43" s="63">
-        <v>6</v>
-      </c>
-      <c r="C43" s="63">
-        <v>9</v>
-      </c>
-      <c r="D43" s="45">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>541</v>
-      </c>
-      <c r="B44" s="63">
-        <v>5</v>
-      </c>
-      <c r="C44" s="63">
-        <v>27</v>
-      </c>
-      <c r="D44" s="25"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="33" t="s">
-        <v>542</v>
-      </c>
-      <c r="B45" s="63">
-        <v>32</v>
-      </c>
-      <c r="C45" s="63">
-        <v>30</v>
-      </c>
-      <c r="D45" s="25"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="35" t="str">
-        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
-        <v>总时长：28:01:05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added notes for 16_Vue_scratch:L05: template and computed properties
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244248A5-E8CD-47CE-A1C6-01F721F660B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6976B761-C181-46E4-96AF-68225DA8621C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="13" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6695,7 +6695,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6785,13 +6785,15 @@
       <c r="A7" t="s">
         <v>587</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="57">
         <v>55</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="57">
         <v>51</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="45">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
added notes for 16_Vue_scratch:L06: Vue component essentials
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6976B761-C181-46E4-96AF-68225DA8621C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CC779D-5654-4040-B21C-0F2DF3098A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="13" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" firstSheet="13" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -6695,7 +6695,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6799,13 +6799,15 @@
       <c r="A8" t="s">
         <v>588</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="57">
         <v>58</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="57">
         <v>52</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="45">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
@@ -6817,25 +6819,29 @@
       <c r="A10" t="s">
         <v>589</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="57">
         <v>24</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="57">
         <v>38</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="45">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>590</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="57">
         <v>29</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="57">
         <v>51</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="45">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
added notes for 16_Vue_scratch:L12: Channel & ChannelList components
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CC779D-5654-4040-B21C-0F2DF3098A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD38B22-37DD-4A80-B1C6-F8634770F811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" firstSheet="13" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6695,7 +6695,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6847,37 +6847,43 @@
       <c r="A12" t="s">
         <v>591</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="57">
         <v>17</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="57">
         <v>57</v>
       </c>
-      <c r="D12" s="25"/>
+      <c r="D12" s="45">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>592</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="57">
         <v>20</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="57">
         <v>28</v>
       </c>
-      <c r="D13" s="25"/>
+      <c r="D13" s="45">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>593</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="57">
         <v>24</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="57">
         <v>21</v>
       </c>
-      <c r="D14" s="25"/>
+      <c r="D14" s="45">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
@@ -6889,25 +6895,29 @@
       <c r="A16" t="s">
         <v>594</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="63">
         <v>41</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="63">
         <v>7</v>
       </c>
-      <c r="D16" s="25"/>
+      <c r="D16" s="45">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>595</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="63">
         <v>20</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="63">
         <v>20</v>
       </c>
-      <c r="D17" s="25"/>
+      <c r="D17" s="45">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">

</xml_diff>

<commit_message>
added notes for 16_Vue_scratch:L15: Layout component
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5D08E8-F381-43F8-AF3B-C6DC16F88B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15228A4E-C8F2-41C0-9227-258D4B9FA169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" firstSheet="13" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6695,7 +6695,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6923,37 +6923,43 @@
       <c r="A18" t="s">
         <v>596</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="57">
         <v>46</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="57">
         <v>4</v>
       </c>
-      <c r="D18" s="25"/>
+      <c r="D18" s="45">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>597</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="63">
         <v>25</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="63">
         <v>25</v>
       </c>
-      <c r="D19" s="25"/>
+      <c r="D19" s="45">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>598</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="63">
         <v>10</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="63">
         <v>11</v>
       </c>
-      <c r="D20" s="25"/>
+      <c r="D20" s="45">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="37" t="str">

</xml_diff>

<commit_message>
Start Section 17: Webpack in Depth
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15228A4E-C8F2-41C0-9227-258D4B9FA169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7033DAB0-A842-4F9A-A8CF-A5922A74E820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" firstSheet="13" activeTab="16" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="17" activeTab="17" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -30,14 +30,14 @@
     <sheet name="15Build" sheetId="14" r:id="rId15"/>
     <sheet name="16Vue_intro" sheetId="15" r:id="rId16"/>
     <sheet name="17Vue_scratch" sheetId="19" r:id="rId17"/>
-    <sheet name="18Vue_comp" sheetId="16" r:id="rId18"/>
-    <sheet name="19Vue3" sheetId="23" r:id="rId19"/>
-    <sheet name="20Vue3_new" sheetId="24" r:id="rId20"/>
-    <sheet name="21Lowcode_proj" sheetId="25" r:id="rId21"/>
-    <sheet name="22Webpack" sheetId="21" r:id="rId22"/>
-    <sheet name="23Miniapp" sheetId="17" r:id="rId23"/>
-    <sheet name="24Echarts" sheetId="20" r:id="rId24"/>
-    <sheet name="25BPMN" sheetId="22" r:id="rId25"/>
+    <sheet name="18Webpack" sheetId="21" r:id="rId18"/>
+    <sheet name="19Vue_comp" sheetId="16" r:id="rId19"/>
+    <sheet name="Vue3" sheetId="23" r:id="rId20"/>
+    <sheet name="Vue3_new" sheetId="24" r:id="rId21"/>
+    <sheet name="Lowcode_proj" sheetId="25" r:id="rId22"/>
+    <sheet name="Miniapp" sheetId="17" r:id="rId23"/>
+    <sheet name="Echarts" sheetId="20" r:id="rId24"/>
+    <sheet name="BPMN" sheetId="22" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2773,6 +2773,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="hh:mm:ss"/>
+  </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3021,7 +3024,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3260,6 +3263,9 @@
       <alignment horizontal="left" vertical="center" indent="27"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6694,7 +6700,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -6975,6 +6981,997 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97C62C-B5D1-4E72-812F-7EA03DA117C7}">
+  <dimension ref="A1:F69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D63" sqref="D63:D68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="60" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>719</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>45</v>
+      </c>
+      <c r="D3" s="80">
+        <f t="shared" ref="D3:D21" si="0">B3/60/24+C3/3600/24</f>
+        <v>3.9930555555555552E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>51</v>
+      </c>
+      <c r="D4" s="80">
+        <f t="shared" si="0"/>
+        <v>2.975694444444444E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>655</v>
+      </c>
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>23</v>
+      </c>
+      <c r="D5" s="80">
+        <f t="shared" si="0"/>
+        <v>2.8738425925925924E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>656</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6" s="80">
+        <f t="shared" si="0"/>
+        <v>1.1238425925925926E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>657</v>
+      </c>
+      <c r="B7">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="D7" s="80">
+        <f t="shared" si="0"/>
+        <v>3.560185185185185E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>658</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="D8" s="80">
+        <f t="shared" si="0"/>
+        <v>2.8275462962962961E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>718</v>
+      </c>
+      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="80">
+        <f t="shared" si="0"/>
+        <v>1.4606481481481481E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>659</v>
+      </c>
+      <c r="B10">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>45</v>
+      </c>
+      <c r="D10" s="80">
+        <f t="shared" si="0"/>
+        <v>1.5104166666666665E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>660</v>
+      </c>
+      <c r="B11">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="80">
+        <f t="shared" si="0"/>
+        <v>2.6435185185185187E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>661</v>
+      </c>
+      <c r="B12">
+        <v>51</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="80">
+        <f t="shared" si="0"/>
+        <v>3.5416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>662</v>
+      </c>
+      <c r="B13">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>43</v>
+      </c>
+      <c r="D13" s="80">
+        <f t="shared" si="0"/>
+        <v>3.3831018518518517E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>663</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="D14" s="80">
+        <f t="shared" si="0"/>
+        <v>1.695601851851852E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>664</v>
+      </c>
+      <c r="B15">
+        <v>44</v>
+      </c>
+      <c r="C15">
+        <v>49</v>
+      </c>
+      <c r="D15" s="80">
+        <f t="shared" si="0"/>
+        <v>3.1122685185185184E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>665</v>
+      </c>
+      <c r="B16">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>47</v>
+      </c>
+      <c r="D16" s="80">
+        <f t="shared" si="0"/>
+        <v>1.5127314814814814E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>666</v>
+      </c>
+      <c r="B17">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>46</v>
+      </c>
+      <c r="D17" s="80">
+        <f t="shared" si="0"/>
+        <v>1.8587962962962966E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>667</v>
+      </c>
+      <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>55</v>
+      </c>
+      <c r="D18" s="80">
+        <f t="shared" si="0"/>
+        <v>1.7303240740740741E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>668</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>37</v>
+      </c>
+      <c r="D19" s="80">
+        <f t="shared" si="0"/>
+        <v>1.0150462962962964E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>669</v>
+      </c>
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>39</v>
+      </c>
+      <c r="D20" s="80">
+        <f t="shared" si="0"/>
+        <v>1.2256944444444444E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>670</v>
+      </c>
+      <c r="B21">
+        <v>68</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="80">
+        <f t="shared" si="0"/>
+        <v>4.7245370370370368E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="60" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>672</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23" s="80">
+        <f t="shared" ref="D23:D30" si="1">B23/60/24+C23/3600/24</f>
+        <v>6.3194444444444435E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>673</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" s="80">
+        <f t="shared" si="1"/>
+        <v>1.1157407407407408E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>674</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="80">
+        <f t="shared" si="1"/>
+        <v>4.8726851851851856E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>675</v>
+      </c>
+      <c r="B26">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>55</v>
+      </c>
+      <c r="D26" s="80">
+        <f t="shared" si="1"/>
+        <v>3.1192129629629629E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>676</v>
+      </c>
+      <c r="B27">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>21</v>
+      </c>
+      <c r="D27" s="80">
+        <f t="shared" si="1"/>
+        <v>2.5937500000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>677</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>14</v>
+      </c>
+      <c r="D28" s="80">
+        <f t="shared" si="1"/>
+        <v>1.8912037037037036E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>678</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" s="80">
+        <f t="shared" si="1"/>
+        <v>1.1168981481481481E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>679</v>
+      </c>
+      <c r="B30">
+        <v>47</v>
+      </c>
+      <c r="C30">
+        <v>31</v>
+      </c>
+      <c r="D30" s="80">
+        <f t="shared" si="1"/>
+        <v>3.2997685185185185E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="60" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>681</v>
+      </c>
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32" s="80">
+        <f t="shared" ref="D32:D41" si="2">B32/60/24+C32/3600/24</f>
+        <v>1.6805555555555556E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>682</v>
+      </c>
+      <c r="B33">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>54</v>
+      </c>
+      <c r="D33" s="80">
+        <f t="shared" si="2"/>
+        <v>2.0069444444444445E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>683</v>
+      </c>
+      <c r="B34">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>38</v>
+      </c>
+      <c r="D34" s="80">
+        <f t="shared" si="2"/>
+        <v>1.7106481481481483E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>684</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>57</v>
+      </c>
+      <c r="D35" s="80">
+        <f t="shared" si="2"/>
+        <v>1.1770833333333335E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>685</v>
+      </c>
+      <c r="B36">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>19</v>
+      </c>
+      <c r="D36" s="80">
+        <f t="shared" si="2"/>
+        <v>3.1469907407407405E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>686</v>
+      </c>
+      <c r="B37">
+        <v>52</v>
+      </c>
+      <c r="C37">
+        <v>26</v>
+      </c>
+      <c r="D37" s="80">
+        <f t="shared" si="2"/>
+        <v>3.6412037037037041E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>687</v>
+      </c>
+      <c r="B38">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>53</v>
+      </c>
+      <c r="D38" s="80">
+        <f t="shared" si="2"/>
+        <v>9.6412037037037039E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>688</v>
+      </c>
+      <c r="B39">
+        <v>69</v>
+      </c>
+      <c r="C39">
+        <v>24</v>
+      </c>
+      <c r="D39" s="80">
+        <f t="shared" si="2"/>
+        <v>4.8194444444444443E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>689</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40" s="80">
+        <f t="shared" si="2"/>
+        <v>9.8495370370370369E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>690</v>
+      </c>
+      <c r="B41">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+      <c r="D41" s="80">
+        <f t="shared" si="2"/>
+        <v>1.2094907407407407E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="60" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>692</v>
+      </c>
+      <c r="B43">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>39</v>
+      </c>
+      <c r="D43" s="80">
+        <f t="shared" ref="D43:D48" si="3">B43/60/24+C43/3600/24</f>
+        <v>8.7847222222222215E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>693</v>
+      </c>
+      <c r="B44">
+        <v>22</v>
+      </c>
+      <c r="C44">
+        <v>36</v>
+      </c>
+      <c r="D44" s="80">
+        <f t="shared" si="3"/>
+        <v>1.5694444444444445E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>694</v>
+      </c>
+      <c r="B45">
+        <v>24</v>
+      </c>
+      <c r="C45">
+        <v>54</v>
+      </c>
+      <c r="D45" s="80">
+        <f t="shared" si="3"/>
+        <v>1.7291666666666667E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>695</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>13</v>
+      </c>
+      <c r="D46" s="80">
+        <f t="shared" si="3"/>
+        <v>7.0949074074074074E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>696</v>
+      </c>
+      <c r="B47">
+        <v>31</v>
+      </c>
+      <c r="C47">
+        <v>29</v>
+      </c>
+      <c r="D47" s="80">
+        <f t="shared" si="3"/>
+        <v>2.1863425925925929E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>697</v>
+      </c>
+      <c r="B48">
+        <v>40</v>
+      </c>
+      <c r="C48">
+        <v>18</v>
+      </c>
+      <c r="D48" s="80">
+        <f t="shared" si="3"/>
+        <v>2.7986111111111111E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="60" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>699</v>
+      </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>51</v>
+      </c>
+      <c r="D50" s="80">
+        <f t="shared" ref="D50:D61" si="4">B50/60/24+C50/3600/24</f>
+        <v>1.1006944444444444E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>700</v>
+      </c>
+      <c r="B51">
+        <v>23</v>
+      </c>
+      <c r="C51">
+        <v>17</v>
+      </c>
+      <c r="D51" s="80">
+        <f t="shared" si="4"/>
+        <v>1.6168981481481482E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>701</v>
+      </c>
+      <c r="B52">
+        <v>33</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="80">
+        <f t="shared" si="4"/>
+        <v>2.2939814814814816E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>702</v>
+      </c>
+      <c r="B53">
+        <v>22</v>
+      </c>
+      <c r="C53">
+        <v>54</v>
+      </c>
+      <c r="D53" s="80">
+        <f t="shared" si="4"/>
+        <v>1.5902777777777776E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>703</v>
+      </c>
+      <c r="B54">
+        <v>45</v>
+      </c>
+      <c r="C54">
+        <v>24</v>
+      </c>
+      <c r="D54" s="80">
+        <f t="shared" si="4"/>
+        <v>3.152777777777778E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>704</v>
+      </c>
+      <c r="B55">
+        <v>51</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55" s="80">
+        <f t="shared" si="4"/>
+        <v>3.546296296296296E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>705</v>
+      </c>
+      <c r="B56">
+        <v>32</v>
+      </c>
+      <c r="C56">
+        <v>55</v>
+      </c>
+      <c r="D56" s="80">
+        <f t="shared" si="4"/>
+        <v>2.2858796296296297E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>706</v>
+      </c>
+      <c r="B57">
+        <v>54</v>
+      </c>
+      <c r="C57">
+        <v>40</v>
+      </c>
+      <c r="D57" s="80">
+        <f t="shared" si="4"/>
+        <v>3.7962962962962962E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>707</v>
+      </c>
+      <c r="B58">
+        <v>11</v>
+      </c>
+      <c r="C58">
+        <v>16</v>
+      </c>
+      <c r="D58" s="80">
+        <f t="shared" si="4"/>
+        <v>7.8240740740740736E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>708</v>
+      </c>
+      <c r="B59">
+        <v>31</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" s="80">
+        <f t="shared" si="4"/>
+        <v>2.1539351851851855E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>709</v>
+      </c>
+      <c r="B60">
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>14</v>
+      </c>
+      <c r="D60" s="80">
+        <f t="shared" si="4"/>
+        <v>8.4953703703703701E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>710</v>
+      </c>
+      <c r="B61">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>47</v>
+      </c>
+      <c r="D61" s="80">
+        <f t="shared" si="4"/>
+        <v>9.5717592592592608E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="60" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>712</v>
+      </c>
+      <c r="B63">
+        <v>24</v>
+      </c>
+      <c r="C63">
+        <v>30</v>
+      </c>
+      <c r="D63" s="80">
+        <f t="shared" ref="D63:D68" si="5">B63/60/24+C63/3600/24</f>
+        <v>1.7013888888888887E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>713</v>
+      </c>
+      <c r="B64">
+        <v>19</v>
+      </c>
+      <c r="C64">
+        <v>53</v>
+      </c>
+      <c r="D64" s="80">
+        <f t="shared" si="5"/>
+        <v>1.380787037037037E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>714</v>
+      </c>
+      <c r="B65">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <v>30</v>
+      </c>
+      <c r="D65" s="80">
+        <f t="shared" si="5"/>
+        <v>6.5972222222222213E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>715</v>
+      </c>
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <v>14</v>
+      </c>
+      <c r="D66" s="80">
+        <f t="shared" si="5"/>
+        <v>4.3287037037037035E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>716</v>
+      </c>
+      <c r="B67">
+        <v>16</v>
+      </c>
+      <c r="C67">
+        <v>57</v>
+      </c>
+      <c r="D67" s="80">
+        <f t="shared" si="5"/>
+        <v>1.1770833333333335E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>717</v>
+      </c>
+      <c r="B68">
+        <v>14</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" s="80">
+        <f t="shared" si="5"/>
+        <v>9.7685185185185184E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="69" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：28:35:01</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE55571-67F4-430B-911B-F444D39A2E21}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:F37"/>
@@ -7379,292 +8376,6 @@
       <c r="A37" s="11" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：16:30:44</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC8EE39-FEF0-4DE1-BCE0-97DA15E5D3E9}">
-  <dimension ref="A1:F25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="47.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>742</v>
-      </c>
-      <c r="B3">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>743</v>
-      </c>
-      <c r="B4">
-        <v>39</v>
-      </c>
-      <c r="C4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>744</v>
-      </c>
-      <c r="B5">
-        <v>34</v>
-      </c>
-      <c r="C5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>745</v>
-      </c>
-      <c r="B6">
-        <v>35</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
-        <v>746</v>
-      </c>
-      <c r="B7">
-        <v>25</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="36" t="s">
-        <v>747</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="64" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>749</v>
-      </c>
-      <c r="B10">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>750</v>
-      </c>
-      <c r="B11">
-        <v>23</v>
-      </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>751</v>
-      </c>
-      <c r="B12">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>752</v>
-      </c>
-      <c r="B13">
-        <v>46</v>
-      </c>
-      <c r="C13">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>753</v>
-      </c>
-      <c r="B14">
-        <v>41</v>
-      </c>
-      <c r="C14">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>754</v>
-      </c>
-      <c r="B15">
-        <v>67</v>
-      </c>
-      <c r="C15">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>755</v>
-      </c>
-      <c r="B16">
-        <v>65</v>
-      </c>
-      <c r="C16">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>756</v>
-      </c>
-      <c r="B17">
-        <v>64</v>
-      </c>
-      <c r="C17">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>757</v>
-      </c>
-      <c r="B18">
-        <v>27</v>
-      </c>
-      <c r="C18">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>758</v>
-      </c>
-      <c r="B19">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>759</v>
-      </c>
-      <c r="B20">
-        <v>41</v>
-      </c>
-      <c r="C20">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>760</v>
-      </c>
-      <c r="B21">
-        <v>42</v>
-      </c>
-      <c r="C21">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>761</v>
-      </c>
-      <c r="B22">
-        <v>38</v>
-      </c>
-      <c r="C22">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>762</v>
-      </c>
-      <c r="B23">
-        <v>64</v>
-      </c>
-      <c r="C23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>763</v>
-      </c>
-      <c r="B24">
-        <v>35</v>
-      </c>
-      <c r="C24">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="str">
-        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
-        <v>总时长：13:06:04</v>
       </c>
     </row>
   </sheetData>
@@ -8601,6 +9312,292 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC8EE39-FEF0-4DE1-BCE0-97DA15E5D3E9}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>742</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>743</v>
+      </c>
+      <c r="B4">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>744</v>
+      </c>
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>745</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
+        <v>746</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
+        <v>747</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="64" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>749</v>
+      </c>
+      <c r="B10">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>750</v>
+      </c>
+      <c r="B11">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>751</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>752</v>
+      </c>
+      <c r="B13">
+        <v>46</v>
+      </c>
+      <c r="C13">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>753</v>
+      </c>
+      <c r="B14">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>754</v>
+      </c>
+      <c r="B15">
+        <v>67</v>
+      </c>
+      <c r="C15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>755</v>
+      </c>
+      <c r="B16">
+        <v>65</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>756</v>
+      </c>
+      <c r="B17">
+        <v>64</v>
+      </c>
+      <c r="C17">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>757</v>
+      </c>
+      <c r="B18">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>758</v>
+      </c>
+      <c r="B19">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>759</v>
+      </c>
+      <c r="B20">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>760</v>
+      </c>
+      <c r="B21">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>761</v>
+      </c>
+      <c r="B22">
+        <v>38</v>
+      </c>
+      <c r="C22">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>762</v>
+      </c>
+      <c r="B23">
+        <v>64</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>763</v>
+      </c>
+      <c r="B24">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="str">
+        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
+        <v>总时长：13:06:04</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6EF9A4-06A0-4B42-AB44-860D68BC6616}">
   <dimension ref="A1:F103"/>
   <sheetViews>
@@ -9732,7 +10729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08238647-BBF6-4C2C-B188-33145A4D65D9}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -10011,753 +11008,6 @@
       <c r="A24" s="11" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：15:45:35</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97C62C-B5D1-4E72-812F-7EA03DA117C7}">
-  <dimension ref="A1:F69"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E56" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>719</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>654</v>
-      </c>
-      <c r="B4">
-        <v>42</v>
-      </c>
-      <c r="C4">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>655</v>
-      </c>
-      <c r="B5">
-        <v>41</v>
-      </c>
-      <c r="C5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>656</v>
-      </c>
-      <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>657</v>
-      </c>
-      <c r="B7">
-        <v>51</v>
-      </c>
-      <c r="C7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>658</v>
-      </c>
-      <c r="B8">
-        <v>40</v>
-      </c>
-      <c r="C8">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>718</v>
-      </c>
-      <c r="B9">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>659</v>
-      </c>
-      <c r="B10">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>660</v>
-      </c>
-      <c r="B11">
-        <v>38</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>661</v>
-      </c>
-      <c r="B12">
-        <v>51</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>662</v>
-      </c>
-      <c r="B13">
-        <v>48</v>
-      </c>
-      <c r="C13">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>663</v>
-      </c>
-      <c r="B14">
-        <v>24</v>
-      </c>
-      <c r="C14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>664</v>
-      </c>
-      <c r="B15">
-        <v>44</v>
-      </c>
-      <c r="C15">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>665</v>
-      </c>
-      <c r="B16">
-        <v>21</v>
-      </c>
-      <c r="C16">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>666</v>
-      </c>
-      <c r="B17">
-        <v>26</v>
-      </c>
-      <c r="C17">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>667</v>
-      </c>
-      <c r="B18">
-        <v>24</v>
-      </c>
-      <c r="C18">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>668</v>
-      </c>
-      <c r="B19">
-        <v>14</v>
-      </c>
-      <c r="C19">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>669</v>
-      </c>
-      <c r="B20">
-        <v>17</v>
-      </c>
-      <c r="C20">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>670</v>
-      </c>
-      <c r="B21">
-        <v>68</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="60" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>672</v>
-      </c>
-      <c r="B23">
-        <v>9</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>673</v>
-      </c>
-      <c r="B24">
-        <v>16</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>674</v>
-      </c>
-      <c r="B25">
-        <v>7</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>675</v>
-      </c>
-      <c r="B26">
-        <v>44</v>
-      </c>
-      <c r="C26">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>676</v>
-      </c>
-      <c r="B27">
-        <v>37</v>
-      </c>
-      <c r="C27">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>677</v>
-      </c>
-      <c r="B28">
-        <v>27</v>
-      </c>
-      <c r="C28">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>678</v>
-      </c>
-      <c r="B29">
-        <v>16</v>
-      </c>
-      <c r="C29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>679</v>
-      </c>
-      <c r="B30">
-        <v>47</v>
-      </c>
-      <c r="C30">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="60" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>681</v>
-      </c>
-      <c r="B32">
-        <v>24</v>
-      </c>
-      <c r="C32">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>682</v>
-      </c>
-      <c r="B33">
-        <v>28</v>
-      </c>
-      <c r="C33">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>683</v>
-      </c>
-      <c r="B34">
-        <v>24</v>
-      </c>
-      <c r="C34">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>684</v>
-      </c>
-      <c r="B35">
-        <v>16</v>
-      </c>
-      <c r="C35">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>685</v>
-      </c>
-      <c r="B36">
-        <v>45</v>
-      </c>
-      <c r="C36">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>686</v>
-      </c>
-      <c r="B37">
-        <v>52</v>
-      </c>
-      <c r="C37">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>687</v>
-      </c>
-      <c r="B38">
-        <v>13</v>
-      </c>
-      <c r="C38">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>688</v>
-      </c>
-      <c r="B39">
-        <v>69</v>
-      </c>
-      <c r="C39">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>689</v>
-      </c>
-      <c r="B40">
-        <v>14</v>
-      </c>
-      <c r="C40">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>690</v>
-      </c>
-      <c r="B41">
-        <v>17</v>
-      </c>
-      <c r="C41">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="60" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>692</v>
-      </c>
-      <c r="B43">
-        <v>12</v>
-      </c>
-      <c r="C43">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>693</v>
-      </c>
-      <c r="B44">
-        <v>22</v>
-      </c>
-      <c r="C44">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>694</v>
-      </c>
-      <c r="B45">
-        <v>24</v>
-      </c>
-      <c r="C45">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>695</v>
-      </c>
-      <c r="B46">
-        <v>10</v>
-      </c>
-      <c r="C46">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>696</v>
-      </c>
-      <c r="B47">
-        <v>31</v>
-      </c>
-      <c r="C47">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>697</v>
-      </c>
-      <c r="B48">
-        <v>40</v>
-      </c>
-      <c r="C48">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="60" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>699</v>
-      </c>
-      <c r="B50">
-        <v>15</v>
-      </c>
-      <c r="C50">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>700</v>
-      </c>
-      <c r="B51">
-        <v>23</v>
-      </c>
-      <c r="C51">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>701</v>
-      </c>
-      <c r="B52">
-        <v>33</v>
-      </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>702</v>
-      </c>
-      <c r="B53">
-        <v>22</v>
-      </c>
-      <c r="C53">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>703</v>
-      </c>
-      <c r="B54">
-        <v>45</v>
-      </c>
-      <c r="C54">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>704</v>
-      </c>
-      <c r="B55">
-        <v>51</v>
-      </c>
-      <c r="C55">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>705</v>
-      </c>
-      <c r="B56">
-        <v>32</v>
-      </c>
-      <c r="C56">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>706</v>
-      </c>
-      <c r="B57">
-        <v>54</v>
-      </c>
-      <c r="C57">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>707</v>
-      </c>
-      <c r="B58">
-        <v>11</v>
-      </c>
-      <c r="C58">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>708</v>
-      </c>
-      <c r="B59">
-        <v>31</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>709</v>
-      </c>
-      <c r="B60">
-        <v>12</v>
-      </c>
-      <c r="C60">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>710</v>
-      </c>
-      <c r="B61">
-        <v>13</v>
-      </c>
-      <c r="C61">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="60" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>712</v>
-      </c>
-      <c r="B63">
-        <v>24</v>
-      </c>
-      <c r="C63">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>713</v>
-      </c>
-      <c r="B64">
-        <v>19</v>
-      </c>
-      <c r="C64">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>714</v>
-      </c>
-      <c r="B65">
-        <v>9</v>
-      </c>
-      <c r="C65">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>715</v>
-      </c>
-      <c r="B66">
-        <v>6</v>
-      </c>
-      <c r="C66">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>716</v>
-      </c>
-      <c r="B67">
-        <v>16</v>
-      </c>
-      <c r="C67">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>717</v>
-      </c>
-      <c r="B68">
-        <v>14</v>
-      </c>
-      <c r="C68">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="69" t="str">
-        <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
-        <v>总时长：28:35:01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added notes for 17_Webpack:L02: Webpack installation
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7033DAB0-A842-4F9A-A8CF-A5922A74E820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6C9117-2E60-408F-9728-96E6F318F425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="17" activeTab="17" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="893">
   <si>
     <t>1. 环境准备</t>
   </si>
@@ -2767,6 +2767,10 @@
   </si>
   <si>
     <t>Echarts详细版 - 陈学辉</t>
+  </si>
+  <si>
+    <t>Duration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6982,22 +6986,23 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97C62C-B5D1-4E72-812F-7EA03DA117C7}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D63" sqref="D63:D68"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.375" customWidth="1"/>
+    <col min="5" max="5" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
@@ -7008,18 +7013,21 @@
         <v>37</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>892</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>889</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="60" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>719</v>
       </c>
@@ -7030,11 +7038,14 @@
         <v>45</v>
       </c>
       <c r="D3" s="80">
-        <f t="shared" ref="D3:D21" si="0">B3/60/24+C3/3600/24</f>
+        <f>B3/60/24+C3/3600/24</f>
         <v>3.9930555555555552E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>654</v>
       </c>
@@ -7045,11 +7056,14 @@
         <v>51</v>
       </c>
       <c r="D4" s="80">
-        <f t="shared" si="0"/>
+        <f>B4/60/24+C4/3600/24</f>
         <v>2.975694444444444E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>655</v>
       </c>
@@ -7060,11 +7074,14 @@
         <v>23</v>
       </c>
       <c r="D5" s="80">
-        <f t="shared" si="0"/>
+        <f>B5/60/24+C5/3600/24</f>
         <v>2.8738425925925924E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>656</v>
       </c>
@@ -7075,11 +7092,14 @@
         <v>11</v>
       </c>
       <c r="D6" s="80">
-        <f t="shared" si="0"/>
+        <f>B6/60/24+C6/3600/24</f>
         <v>1.1238425925925926E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>657</v>
       </c>
@@ -7090,11 +7110,14 @@
         <v>16</v>
       </c>
       <c r="D7" s="80">
-        <f t="shared" si="0"/>
+        <f>B7/60/24+C7/3600/24</f>
         <v>3.560185185185185E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>658</v>
       </c>
@@ -7105,11 +7128,14 @@
         <v>43</v>
       </c>
       <c r="D8" s="80">
-        <f t="shared" si="0"/>
+        <f>B8/60/24+C8/3600/24</f>
         <v>2.8275462962962961E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>718</v>
       </c>
@@ -7120,11 +7146,14 @@
         <v>2</v>
       </c>
       <c r="D9" s="80">
-        <f t="shared" si="0"/>
+        <f>B9/60/24+C9/3600/24</f>
         <v>1.4606481481481481E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E9" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>659</v>
       </c>
@@ -7135,11 +7164,12 @@
         <v>45</v>
       </c>
       <c r="D10" s="80">
-        <f t="shared" si="0"/>
+        <f>B10/60/24+C10/3600/24</f>
         <v>1.5104166666666665E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>660</v>
       </c>
@@ -7150,11 +7180,12 @@
         <v>4</v>
       </c>
       <c r="D11" s="80">
-        <f t="shared" si="0"/>
+        <f>B11/60/24+C11/3600/24</f>
         <v>2.6435185185185187E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>661</v>
       </c>
@@ -7165,11 +7196,12 @@
         <v>0</v>
       </c>
       <c r="D12" s="80">
-        <f t="shared" si="0"/>
+        <f>B12/60/24+C12/3600/24</f>
         <v>3.5416666666666666E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>662</v>
       </c>
@@ -7180,11 +7212,12 @@
         <v>43</v>
       </c>
       <c r="D13" s="80">
-        <f t="shared" si="0"/>
+        <f>B13/60/24+C13/3600/24</f>
         <v>3.3831018518518517E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>663</v>
       </c>
@@ -7195,11 +7228,12 @@
         <v>25</v>
       </c>
       <c r="D14" s="80">
-        <f t="shared" si="0"/>
+        <f>B14/60/24+C14/3600/24</f>
         <v>1.695601851851852E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>664</v>
       </c>
@@ -7210,11 +7244,12 @@
         <v>49</v>
       </c>
       <c r="D15" s="80">
-        <f t="shared" si="0"/>
+        <f>B15/60/24+C15/3600/24</f>
         <v>3.1122685185185184E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>665</v>
       </c>
@@ -7225,11 +7260,12 @@
         <v>47</v>
       </c>
       <c r="D16" s="80">
-        <f t="shared" si="0"/>
+        <f>B16/60/24+C16/3600/24</f>
         <v>1.5127314814814814E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>666</v>
       </c>
@@ -7240,11 +7276,12 @@
         <v>46</v>
       </c>
       <c r="D17" s="80">
-        <f t="shared" si="0"/>
+        <f>B17/60/24+C17/3600/24</f>
         <v>1.8587962962962966E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>667</v>
       </c>
@@ -7255,11 +7292,12 @@
         <v>55</v>
       </c>
       <c r="D18" s="80">
-        <f t="shared" si="0"/>
+        <f>B18/60/24+C18/3600/24</f>
         <v>1.7303240740740741E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="25"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>668</v>
       </c>
@@ -7270,11 +7308,12 @@
         <v>37</v>
       </c>
       <c r="D19" s="80">
-        <f t="shared" si="0"/>
+        <f>B19/60/24+C19/3600/24</f>
         <v>1.0150462962962964E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>669</v>
       </c>
@@ -7285,11 +7324,12 @@
         <v>39</v>
       </c>
       <c r="D20" s="80">
-        <f t="shared" si="0"/>
+        <f>B20/60/24+C20/3600/24</f>
         <v>1.2256944444444444E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="25"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>670</v>
       </c>
@@ -7300,16 +7340,18 @@
         <v>2</v>
       </c>
       <c r="D21" s="80">
-        <f t="shared" si="0"/>
+        <f>B21/60/24+C21/3600/24</f>
         <v>4.7245370370370368E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="25"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="60" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="25"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>672</v>
       </c>
@@ -7320,11 +7362,12 @@
         <v>6</v>
       </c>
       <c r="D23" s="80">
-        <f t="shared" ref="D23:D30" si="1">B23/60/24+C23/3600/24</f>
+        <f>B23/60/24+C23/3600/24</f>
         <v>6.3194444444444435E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="25"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>673</v>
       </c>
@@ -7335,11 +7378,12 @@
         <v>4</v>
       </c>
       <c r="D24" s="80">
-        <f t="shared" si="1"/>
+        <f>B24/60/24+C24/3600/24</f>
         <v>1.1157407407407408E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="25"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>674</v>
       </c>
@@ -7350,11 +7394,12 @@
         <v>1</v>
       </c>
       <c r="D25" s="80">
-        <f t="shared" si="1"/>
+        <f>B25/60/24+C25/3600/24</f>
         <v>4.8726851851851856E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="25"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>675</v>
       </c>
@@ -7365,11 +7410,12 @@
         <v>55</v>
       </c>
       <c r="D26" s="80">
-        <f t="shared" si="1"/>
+        <f>B26/60/24+C26/3600/24</f>
         <v>3.1192129629629629E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="25"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>676</v>
       </c>
@@ -7380,11 +7426,12 @@
         <v>21</v>
       </c>
       <c r="D27" s="80">
-        <f t="shared" si="1"/>
+        <f>B27/60/24+C27/3600/24</f>
         <v>2.5937500000000002E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="25"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>677</v>
       </c>
@@ -7395,11 +7442,12 @@
         <v>14</v>
       </c>
       <c r="D28" s="80">
-        <f t="shared" si="1"/>
+        <f>B28/60/24+C28/3600/24</f>
         <v>1.8912037037037036E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="25"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>678</v>
       </c>
@@ -7410,11 +7458,12 @@
         <v>5</v>
       </c>
       <c r="D29" s="80">
-        <f t="shared" si="1"/>
+        <f>B29/60/24+C29/3600/24</f>
         <v>1.1168981481481481E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="25"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>679</v>
       </c>
@@ -7425,16 +7474,18 @@
         <v>31</v>
       </c>
       <c r="D30" s="80">
-        <f t="shared" si="1"/>
+        <f>B30/60/24+C30/3600/24</f>
         <v>3.2997685185185185E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="25"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="60" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="25"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>681</v>
       </c>
@@ -7445,11 +7496,12 @@
         <v>12</v>
       </c>
       <c r="D32" s="80">
-        <f t="shared" ref="D32:D41" si="2">B32/60/24+C32/3600/24</f>
+        <f>B32/60/24+C32/3600/24</f>
         <v>1.6805555555555556E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="25"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>682</v>
       </c>
@@ -7460,11 +7512,12 @@
         <v>54</v>
       </c>
       <c r="D33" s="80">
-        <f t="shared" si="2"/>
+        <f>B33/60/24+C33/3600/24</f>
         <v>2.0069444444444445E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="25"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>683</v>
       </c>
@@ -7475,11 +7528,12 @@
         <v>38</v>
       </c>
       <c r="D34" s="80">
-        <f t="shared" si="2"/>
+        <f>B34/60/24+C34/3600/24</f>
         <v>1.7106481481481483E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="25"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>684</v>
       </c>
@@ -7490,11 +7544,12 @@
         <v>57</v>
       </c>
       <c r="D35" s="80">
-        <f t="shared" si="2"/>
+        <f>B35/60/24+C35/3600/24</f>
         <v>1.1770833333333335E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="25"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>685</v>
       </c>
@@ -7505,11 +7560,12 @@
         <v>19</v>
       </c>
       <c r="D36" s="80">
-        <f t="shared" si="2"/>
+        <f>B36/60/24+C36/3600/24</f>
         <v>3.1469907407407405E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="25"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>686</v>
       </c>
@@ -7520,11 +7576,12 @@
         <v>26</v>
       </c>
       <c r="D37" s="80">
-        <f t="shared" si="2"/>
+        <f>B37/60/24+C37/3600/24</f>
         <v>3.6412037037037041E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="25"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>687</v>
       </c>
@@ -7535,11 +7592,12 @@
         <v>53</v>
       </c>
       <c r="D38" s="80">
-        <f t="shared" si="2"/>
+        <f>B38/60/24+C38/3600/24</f>
         <v>9.6412037037037039E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="25"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>688</v>
       </c>
@@ -7550,11 +7608,12 @@
         <v>24</v>
       </c>
       <c r="D39" s="80">
-        <f t="shared" si="2"/>
+        <f>B39/60/24+C39/3600/24</f>
         <v>4.8194444444444443E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="25"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>689</v>
       </c>
@@ -7565,11 +7624,12 @@
         <v>11</v>
       </c>
       <c r="D40" s="80">
-        <f t="shared" si="2"/>
+        <f>B40/60/24+C40/3600/24</f>
         <v>9.8495370370370369E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="25"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>690</v>
       </c>
@@ -7580,16 +7640,18 @@
         <v>25</v>
       </c>
       <c r="D41" s="80">
-        <f t="shared" si="2"/>
+        <f>B41/60/24+C41/3600/24</f>
         <v>1.2094907407407407E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="25"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="25"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>692</v>
       </c>
@@ -7600,11 +7662,12 @@
         <v>39</v>
       </c>
       <c r="D43" s="80">
-        <f t="shared" ref="D43:D48" si="3">B43/60/24+C43/3600/24</f>
+        <f>B43/60/24+C43/3600/24</f>
         <v>8.7847222222222215E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="25"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>693</v>
       </c>
@@ -7615,11 +7678,12 @@
         <v>36</v>
       </c>
       <c r="D44" s="80">
-        <f t="shared" si="3"/>
+        <f>B44/60/24+C44/3600/24</f>
         <v>1.5694444444444445E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="25"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>694</v>
       </c>
@@ -7630,11 +7694,12 @@
         <v>54</v>
       </c>
       <c r="D45" s="80">
-        <f t="shared" si="3"/>
+        <f>B45/60/24+C45/3600/24</f>
         <v>1.7291666666666667E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="25"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>695</v>
       </c>
@@ -7645,11 +7710,12 @@
         <v>13</v>
       </c>
       <c r="D46" s="80">
-        <f t="shared" si="3"/>
+        <f>B46/60/24+C46/3600/24</f>
         <v>7.0949074074074074E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="25"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>696</v>
       </c>
@@ -7660,11 +7726,12 @@
         <v>29</v>
       </c>
       <c r="D47" s="80">
-        <f t="shared" si="3"/>
+        <f>B47/60/24+C47/3600/24</f>
         <v>2.1863425925925929E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="25"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>697</v>
       </c>
@@ -7675,16 +7742,18 @@
         <v>18</v>
       </c>
       <c r="D48" s="80">
-        <f t="shared" si="3"/>
+        <f>B48/60/24+C48/3600/24</f>
         <v>2.7986111111111111E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="25"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="60" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="25"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>699</v>
       </c>
@@ -7695,11 +7764,12 @@
         <v>51</v>
       </c>
       <c r="D50" s="80">
-        <f t="shared" ref="D50:D61" si="4">B50/60/24+C50/3600/24</f>
+        <f>B50/60/24+C50/3600/24</f>
         <v>1.1006944444444444E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="25"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>700</v>
       </c>
@@ -7710,11 +7780,12 @@
         <v>17</v>
       </c>
       <c r="D51" s="80">
-        <f t="shared" si="4"/>
+        <f>B51/60/24+C51/3600/24</f>
         <v>1.6168981481481482E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="25"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>701</v>
       </c>
@@ -7725,11 +7796,12 @@
         <v>2</v>
       </c>
       <c r="D52" s="80">
-        <f t="shared" si="4"/>
+        <f>B52/60/24+C52/3600/24</f>
         <v>2.2939814814814816E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="25"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>702</v>
       </c>
@@ -7740,11 +7812,12 @@
         <v>54</v>
       </c>
       <c r="D53" s="80">
-        <f t="shared" si="4"/>
+        <f>B53/60/24+C53/3600/24</f>
         <v>1.5902777777777776E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="25"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>703</v>
       </c>
@@ -7755,11 +7828,12 @@
         <v>24</v>
       </c>
       <c r="D54" s="80">
-        <f t="shared" si="4"/>
+        <f>B54/60/24+C54/3600/24</f>
         <v>3.152777777777778E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="25"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>704</v>
       </c>
@@ -7770,11 +7844,12 @@
         <v>4</v>
       </c>
       <c r="D55" s="80">
-        <f t="shared" si="4"/>
+        <f>B55/60/24+C55/3600/24</f>
         <v>3.546296296296296E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="25"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>705</v>
       </c>
@@ -7785,11 +7860,12 @@
         <v>55</v>
       </c>
       <c r="D56" s="80">
-        <f t="shared" si="4"/>
+        <f>B56/60/24+C56/3600/24</f>
         <v>2.2858796296296297E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="25"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>706</v>
       </c>
@@ -7800,11 +7876,12 @@
         <v>40</v>
       </c>
       <c r="D57" s="80">
-        <f t="shared" si="4"/>
+        <f>B57/60/24+C57/3600/24</f>
         <v>3.7962962962962962E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="25"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>707</v>
       </c>
@@ -7815,11 +7892,12 @@
         <v>16</v>
       </c>
       <c r="D58" s="80">
-        <f t="shared" si="4"/>
+        <f>B58/60/24+C58/3600/24</f>
         <v>7.8240740740740736E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="25"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>708</v>
       </c>
@@ -7830,11 +7908,12 @@
         <v>1</v>
       </c>
       <c r="D59" s="80">
-        <f t="shared" si="4"/>
+        <f>B59/60/24+C59/3600/24</f>
         <v>2.1539351851851855E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="25"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>709</v>
       </c>
@@ -7845,11 +7924,12 @@
         <v>14</v>
       </c>
       <c r="D60" s="80">
-        <f t="shared" si="4"/>
+        <f>B60/60/24+C60/3600/24</f>
         <v>8.4953703703703701E-3</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="25"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>710</v>
       </c>
@@ -7860,16 +7940,18 @@
         <v>47</v>
       </c>
       <c r="D61" s="80">
-        <f t="shared" si="4"/>
+        <f>B61/60/24+C61/3600/24</f>
         <v>9.5717592592592608E-3</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="25"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="60" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="25"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>712</v>
       </c>
@@ -7880,11 +7962,12 @@
         <v>30</v>
       </c>
       <c r="D63" s="80">
-        <f t="shared" ref="D63:D68" si="5">B63/60/24+C63/3600/24</f>
+        <f>B63/60/24+C63/3600/24</f>
         <v>1.7013888888888887E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="25"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>713</v>
       </c>
@@ -7895,11 +7978,12 @@
         <v>53</v>
       </c>
       <c r="D64" s="80">
-        <f t="shared" si="5"/>
+        <f>B64/60/24+C64/3600/24</f>
         <v>1.380787037037037E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="25"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>714</v>
       </c>
@@ -7910,11 +7994,12 @@
         <v>30</v>
       </c>
       <c r="D65" s="80">
-        <f t="shared" si="5"/>
+        <f>B65/60/24+C65/3600/24</f>
         <v>6.5972222222222213E-3</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="25"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>715</v>
       </c>
@@ -7925,11 +8010,12 @@
         <v>14</v>
       </c>
       <c r="D66" s="80">
-        <f t="shared" si="5"/>
+        <f>B66/60/24+C66/3600/24</f>
         <v>4.3287037037037035E-3</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" s="25"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>716</v>
       </c>
@@ -7940,11 +8026,12 @@
         <v>57</v>
       </c>
       <c r="D67" s="80">
-        <f t="shared" si="5"/>
+        <f>B67/60/24+C67/3600/24</f>
         <v>1.1770833333333335E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="25"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>717</v>
       </c>
@@ -7955,11 +8042,12 @@
         <v>4</v>
       </c>
       <c r="D68" s="80">
-        <f t="shared" si="5"/>
+        <f>B68/60/24+C68/3600/24</f>
         <v>9.7685185185185184E-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="25"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="69" t="str">
         <f>"总时长："&amp;TEXT(SUM(B:B)/1440+SUM(C:C)/86400,"[h]:mm:ss")</f>
         <v>总时长：28:35:01</v>

</xml_diff>

<commit_message>
updated progress for 17_Webpack
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6C9117-2E60-408F-9728-96E6F318F425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9958867-51A0-41A6-9E02-A2FFA94D03E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="17" activeTab="17" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6992,7 +6992,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7038,7 +7038,7 @@
         <v>45</v>
       </c>
       <c r="D3" s="80">
-        <f>B3/60/24+C3/3600/24</f>
+        <f t="shared" ref="D3:D21" si="0">B3/60/24+C3/3600/24</f>
         <v>3.9930555555555552E-3</v>
       </c>
       <c r="E3" s="25">
@@ -7056,7 +7056,7 @@
         <v>51</v>
       </c>
       <c r="D4" s="80">
-        <f>B4/60/24+C4/3600/24</f>
+        <f t="shared" si="0"/>
         <v>2.975694444444444E-2</v>
       </c>
       <c r="E4" s="25">
@@ -7074,7 +7074,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="80">
-        <f>B5/60/24+C5/3600/24</f>
+        <f t="shared" si="0"/>
         <v>2.8738425925925924E-2</v>
       </c>
       <c r="E5" s="25">
@@ -7092,7 +7092,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="80">
-        <f>B6/60/24+C6/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.1238425925925926E-2</v>
       </c>
       <c r="E6" s="25">
@@ -7110,11 +7110,11 @@
         <v>16</v>
       </c>
       <c r="D7" s="80">
-        <f>B7/60/24+C7/3600/24</f>
+        <f t="shared" si="0"/>
         <v>3.560185185185185E-2</v>
       </c>
       <c r="E7" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7128,11 +7128,11 @@
         <v>43</v>
       </c>
       <c r="D8" s="80">
-        <f>B8/60/24+C8/3600/24</f>
+        <f t="shared" si="0"/>
         <v>2.8275462962962961E-2</v>
       </c>
       <c r="E8" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -7146,11 +7146,11 @@
         <v>2</v>
       </c>
       <c r="D9" s="80">
-        <f>B9/60/24+C9/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.4606481481481481E-2</v>
       </c>
       <c r="E9" s="25">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7164,7 +7164,7 @@
         <v>45</v>
       </c>
       <c r="D10" s="80">
-        <f>B10/60/24+C10/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.5104166666666665E-2</v>
       </c>
       <c r="E10" s="25"/>
@@ -7180,7 +7180,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="80">
-        <f>B11/60/24+C11/3600/24</f>
+        <f t="shared" si="0"/>
         <v>2.6435185185185187E-2</v>
       </c>
       <c r="E11" s="25"/>
@@ -7196,7 +7196,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="80">
-        <f>B12/60/24+C12/3600/24</f>
+        <f t="shared" si="0"/>
         <v>3.5416666666666666E-2</v>
       </c>
       <c r="E12" s="25"/>
@@ -7212,7 +7212,7 @@
         <v>43</v>
       </c>
       <c r="D13" s="80">
-        <f>B13/60/24+C13/3600/24</f>
+        <f t="shared" si="0"/>
         <v>3.3831018518518517E-2</v>
       </c>
       <c r="E13" s="25"/>
@@ -7228,7 +7228,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="80">
-        <f>B14/60/24+C14/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.695601851851852E-2</v>
       </c>
       <c r="E14" s="25"/>
@@ -7244,7 +7244,7 @@
         <v>49</v>
       </c>
       <c r="D15" s="80">
-        <f>B15/60/24+C15/3600/24</f>
+        <f t="shared" si="0"/>
         <v>3.1122685185185184E-2</v>
       </c>
       <c r="E15" s="25"/>
@@ -7260,7 +7260,7 @@
         <v>47</v>
       </c>
       <c r="D16" s="80">
-        <f>B16/60/24+C16/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.5127314814814814E-2</v>
       </c>
       <c r="E16" s="25"/>
@@ -7276,7 +7276,7 @@
         <v>46</v>
       </c>
       <c r="D17" s="80">
-        <f>B17/60/24+C17/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.8587962962962966E-2</v>
       </c>
       <c r="E17" s="25"/>
@@ -7292,7 +7292,7 @@
         <v>55</v>
       </c>
       <c r="D18" s="80">
-        <f>B18/60/24+C18/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.7303240740740741E-2</v>
       </c>
       <c r="E18" s="25"/>
@@ -7308,7 +7308,7 @@
         <v>37</v>
       </c>
       <c r="D19" s="80">
-        <f>B19/60/24+C19/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.0150462962962964E-2</v>
       </c>
       <c r="E19" s="25"/>
@@ -7324,7 +7324,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="80">
-        <f>B20/60/24+C20/3600/24</f>
+        <f t="shared" si="0"/>
         <v>1.2256944444444444E-2</v>
       </c>
       <c r="E20" s="25"/>
@@ -7340,7 +7340,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="80">
-        <f>B21/60/24+C21/3600/24</f>
+        <f t="shared" si="0"/>
         <v>4.7245370370370368E-2</v>
       </c>
       <c r="E21" s="25"/>
@@ -7362,7 +7362,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="80">
-        <f>B23/60/24+C23/3600/24</f>
+        <f t="shared" ref="D23:D30" si="1">B23/60/24+C23/3600/24</f>
         <v>6.3194444444444435E-3</v>
       </c>
       <c r="E23" s="25"/>
@@ -7378,7 +7378,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="80">
-        <f>B24/60/24+C24/3600/24</f>
+        <f t="shared" si="1"/>
         <v>1.1157407407407408E-2</v>
       </c>
       <c r="E24" s="25"/>
@@ -7394,7 +7394,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="80">
-        <f>B25/60/24+C25/3600/24</f>
+        <f t="shared" si="1"/>
         <v>4.8726851851851856E-3</v>
       </c>
       <c r="E25" s="25"/>
@@ -7410,7 +7410,7 @@
         <v>55</v>
       </c>
       <c r="D26" s="80">
-        <f>B26/60/24+C26/3600/24</f>
+        <f t="shared" si="1"/>
         <v>3.1192129629629629E-2</v>
       </c>
       <c r="E26" s="25"/>
@@ -7426,7 +7426,7 @@
         <v>21</v>
       </c>
       <c r="D27" s="80">
-        <f>B27/60/24+C27/3600/24</f>
+        <f t="shared" si="1"/>
         <v>2.5937500000000002E-2</v>
       </c>
       <c r="E27" s="25"/>
@@ -7442,7 +7442,7 @@
         <v>14</v>
       </c>
       <c r="D28" s="80">
-        <f>B28/60/24+C28/3600/24</f>
+        <f t="shared" si="1"/>
         <v>1.8912037037037036E-2</v>
       </c>
       <c r="E28" s="25"/>
@@ -7458,7 +7458,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="80">
-        <f>B29/60/24+C29/3600/24</f>
+        <f t="shared" si="1"/>
         <v>1.1168981481481481E-2</v>
       </c>
       <c r="E29" s="25"/>
@@ -7474,7 +7474,7 @@
         <v>31</v>
       </c>
       <c r="D30" s="80">
-        <f>B30/60/24+C30/3600/24</f>
+        <f t="shared" si="1"/>
         <v>3.2997685185185185E-2</v>
       </c>
       <c r="E30" s="25"/>
@@ -7496,7 +7496,7 @@
         <v>12</v>
       </c>
       <c r="D32" s="80">
-        <f>B32/60/24+C32/3600/24</f>
+        <f t="shared" ref="D32:D41" si="2">B32/60/24+C32/3600/24</f>
         <v>1.6805555555555556E-2</v>
       </c>
       <c r="E32" s="25"/>
@@ -7512,7 +7512,7 @@
         <v>54</v>
       </c>
       <c r="D33" s="80">
-        <f>B33/60/24+C33/3600/24</f>
+        <f t="shared" si="2"/>
         <v>2.0069444444444445E-2</v>
       </c>
       <c r="E33" s="25"/>
@@ -7528,7 +7528,7 @@
         <v>38</v>
       </c>
       <c r="D34" s="80">
-        <f>B34/60/24+C34/3600/24</f>
+        <f t="shared" si="2"/>
         <v>1.7106481481481483E-2</v>
       </c>
       <c r="E34" s="25"/>
@@ -7544,7 +7544,7 @@
         <v>57</v>
       </c>
       <c r="D35" s="80">
-        <f>B35/60/24+C35/3600/24</f>
+        <f t="shared" si="2"/>
         <v>1.1770833333333335E-2</v>
       </c>
       <c r="E35" s="25"/>
@@ -7560,7 +7560,7 @@
         <v>19</v>
       </c>
       <c r="D36" s="80">
-        <f>B36/60/24+C36/3600/24</f>
+        <f t="shared" si="2"/>
         <v>3.1469907407407405E-2</v>
       </c>
       <c r="E36" s="25"/>
@@ -7576,7 +7576,7 @@
         <v>26</v>
       </c>
       <c r="D37" s="80">
-        <f>B37/60/24+C37/3600/24</f>
+        <f t="shared" si="2"/>
         <v>3.6412037037037041E-2</v>
       </c>
       <c r="E37" s="25"/>
@@ -7592,7 +7592,7 @@
         <v>53</v>
       </c>
       <c r="D38" s="80">
-        <f>B38/60/24+C38/3600/24</f>
+        <f t="shared" si="2"/>
         <v>9.6412037037037039E-3</v>
       </c>
       <c r="E38" s="25"/>
@@ -7608,7 +7608,7 @@
         <v>24</v>
       </c>
       <c r="D39" s="80">
-        <f>B39/60/24+C39/3600/24</f>
+        <f t="shared" si="2"/>
         <v>4.8194444444444443E-2</v>
       </c>
       <c r="E39" s="25"/>
@@ -7624,7 +7624,7 @@
         <v>11</v>
       </c>
       <c r="D40" s="80">
-        <f>B40/60/24+C40/3600/24</f>
+        <f t="shared" si="2"/>
         <v>9.8495370370370369E-3</v>
       </c>
       <c r="E40" s="25"/>
@@ -7640,7 +7640,7 @@
         <v>25</v>
       </c>
       <c r="D41" s="80">
-        <f>B41/60/24+C41/3600/24</f>
+        <f t="shared" si="2"/>
         <v>1.2094907407407407E-2</v>
       </c>
       <c r="E41" s="25"/>
@@ -7662,7 +7662,7 @@
         <v>39</v>
       </c>
       <c r="D43" s="80">
-        <f>B43/60/24+C43/3600/24</f>
+        <f t="shared" ref="D43:D48" si="3">B43/60/24+C43/3600/24</f>
         <v>8.7847222222222215E-3</v>
       </c>
       <c r="E43" s="25"/>
@@ -7678,7 +7678,7 @@
         <v>36</v>
       </c>
       <c r="D44" s="80">
-        <f>B44/60/24+C44/3600/24</f>
+        <f t="shared" si="3"/>
         <v>1.5694444444444445E-2</v>
       </c>
       <c r="E44" s="25"/>
@@ -7694,7 +7694,7 @@
         <v>54</v>
       </c>
       <c r="D45" s="80">
-        <f>B45/60/24+C45/3600/24</f>
+        <f t="shared" si="3"/>
         <v>1.7291666666666667E-2</v>
       </c>
       <c r="E45" s="25"/>
@@ -7710,7 +7710,7 @@
         <v>13</v>
       </c>
       <c r="D46" s="80">
-        <f>B46/60/24+C46/3600/24</f>
+        <f t="shared" si="3"/>
         <v>7.0949074074074074E-3</v>
       </c>
       <c r="E46" s="25"/>
@@ -7726,7 +7726,7 @@
         <v>29</v>
       </c>
       <c r="D47" s="80">
-        <f>B47/60/24+C47/3600/24</f>
+        <f t="shared" si="3"/>
         <v>2.1863425925925929E-2</v>
       </c>
       <c r="E47" s="25"/>
@@ -7742,7 +7742,7 @@
         <v>18</v>
       </c>
       <c r="D48" s="80">
-        <f>B48/60/24+C48/3600/24</f>
+        <f t="shared" si="3"/>
         <v>2.7986111111111111E-2</v>
       </c>
       <c r="E48" s="25"/>
@@ -7764,7 +7764,7 @@
         <v>51</v>
       </c>
       <c r="D50" s="80">
-        <f>B50/60/24+C50/3600/24</f>
+        <f t="shared" ref="D50:D61" si="4">B50/60/24+C50/3600/24</f>
         <v>1.1006944444444444E-2</v>
       </c>
       <c r="E50" s="25"/>
@@ -7780,7 +7780,7 @@
         <v>17</v>
       </c>
       <c r="D51" s="80">
-        <f>B51/60/24+C51/3600/24</f>
+        <f t="shared" si="4"/>
         <v>1.6168981481481482E-2</v>
       </c>
       <c r="E51" s="25"/>
@@ -7796,7 +7796,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="80">
-        <f>B52/60/24+C52/3600/24</f>
+        <f t="shared" si="4"/>
         <v>2.2939814814814816E-2</v>
       </c>
       <c r="E52" s="25"/>
@@ -7812,7 +7812,7 @@
         <v>54</v>
       </c>
       <c r="D53" s="80">
-        <f>B53/60/24+C53/3600/24</f>
+        <f t="shared" si="4"/>
         <v>1.5902777777777776E-2</v>
       </c>
       <c r="E53" s="25"/>
@@ -7828,7 +7828,7 @@
         <v>24</v>
       </c>
       <c r="D54" s="80">
-        <f>B54/60/24+C54/3600/24</f>
+        <f t="shared" si="4"/>
         <v>3.152777777777778E-2</v>
       </c>
       <c r="E54" s="25"/>
@@ -7844,7 +7844,7 @@
         <v>4</v>
       </c>
       <c r="D55" s="80">
-        <f>B55/60/24+C55/3600/24</f>
+        <f t="shared" si="4"/>
         <v>3.546296296296296E-2</v>
       </c>
       <c r="E55" s="25"/>
@@ -7860,7 +7860,7 @@
         <v>55</v>
       </c>
       <c r="D56" s="80">
-        <f>B56/60/24+C56/3600/24</f>
+        <f t="shared" si="4"/>
         <v>2.2858796296296297E-2</v>
       </c>
       <c r="E56" s="25"/>
@@ -7876,7 +7876,7 @@
         <v>40</v>
       </c>
       <c r="D57" s="80">
-        <f>B57/60/24+C57/3600/24</f>
+        <f t="shared" si="4"/>
         <v>3.7962962962962962E-2</v>
       </c>
       <c r="E57" s="25"/>
@@ -7892,7 +7892,7 @@
         <v>16</v>
       </c>
       <c r="D58" s="80">
-        <f>B58/60/24+C58/3600/24</f>
+        <f t="shared" si="4"/>
         <v>7.8240740740740736E-3</v>
       </c>
       <c r="E58" s="25"/>
@@ -7908,7 +7908,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="80">
-        <f>B59/60/24+C59/3600/24</f>
+        <f t="shared" si="4"/>
         <v>2.1539351851851855E-2</v>
       </c>
       <c r="E59" s="25"/>
@@ -7924,7 +7924,7 @@
         <v>14</v>
       </c>
       <c r="D60" s="80">
-        <f>B60/60/24+C60/3600/24</f>
+        <f t="shared" si="4"/>
         <v>8.4953703703703701E-3</v>
       </c>
       <c r="E60" s="25"/>
@@ -7940,7 +7940,7 @@
         <v>47</v>
       </c>
       <c r="D61" s="80">
-        <f>B61/60/24+C61/3600/24</f>
+        <f t="shared" si="4"/>
         <v>9.5717592592592608E-3</v>
       </c>
       <c r="E61" s="25"/>
@@ -7962,7 +7962,7 @@
         <v>30</v>
       </c>
       <c r="D63" s="80">
-        <f>B63/60/24+C63/3600/24</f>
+        <f t="shared" ref="D63:D68" si="5">B63/60/24+C63/3600/24</f>
         <v>1.7013888888888887E-2</v>
       </c>
       <c r="E63" s="25"/>
@@ -7978,7 +7978,7 @@
         <v>53</v>
       </c>
       <c r="D64" s="80">
-        <f>B64/60/24+C64/3600/24</f>
+        <f t="shared" si="5"/>
         <v>1.380787037037037E-2</v>
       </c>
       <c r="E64" s="25"/>
@@ -7994,7 +7994,7 @@
         <v>30</v>
       </c>
       <c r="D65" s="80">
-        <f>B65/60/24+C65/3600/24</f>
+        <f t="shared" si="5"/>
         <v>6.5972222222222213E-3</v>
       </c>
       <c r="E65" s="25"/>
@@ -8010,7 +8010,7 @@
         <v>14</v>
       </c>
       <c r="D66" s="80">
-        <f>B66/60/24+C66/3600/24</f>
+        <f t="shared" si="5"/>
         <v>4.3287037037037035E-3</v>
       </c>
       <c r="E66" s="25"/>
@@ -8026,7 +8026,7 @@
         <v>57</v>
       </c>
       <c r="D67" s="80">
-        <f>B67/60/24+C67/3600/24</f>
+        <f t="shared" si="5"/>
         <v>1.1770833333333335E-2</v>
       </c>
       <c r="E67" s="25"/>
@@ -8042,7 +8042,7 @@
         <v>4</v>
       </c>
       <c r="D68" s="80">
-        <f>B68/60/24+C68/3600/24</f>
+        <f t="shared" si="5"/>
         <v>9.7685185185185184E-3</v>
       </c>
       <c r="E68" s="25"/>

</xml_diff>

<commit_message>
updated progress for 17_Webpack:L10-L13
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9958867-51A0-41A6-9E02-A2FFA94D03E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53829C-46F4-48C7-9341-B48A054506D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="17" activeTab="17" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
@@ -6992,7 +6992,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7167,7 +7167,9 @@
         <f t="shared" si="0"/>
         <v>1.5104166666666665E-2</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -7183,7 +7185,9 @@
         <f t="shared" si="0"/>
         <v>2.6435185185185187E-2</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="25">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -7199,7 +7203,9 @@
         <f t="shared" si="0"/>
         <v>3.5416666666666666E-2</v>
       </c>
-      <c r="E12" s="25"/>
+      <c r="E12" s="25">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -7215,7 +7221,9 @@
         <f t="shared" si="0"/>
         <v>3.3831018518518517E-2</v>
       </c>
-      <c r="E13" s="25"/>
+      <c r="E13" s="25">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -7231,7 +7239,9 @@
         <f t="shared" si="0"/>
         <v>1.695601851851852E-2</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="25">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -7247,7 +7257,9 @@
         <f t="shared" si="0"/>
         <v>3.1122685185185184E-2</v>
       </c>
-      <c r="E15" s="25"/>
+      <c r="E15" s="25">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -7263,7 +7275,9 @@
         <f t="shared" si="0"/>
         <v>1.5127314814814814E-2</v>
       </c>
-      <c r="E16" s="25"/>
+      <c r="E16" s="25">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -7279,7 +7293,9 @@
         <f t="shared" si="0"/>
         <v>1.8587962962962966E-2</v>
       </c>
-      <c r="E17" s="25"/>
+      <c r="E17" s="25">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">

</xml_diff>

<commit_message>
updated progress for 17_Webpack: completed L6-4: React SPA with Webpack
</commit_message>
<xml_diff>
--- a/assets/contents.xlsx
+++ b/assets/contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\duyiFe\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48302F20-FD2C-408F-BCF9-1A51ECAA3902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE24DF0B-63EE-43C9-BE5B-4C9E9B40828B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="1905" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="11" activeTab="17" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
+    <workbookView xWindow="4965" yWindow="2085" windowWidth="21600" windowHeight="11820" tabRatio="722" firstSheet="13" activeTab="17" xr2:uid="{977D219B-3D5A-4B74-BC43-A61DD328A31A}"/>
   </bookViews>
   <sheets>
     <sheet name="1HTML_scratch" sheetId="9" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="1189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="1194">
   <si>
     <t>1. 环境准备</t>
   </si>
@@ -3675,6 +3675,26 @@
   </si>
   <si>
     <t>补充完整实测代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2026 除夕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 19</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3933,7 +3953,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4172,9 +4192,6 @@
       <alignment horizontal="left" vertical="center" indent="27"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -7918,10 +7935,10 @@
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomRight" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7961,17 +7978,17 @@
       <c r="A3" t="s">
         <v>719</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="57">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="57">
         <v>45</v>
       </c>
-      <c r="D3" s="80">
+      <c r="D3" s="86">
         <f t="shared" ref="D3:D21" si="0">B3/60/24+C3/3600/24</f>
         <v>3.9930555555555552E-3</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="45">
         <v>1</v>
       </c>
     </row>
@@ -7979,17 +7996,17 @@
       <c r="A4" t="s">
         <v>654</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="57">
         <v>42</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="57">
         <v>51</v>
       </c>
-      <c r="D4" s="80">
+      <c r="D4" s="86">
         <f t="shared" si="0"/>
         <v>2.975694444444444E-2</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="45">
         <v>2</v>
       </c>
     </row>
@@ -7997,17 +8014,17 @@
       <c r="A5" t="s">
         <v>655</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="57">
         <v>41</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="57">
         <v>23</v>
       </c>
-      <c r="D5" s="80">
+      <c r="D5" s="86">
         <f t="shared" si="0"/>
         <v>2.8738425925925924E-2</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="45">
         <v>2</v>
       </c>
     </row>
@@ -8015,17 +8032,17 @@
       <c r="A6" t="s">
         <v>656</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="57">
         <v>16</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="57">
         <v>11</v>
       </c>
-      <c r="D6" s="80">
+      <c r="D6" s="86">
         <f t="shared" si="0"/>
         <v>1.1238425925925926E-2</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="45">
         <v>2</v>
       </c>
     </row>
@@ -8033,17 +8050,17 @@
       <c r="A7" t="s">
         <v>657</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="57">
         <v>51</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="57">
         <v>16</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="86">
         <f t="shared" si="0"/>
         <v>3.560185185185185E-2</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="45">
         <v>3</v>
       </c>
     </row>
@@ -8051,17 +8068,17 @@
       <c r="A8" t="s">
         <v>658</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="57">
         <v>40</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="57">
         <v>43</v>
       </c>
-      <c r="D8" s="80">
+      <c r="D8" s="86">
         <f t="shared" si="0"/>
         <v>2.8275462962962961E-2</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="45">
         <v>4</v>
       </c>
     </row>
@@ -8069,17 +8086,17 @@
       <c r="A9" t="s">
         <v>718</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="57">
         <v>21</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="57">
         <v>2</v>
       </c>
-      <c r="D9" s="80">
+      <c r="D9" s="86">
         <f t="shared" si="0"/>
         <v>1.4606481481481481E-2</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="45">
         <v>4</v>
       </c>
     </row>
@@ -8087,17 +8104,17 @@
       <c r="A10" t="s">
         <v>659</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="57">
         <v>21</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="57">
         <v>45</v>
       </c>
-      <c r="D10" s="80">
+      <c r="D10" s="86">
         <f t="shared" si="0"/>
         <v>1.5104166666666665E-2</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="45">
         <v>4</v>
       </c>
     </row>
@@ -8105,17 +8122,17 @@
       <c r="A11" t="s">
         <v>660</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="57">
         <v>38</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="57">
         <v>4</v>
       </c>
-      <c r="D11" s="80">
+      <c r="D11" s="86">
         <f t="shared" si="0"/>
         <v>2.6435185185185187E-2</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="45">
         <v>5</v>
       </c>
     </row>
@@ -8123,17 +8140,17 @@
       <c r="A12" t="s">
         <v>661</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="57">
         <v>51</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="57">
         <v>0</v>
       </c>
-      <c r="D12" s="80">
+      <c r="D12" s="86">
         <f t="shared" si="0"/>
         <v>3.5416666666666666E-2</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="45">
         <v>5</v>
       </c>
     </row>
@@ -8141,17 +8158,17 @@
       <c r="A13" t="s">
         <v>662</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="57">
         <v>48</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="57">
         <v>43</v>
       </c>
-      <c r="D13" s="80">
+      <c r="D13" s="86">
         <f t="shared" si="0"/>
         <v>3.3831018518518517E-2</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="45">
         <v>5</v>
       </c>
     </row>
@@ -8159,17 +8176,17 @@
       <c r="A14" t="s">
         <v>663</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="57">
         <v>24</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="57">
         <v>25</v>
       </c>
-      <c r="D14" s="80">
+      <c r="D14" s="86">
         <f t="shared" si="0"/>
         <v>1.695601851851852E-2</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="45">
         <v>6</v>
       </c>
     </row>
@@ -8177,17 +8194,17 @@
       <c r="A15" t="s">
         <v>664</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="57">
         <v>44</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="57">
         <v>49</v>
       </c>
-      <c r="D15" s="80">
+      <c r="D15" s="86">
         <f t="shared" si="0"/>
         <v>3.1122685185185184E-2</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="45">
         <v>6</v>
       </c>
     </row>
@@ -8195,17 +8212,17 @@
       <c r="A16" t="s">
         <v>665</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="57">
         <v>21</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="57">
         <v>47</v>
       </c>
-      <c r="D16" s="80">
+      <c r="D16" s="86">
         <f t="shared" si="0"/>
         <v>1.5127314814814814E-2</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="45">
         <v>6</v>
       </c>
     </row>
@@ -8213,17 +8230,17 @@
       <c r="A17" t="s">
         <v>666</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="57">
         <v>26</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="57">
         <v>46</v>
       </c>
-      <c r="D17" s="80">
+      <c r="D17" s="86">
         <f t="shared" si="0"/>
         <v>1.8587962962962966E-2</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="45">
         <v>6</v>
       </c>
     </row>
@@ -8231,17 +8248,17 @@
       <c r="A18" t="s">
         <v>667</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="57">
         <v>24</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="57">
         <v>55</v>
       </c>
-      <c r="D18" s="80">
+      <c r="D18" s="86">
         <f t="shared" si="0"/>
         <v>1.7303240740740741E-2</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="45">
         <v>6</v>
       </c>
     </row>
@@ -8249,17 +8266,17 @@
       <c r="A19" t="s">
         <v>668</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="57">
         <v>14</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="57">
         <v>37</v>
       </c>
-      <c r="D19" s="80">
+      <c r="D19" s="86">
         <f t="shared" si="0"/>
         <v>1.0150462962962964E-2</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="45">
         <v>6</v>
       </c>
     </row>
@@ -8273,7 +8290,7 @@
       <c r="C20" s="63">
         <v>39</v>
       </c>
-      <c r="D20" s="82">
+      <c r="D20" s="81">
         <f t="shared" si="0"/>
         <v>1.2256944444444444E-2</v>
       </c>
@@ -8291,7 +8308,7 @@
       <c r="C21" s="26">
         <v>2</v>
       </c>
-      <c r="D21" s="83">
+      <c r="D21" s="82">
         <f t="shared" si="0"/>
         <v>4.7245370370370368E-2</v>
       </c>
@@ -8318,7 +8335,7 @@
       <c r="C23" s="63">
         <v>6</v>
       </c>
-      <c r="D23" s="82">
+      <c r="D23" s="81">
         <f t="shared" ref="D23:D30" si="1">B23/60/24+C23/3600/24</f>
         <v>6.3194444444444435E-3</v>
       </c>
@@ -8336,7 +8353,7 @@
       <c r="C24" s="63">
         <v>4</v>
       </c>
-      <c r="D24" s="82">
+      <c r="D24" s="81">
         <f t="shared" si="1"/>
         <v>1.1157407407407408E-2</v>
       </c>
@@ -8354,7 +8371,7 @@
       <c r="C25" s="63">
         <v>1</v>
       </c>
-      <c r="D25" s="82">
+      <c r="D25" s="81">
         <f t="shared" si="1"/>
         <v>4.8726851851851856E-3</v>
       </c>
@@ -8372,7 +8389,7 @@
       <c r="C26" s="63">
         <v>55</v>
       </c>
-      <c r="D26" s="82">
+      <c r="D26" s="81">
         <f t="shared" si="1"/>
         <v>3.1192129629629629E-2</v>
       </c>
@@ -8390,14 +8407,14 @@
       <c r="C27" s="63">
         <v>21</v>
       </c>
-      <c r="D27" s="82">
+      <c r="D27" s="81">
         <f t="shared" si="1"/>
         <v>2.5937500000000002E-2</v>
       </c>
       <c r="E27" s="45" t="s">
         <v>1186</v>
       </c>
-      <c r="F27" s="81">
+      <c r="F27" s="80">
         <v>43849</v>
       </c>
     </row>
@@ -8411,7 +8428,7 @@
       <c r="C28" s="63">
         <v>14</v>
       </c>
-      <c r="D28" s="87">
+      <c r="D28" s="86">
         <f t="shared" si="1"/>
         <v>1.8912037037037036E-2</v>
       </c>
@@ -8429,7 +8446,7 @@
       <c r="C29" s="63">
         <v>5</v>
       </c>
-      <c r="D29" s="87">
+      <c r="D29" s="86">
         <f t="shared" si="1"/>
         <v>1.1168981481481481E-2</v>
       </c>
@@ -8447,7 +8464,7 @@
       <c r="C30" s="63">
         <v>31</v>
       </c>
-      <c r="D30" s="87">
+      <c r="D30" s="86">
         <f t="shared" si="1"/>
         <v>3.2997685185185185E-2</v>
       </c>
@@ -8471,7 +8488,7 @@
       <c r="C32" s="57">
         <v>12</v>
       </c>
-      <c r="D32" s="87">
+      <c r="D32" s="86">
         <f t="shared" ref="D32:D41" si="2">B32/60/24+C32/3600/24</f>
         <v>1.6805555555555556E-2</v>
       </c>
@@ -8492,7 +8509,7 @@
       <c r="C33" s="57">
         <v>54</v>
       </c>
-      <c r="D33" s="87">
+      <c r="D33" s="86">
         <f t="shared" si="2"/>
         <v>2.0069444444444445E-2</v>
       </c>
@@ -8510,7 +8527,7 @@
       <c r="C34" s="57">
         <v>38</v>
       </c>
-      <c r="D34" s="87">
+      <c r="D34" s="86">
         <f t="shared" si="2"/>
         <v>1.7106481481481483E-2</v>
       </c>
@@ -8528,7 +8545,7 @@
       <c r="C35" s="57">
         <v>57</v>
       </c>
-      <c r="D35" s="87">
+      <c r="D35" s="86">
         <f t="shared" si="2"/>
         <v>1.1770833333333335E-2</v>
       </c>
@@ -8546,7 +8563,7 @@
       <c r="C36" s="57">
         <v>19</v>
       </c>
-      <c r="D36" s="87">
+      <c r="D36" s="86">
         <f t="shared" si="2"/>
         <v>3.1469907407407405E-2</v>
       </c>
@@ -8564,7 +8581,7 @@
       <c r="C37" s="57">
         <v>26</v>
       </c>
-      <c r="D37" s="87">
+      <c r="D37" s="86">
         <f t="shared" si="2"/>
         <v>3.6412037037037041E-2</v>
       </c>
@@ -8582,7 +8599,7 @@
       <c r="C38" s="57">
         <v>53</v>
       </c>
-      <c r="D38" s="87">
+      <c r="D38" s="86">
         <f t="shared" si="2"/>
         <v>9.6412037037037039E-3</v>
       </c>
@@ -8600,11 +8617,11 @@
       <c r="C39" s="57">
         <v>24</v>
       </c>
-      <c r="D39" s="87">
+      <c r="D39" s="86">
         <f t="shared" si="2"/>
         <v>4.8194444444444443E-2</v>
       </c>
-      <c r="E39" s="88" t="s">
+      <c r="E39" s="87" t="s">
         <v>1183</v>
       </c>
       <c r="F39" t="s">
@@ -8621,7 +8638,7 @@
       <c r="C40" s="57">
         <v>11</v>
       </c>
-      <c r="D40" s="87">
+      <c r="D40" s="86">
         <f t="shared" si="2"/>
         <v>9.8495370370370369E-3</v>
       </c>
@@ -8639,7 +8656,7 @@
       <c r="C41" s="57">
         <v>25</v>
       </c>
-      <c r="D41" s="87">
+      <c r="D41" s="86">
         <f t="shared" si="2"/>
         <v>1.2094907407407407E-2</v>
       </c>
@@ -8663,7 +8680,7 @@
       <c r="C43" s="63">
         <v>39</v>
       </c>
-      <c r="D43" s="82">
+      <c r="D43" s="81">
         <f t="shared" ref="D43:D48" si="3">B43/60/24+C43/3600/24</f>
         <v>8.7847222222222215E-3</v>
       </c>
@@ -8681,7 +8698,7 @@
       <c r="C44" s="63">
         <v>36</v>
       </c>
-      <c r="D44" s="82">
+      <c r="D44" s="81">
         <f t="shared" si="3"/>
         <v>1.5694444444444445E-2</v>
       </c>
@@ -8699,7 +8716,7 @@
       <c r="C45" s="63">
         <v>54</v>
       </c>
-      <c r="D45" s="82">
+      <c r="D45" s="81">
         <f t="shared" si="3"/>
         <v>1.7291666666666667E-2</v>
       </c>
@@ -8717,7 +8734,7 @@
       <c r="C46" s="63">
         <v>13</v>
       </c>
-      <c r="D46" s="82">
+      <c r="D46" s="81">
         <f t="shared" si="3"/>
         <v>7.0949074074074074E-3</v>
       </c>
@@ -8735,7 +8752,7 @@
       <c r="C47" s="63">
         <v>29</v>
       </c>
-      <c r="D47" s="82">
+      <c r="D47" s="81">
         <f t="shared" si="3"/>
         <v>2.1863425925925929E-2</v>
       </c>
@@ -8753,7 +8770,7 @@
       <c r="C48" s="63">
         <v>18</v>
       </c>
-      <c r="D48" s="82">
+      <c r="D48" s="81">
         <f t="shared" si="3"/>
         <v>2.7986111111111111E-2</v>
       </c>
@@ -8761,340 +8778,343 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="60" t="s">
         <v>698</v>
       </c>
       <c r="E49" s="25"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>699</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="57">
         <v>15</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="57">
         <v>51</v>
       </c>
-      <c r="D50" s="80">
+      <c r="D50" s="86">
         <f t="shared" ref="D50:D61" si="4">B50/60/24+C50/3600/24</f>
         <v>1.1006944444444444E-2</v>
       </c>
-      <c r="E50" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E50" s="45">
+        <v>14</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>700</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="57">
         <v>23</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="57">
         <v>17</v>
       </c>
-      <c r="D51" s="80">
+      <c r="D51" s="86">
         <f t="shared" si="4"/>
         <v>1.6168981481481482E-2</v>
       </c>
-      <c r="E51" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E51" s="45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>701</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="57">
         <v>33</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="57">
         <v>2</v>
       </c>
-      <c r="D52" s="80">
+      <c r="D52" s="86">
         <f t="shared" si="4"/>
         <v>2.2939814814814816E-2</v>
       </c>
-      <c r="E52" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E52" s="45" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>702</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="57">
         <v>22</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="57">
         <v>54</v>
       </c>
-      <c r="D53" s="80">
+      <c r="D53" s="86">
         <f t="shared" si="4"/>
         <v>1.5902777777777776E-2</v>
       </c>
-      <c r="E53" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E53" s="45" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>703</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="57">
         <v>45</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="57">
         <v>24</v>
       </c>
-      <c r="D54" s="80">
+      <c r="D54" s="86">
         <f t="shared" si="4"/>
         <v>3.152777777777778E-2</v>
       </c>
-      <c r="E54" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E54" s="45" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>704</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="57">
         <v>51</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="57">
         <v>4</v>
       </c>
-      <c r="D55" s="80">
+      <c r="D55" s="86">
         <f t="shared" si="4"/>
         <v>3.546296296296296E-2</v>
       </c>
-      <c r="E55" s="25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="45" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>705</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="57">
         <v>32</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="57">
         <v>55</v>
       </c>
-      <c r="D56" s="80">
+      <c r="D56" s="86">
         <f t="shared" si="4"/>
         <v>2.2858796296296297E-2</v>
       </c>
-      <c r="E56" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E56" s="45" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>706</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="57">
         <v>54</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="57">
         <v>40</v>
       </c>
-      <c r="D57" s="80">
+      <c r="D57" s="86">
         <f t="shared" si="4"/>
         <v>3.7962962962962962E-2</v>
       </c>
-      <c r="E57" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="45" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>707</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="57">
         <v>11</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="57">
         <v>16</v>
       </c>
-      <c r="D58" s="80">
+      <c r="D58" s="86">
         <f t="shared" si="4"/>
         <v>7.8240740740740736E-3</v>
       </c>
-      <c r="E58" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E58" s="45" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>708</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="57">
         <v>31</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="57">
         <v>1</v>
       </c>
-      <c r="D59" s="80">
+      <c r="D59" s="86">
         <f t="shared" si="4"/>
         <v>2.1539351851851855E-2</v>
       </c>
-      <c r="E59" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E59" s="45" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>709</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="57">
         <v>12</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="57">
         <v>14</v>
       </c>
-      <c r="D60" s="80">
+      <c r="D60" s="86">
         <f t="shared" si="4"/>
         <v>8.4953703703703701E-3</v>
       </c>
-      <c r="E60" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E60" s="45" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>710</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="57">
         <v>13</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="57">
         <v>47</v>
       </c>
-      <c r="D61" s="80">
+      <c r="D61" s="86">
         <f t="shared" si="4"/>
         <v>9.5717592592592608E-3</v>
       </c>
-      <c r="E61" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E61" s="45" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="60" t="s">
         <v>711</v>
       </c>
       <c r="E62" s="25"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>712</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="57">
         <v>24</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="57">
         <v>30</v>
       </c>
-      <c r="D63" s="80">
+      <c r="D63" s="86">
         <f t="shared" ref="D63:D68" si="5">B63/60/24+C63/3600/24</f>
         <v>1.7013888888888887E-2</v>
       </c>
-      <c r="E63" s="25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E63" s="45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>713</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="57">
         <v>19</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="57">
         <v>53</v>
       </c>
-      <c r="D64" s="80">
+      <c r="D64" s="86">
         <f t="shared" si="5"/>
         <v>1.380787037037037E-2</v>
       </c>
-      <c r="E64" s="25">
-        <v>6</v>
+      <c r="E64" s="45">
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>714</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="57">
         <v>9</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="57">
         <v>30</v>
       </c>
-      <c r="D65" s="80">
+      <c r="D65" s="86">
         <f t="shared" si="5"/>
         <v>6.5972222222222213E-3</v>
       </c>
-      <c r="E65" s="25">
-        <v>6</v>
+      <c r="E65" s="45">
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>715</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="57">
         <v>6</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="57">
         <v>14</v>
       </c>
-      <c r="D66" s="80">
+      <c r="D66" s="86">
         <f t="shared" si="5"/>
         <v>4.3287037037037035E-3</v>
       </c>
-      <c r="E66" s="25">
-        <v>6</v>
+      <c r="E66" s="45">
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>716</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="57">
         <v>16</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="57">
         <v>57</v>
       </c>
-      <c r="D67" s="80">
+      <c r="D67" s="86">
         <f t="shared" si="5"/>
         <v>1.1770833333333335E-2</v>
       </c>
-      <c r="E67" s="25">
-        <v>6</v>
+      <c r="E67" s="45" t="s">
+        <v>1193</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>717</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="57">
         <v>14</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="57">
         <v>4</v>
       </c>
-      <c r="D68" s="80">
+      <c r="D68" s="86">
         <f t="shared" si="5"/>
         <v>9.7685185185185184E-3</v>
       </c>
-      <c r="E68" s="25">
-        <v>6</v>
+      <c r="E68" s="45" t="s">
+        <v>1193</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -9120,6 +9140,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -9151,7 +9172,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10487,10 +10508,10 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -15265,12 +15286,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="83" t="s">
         <v>1122</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -15350,12 +15371,12 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="83" t="s">
         <v>1130</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -15405,10 +15426,10 @@
       <c r="A15" t="s">
         <v>1134</v>
       </c>
-      <c r="B15" s="86">
+      <c r="B15" s="85">
         <v>38</v>
       </c>
-      <c r="C15" s="86">
+      <c r="C15" s="85">
         <v>24</v>
       </c>
     </row>
@@ -15512,12 +15533,12 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="84" t="s">
+      <c r="A25" s="83" t="s">
         <v>1144</v>
       </c>
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -15597,12 +15618,12 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="84" t="s">
+      <c r="A33" s="83" t="s">
         <v>1151</v>
       </c>
-      <c r="B33" s="85"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="85"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -15627,12 +15648,12 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="84" t="s">
+      <c r="A36" s="83" t="s">
         <v>1154</v>
       </c>
-      <c r="B36" s="85"/>
-      <c r="C36" s="85"/>
-      <c r="D36" s="85"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -15668,12 +15689,12 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="84" t="s">
+      <c r="A40" s="83" t="s">
         <v>1157</v>
       </c>
-      <c r="B40" s="85"/>
-      <c r="C40" s="85"/>
-      <c r="D40" s="85"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -15929,12 +15950,12 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="84" t="s">
+      <c r="A64" s="83" t="s">
         <v>1180</v>
       </c>
-      <c r="B64" s="85"/>
-      <c r="C64" s="85"/>
-      <c r="D64" s="85"/>
+      <c r="B64" s="84"/>
+      <c r="C64" s="84"/>
+      <c r="D64" s="84"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">

</xml_diff>